<commit_message>
ActualizaciÃ³n completa (2025-09-16 23:09)
</commit_message>
<xml_diff>
--- a/BACKUP/SUPORT IMAGEN.xlsx
+++ b/BACKUP/SUPORT IMAGEN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jorgg\OneDrive\MasterHIT\BACKUP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6231575A-DDE9-477F-92E1-8E5BCB3908F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFDD00E4-B99E-4718-9CB4-F3FACC95ABB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="45">
   <si>
     <t>id,name,set,type,category,price,compareAtPrice,stock,image,tags,source,createdAt</t>
   </si>
@@ -81,9 +81,6 @@
     <t>spc-prismatic-es</t>
   </si>
   <si>
-    <t>SV Prismatic Evolutions</t>
-  </si>
-  <si>
     <t>['SPC', 'ES']</t>
   </si>
   <si>
@@ -99,18 +96,12 @@
     <t>etb-white-flare-en</t>
   </si>
   <si>
-    <t>SV White Flare</t>
-  </si>
-  <si>
     <t>['ETB', 'EN']</t>
   </si>
   <si>
     <t>etb-black-bolt-en</t>
   </si>
   <si>
-    <t>SV Black Bolt</t>
-  </si>
-  <si>
     <t>etb-black-bolt-es</t>
   </si>
   <si>
@@ -123,9 +114,6 @@
     <t>etb-surging-sparks-en</t>
   </si>
   <si>
-    <t>SV Surging Sparks</t>
-  </si>
-  <si>
     <t>etb-prismatic-en</t>
   </si>
   <si>
@@ -135,67 +123,55 @@
     <t>INGLÉS</t>
   </si>
   <si>
-    <t>Evoluciones Prismáticas – Super Premium Collection – Español</t>
-  </si>
-  <si>
-    <t>Evoluciones Prismáticas – Elite Trainer Box – Español</t>
-  </si>
-  <si>
-    <t>Evoluciones Prismáticas – Elite Trainer Box – Inglés</t>
-  </si>
-  <si>
-    <t>White Flare – Elite Trainer Box – Inglés</t>
-  </si>
-  <si>
-    <t>Black Bolt – Elite Trainer Box – Inglés</t>
-  </si>
-  <si>
-    <t>Black Bolt – Elite Trainer Box – Español</t>
-  </si>
-  <si>
-    <t>Aventuras Compartidas – Elite Trainer Box – Español</t>
-  </si>
-  <si>
-    <t>Surging Sparks – Elite Trainer Box – Inglés</t>
-  </si>
-  <si>
-    <t>Llama Blanca – Elite Trainer Box – Español</t>
-  </si>
-  <si>
-    <t>SV Journey Together</t>
-  </si>
-  <si>
     <t>SPC</t>
   </si>
   <si>
     <t>ETB</t>
   </si>
   <si>
-    <t>spc-prismatic-es,Evoluciones Prismáticas – Super Premium Collection – Español,SV Prismatic Evolutions,ESPAÑOL,SPC,99990,129990,10,img/spc-prismatic-es.webp,['SPC', 'ES'],https://collectorcenter.cl/collections/ver-todo-pokemon,1757822265443</t>
-  </si>
-  <si>
-    <t>etb-prismatic-es,Evoluciones Prismáticas – Elite Trainer Box – Español,SV Prismatic Evolutions,ESPAÑOL,ETB,49990,69990,10,img/etb-prismatic-es.webp,['ETB', 'ES'],https://collectorcenter.cl/collections/ver-todo-pokemon,1757735865443</t>
-  </si>
-  <si>
-    <t>etb-prismatic-en,Evoluciones Prismáticas – Elite Trainer Box – Inglés,SV Prismatic Evolutions,INGLÉS,ETB,49990,69990,10,img/etb-prismatic-en.webp,['ETB', 'ES'],https://collectorcenter.cl/collections/ver-todo-pokemon,1757735865443</t>
-  </si>
-  <si>
-    <t>etb-white-flare-en,White Flare – Elite Trainer Box – Inglés,SV White Flare,INGLÉS,ETB,59990,67990,10,img/etb-white-flare-en.webp,['ETB', 'EN'],https://collectorcenter.cl/collections/ver-todo-pokemon,1757649465443</t>
-  </si>
-  <si>
-    <t>etb-black-bolt-en,Black Bolt – Elite Trainer Box – Inglés,SV Black Bolt,INGLÉS,ETB,59990,67990,10,img/etb-black-bolt-en.webp,['ETB', 'EN'],https://collectorcenter.cl/collections/ver-todo-pokemon,1757563065443</t>
-  </si>
-  <si>
-    <t>etb-black-bolt-es,Black Bolt – Elite Trainer Box – Español,SV Black Bolt,ESPAÑOL,ETB,49990,54990,10,img/etb-black-bolt-es.webp,['ETB', 'ES'],https://collectorcenter.cl/collections/ver-todo-pokemon,1757390265443</t>
-  </si>
-  <si>
-    <t>etb-aventuras-es,Aventuras Compartidas – Elite Trainer Box – Español,SV Journey Together,ESPAÑOL,ETB,42990,59990,10,img/etb-aventuras-es.webp,['ETB', 'ES'],https://collectorcenter.cl/collections/ver-todo-pokemon,1757044665443</t>
-  </si>
-  <si>
-    <t>etb-white-flare-es,Llama Blanca – Elite Trainer Box – Español,SV White Flare,ESPAÑOL,ETB,49990,54990,10,img/etb-white-flare-es.webp,['ETB', 'ES'],https://collectorcenter.cl/collections/ver-todo-pokemon,1756958265443</t>
-  </si>
-  <si>
-    <t>etb-surging-sparks-en,Surging Sparks – Elite Trainer Box – Inglés,SV Surging Sparks,INGLÉS,ETB,54990,64990,10,img/etb-surging-sparks-en.webp,['ETB', 'EN'],https://collectorcenter.cl/collections/ver-todo-pokemon,1756612665443</t>
+    <t>Evoluciones Prismáticas – Super Premium Collection</t>
+  </si>
+  <si>
+    <t>Evoluciones Prismáticas – Elite Trainer Box</t>
+  </si>
+  <si>
+    <t>White Flare – Elite Trainer Box</t>
+  </si>
+  <si>
+    <t>Black Bolt – Elite Trainer Box</t>
+  </si>
+  <si>
+    <t>Aventuras Compartidas – Elite Trainer Box</t>
+  </si>
+  <si>
+    <t>Llama Blanca – Elite Trainer Box</t>
+  </si>
+  <si>
+    <t>Surging Sparks – Elite Trainer Box</t>
+  </si>
+  <si>
+    <t>spc-prismatic-es,Evoluciones Prismáticas – Super Premium Collection,SPC,ESPAÑOL,SPC,99990,129990,10,img/spc-prismatic-es.webp,['SPC', 'ES'],https://collectorcenter.cl/collections/ver-todo-pokemon,1757822265443</t>
+  </si>
+  <si>
+    <t>etb-prismatic-es,Evoluciones Prismáticas – Elite Trainer Box,ETB,ESPAÑOL,ETB,49990,69990,10,img/etb-prismatic-es.webp,['ETB', 'ES'],https://collectorcenter.cl/collections/ver-todo-pokemon,1757735865443</t>
+  </si>
+  <si>
+    <t>etb-prismatic-en,Evoluciones Prismáticas – Elite Trainer Box,ETB,INGLÉS,ETB,49990,69990,10,img/etb-prismatic-en.webp,['ETB', 'ES'],https://collectorcenter.cl/collections/ver-todo-pokemon,1757735865443</t>
+  </si>
+  <si>
+    <t>etb-white-flare-en,White Flare – Elite Trainer Box,ETB,INGLÉS,ETB,59990,67990,10,img/etb-white-flare-en.webp,['ETB', 'EN'],https://collectorcenter.cl/collections/ver-todo-pokemon,1757649465443</t>
+  </si>
+  <si>
+    <t>etb-black-bolt-en,Black Bolt – Elite Trainer Box,ETB,INGLÉS,ETB,59990,67990,10,img/etb-black-bolt-en.webp,['ETB', 'EN'],https://collectorcenter.cl/collections/ver-todo-pokemon,1757563065443</t>
+  </si>
+  <si>
+    <t>etb-black-bolt-es,Black Bolt – Elite Trainer Box,ETB,ESPAÑOL,ETB,49990,54990,10,img/etb-black-bolt-es.webp,['ETB', 'ES'],https://collectorcenter.cl/collections/ver-todo-pokemon,1757390265443</t>
+  </si>
+  <si>
+    <t>etb-aventuras-es,Aventuras Compartidas – Elite Trainer Box,ETB,ESPAÑOL,ETB,42990,59990,10,img/etb-aventuras-es.webp,['ETB', 'ES'],https://collectorcenter.cl/collections/ver-todo-pokemon,1757044665443</t>
+  </si>
+  <si>
+    <t>etb-white-flare-es,Llama Blanca – Elite Trainer Box,ETB,ESPAÑOL,ETB,49990,54990,10,img/etb-white-flare-es.webp,['ETB', 'ES'],https://collectorcenter.cl/collections/ver-todo-pokemon,1756958265443</t>
   </si>
 </sst>
 </file>
@@ -520,10 +496,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A10"/>
+  <dimension ref="A1:A9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A10"/>
+      <selection activeCell="A9" sqref="A1:A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -535,47 +511,42 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -587,14 +558,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3CA635C-1DF7-4EEC-B0B8-3FA5C80D03DF}">
   <dimension ref="A1:O10"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="F1" workbookViewId="0">
       <selection activeCell="O1" sqref="O1:O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="22.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="72.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="53" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.7265625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22.453125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11.81640625" bestFit="1" customWidth="1"/>
@@ -647,16 +618,16 @@
         <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="D2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E2" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="F2">
         <v>99990</v>
@@ -672,34 +643,34 @@
         <v>img/spc-prismatic-es.webp</v>
       </c>
       <c r="J2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" t="s">
         <v>15</v>
-      </c>
-      <c r="K2" t="s">
-        <v>16</v>
       </c>
       <c r="L2">
         <v>1757822265443</v>
       </c>
       <c r="O2" s="1" t="str">
         <f t="shared" ref="O2:O10" si="0">CONCATENATE(A2,",",B2,",",C2,",",D2,",",E2,",",F2,",",G2,",",H2,",",I2,",",J2,",",K2,",",L2)</f>
-        <v>spc-prismatic-es,Evoluciones Prismáticas – Super Premium Collection – Español,SV Prismatic Evolutions,ESPAÑOL,SPC,99990,129990,10,img/spc-prismatic-es.webp,['SPC', 'ES'],https://collectorcenter.cl/collections/ver-todo-pokemon,1757822265443</v>
+        <v>spc-prismatic-es,Evoluciones Prismáticas – Super Premium Collection,SPC,ESPAÑOL,SPC,99990,129990,10,img/spc-prismatic-es.webp,['SPC', 'ES'],https://collectorcenter.cl/collections/ver-todo-pokemon,1757822265443</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="D3" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E3" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="F3">
         <v>49990</v>
@@ -715,34 +686,34 @@
         <v>img/etb-prismatic-es.webp</v>
       </c>
       <c r="J3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L3">
         <v>1757735865443</v>
       </c>
       <c r="O3" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>etb-prismatic-es,Evoluciones Prismáticas – Elite Trainer Box – Español,SV Prismatic Evolutions,ESPAÑOL,ETB,49990,69990,10,img/etb-prismatic-es.webp,['ETB', 'ES'],https://collectorcenter.cl/collections/ver-todo-pokemon,1757735865443</v>
+        <v>etb-prismatic-es,Evoluciones Prismáticas – Elite Trainer Box,ETB,ESPAÑOL,ETB,49990,69990,10,img/etb-prismatic-es.webp,['ETB', 'ES'],https://collectorcenter.cl/collections/ver-todo-pokemon,1757735865443</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="D4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E4" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="F4">
         <v>49990</v>
@@ -758,34 +729,34 @@
         <v>img/etb-prismatic-en.webp</v>
       </c>
       <c r="J4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L4">
         <v>1757735865443</v>
       </c>
       <c r="O4" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>etb-prismatic-en,Evoluciones Prismáticas – Elite Trainer Box – Inglés,SV Prismatic Evolutions,INGLÉS,ETB,49990,69990,10,img/etb-prismatic-en.webp,['ETB', 'ES'],https://collectorcenter.cl/collections/ver-todo-pokemon,1757735865443</v>
+        <v>etb-prismatic-en,Evoluciones Prismáticas – Elite Trainer Box,ETB,INGLÉS,ETB,49990,69990,10,img/etb-prismatic-en.webp,['ETB', 'ES'],https://collectorcenter.cl/collections/ver-todo-pokemon,1757735865443</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B5" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="D5" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E5" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="F5">
         <v>59990</v>
@@ -801,34 +772,34 @@
         <v>img/etb-white-flare-en.webp</v>
       </c>
       <c r="J5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="K5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L5">
         <v>1757649465443</v>
       </c>
       <c r="O5" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>etb-white-flare-en,White Flare – Elite Trainer Box – Inglés,SV White Flare,INGLÉS,ETB,59990,67990,10,img/etb-white-flare-en.webp,['ETB', 'EN'],https://collectorcenter.cl/collections/ver-todo-pokemon,1757649465443</v>
+        <v>etb-white-flare-en,White Flare – Elite Trainer Box,ETB,INGLÉS,ETB,59990,67990,10,img/etb-white-flare-en.webp,['ETB', 'EN'],https://collectorcenter.cl/collections/ver-todo-pokemon,1757649465443</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C6" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="D6" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E6" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="F6">
         <v>59990</v>
@@ -844,34 +815,34 @@
         <v>img/etb-black-bolt-en.webp</v>
       </c>
       <c r="J6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="K6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L6">
         <v>1757563065443</v>
       </c>
       <c r="O6" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>etb-black-bolt-en,Black Bolt – Elite Trainer Box – Inglés,SV Black Bolt,INGLÉS,ETB,59990,67990,10,img/etb-black-bolt-en.webp,['ETB', 'EN'],https://collectorcenter.cl/collections/ver-todo-pokemon,1757563065443</v>
+        <v>etb-black-bolt-en,Black Bolt – Elite Trainer Box,ETB,INGLÉS,ETB,59990,67990,10,img/etb-black-bolt-en.webp,['ETB', 'EN'],https://collectorcenter.cl/collections/ver-todo-pokemon,1757563065443</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B7" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C7" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="D7" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E7" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="F7">
         <v>49990</v>
@@ -887,34 +858,34 @@
         <v>img/etb-black-bolt-es.webp</v>
       </c>
       <c r="J7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L7">
         <v>1757390265443</v>
       </c>
       <c r="O7" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>etb-black-bolt-es,Black Bolt – Elite Trainer Box – Español,SV Black Bolt,ESPAÑOL,ETB,49990,54990,10,img/etb-black-bolt-es.webp,['ETB', 'ES'],https://collectorcenter.cl/collections/ver-todo-pokemon,1757390265443</v>
+        <v>etb-black-bolt-es,Black Bolt – Elite Trainer Box,ETB,ESPAÑOL,ETB,49990,54990,10,img/etb-black-bolt-es.webp,['ETB', 'ES'],https://collectorcenter.cl/collections/ver-todo-pokemon,1757390265443</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B8" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C8" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="D8" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E8" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="F8">
         <v>42990</v>
@@ -930,34 +901,34 @@
         <v>img/etb-aventuras-es.webp</v>
       </c>
       <c r="J8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L8">
         <v>1757044665443</v>
       </c>
       <c r="O8" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>etb-aventuras-es,Aventuras Compartidas – Elite Trainer Box – Español,SV Journey Together,ESPAÑOL,ETB,42990,59990,10,img/etb-aventuras-es.webp,['ETB', 'ES'],https://collectorcenter.cl/collections/ver-todo-pokemon,1757044665443</v>
+        <v>etb-aventuras-es,Aventuras Compartidas – Elite Trainer Box,ETB,ESPAÑOL,ETB,42990,59990,10,img/etb-aventuras-es.webp,['ETB', 'ES'],https://collectorcenter.cl/collections/ver-todo-pokemon,1757044665443</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" t="s">
         <v>26</v>
       </c>
-      <c r="B9" t="s">
-        <v>40</v>
-      </c>
-      <c r="C9" t="s">
-        <v>20</v>
-      </c>
-      <c r="D9" t="s">
-        <v>30</v>
-      </c>
       <c r="E9" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="F9">
         <v>49990</v>
@@ -973,34 +944,34 @@
         <v>img/etb-white-flare-es.webp</v>
       </c>
       <c r="J9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L9">
         <v>1756958265443</v>
       </c>
       <c r="O9" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>etb-white-flare-es,Llama Blanca – Elite Trainer Box – Español,SV White Flare,ESPAÑOL,ETB,49990,54990,10,img/etb-white-flare-es.webp,['ETB', 'ES'],https://collectorcenter.cl/collections/ver-todo-pokemon,1756958265443</v>
+        <v>etb-white-flare-es,Llama Blanca – Elite Trainer Box,ETB,ESPAÑOL,ETB,49990,54990,10,img/etb-white-flare-es.webp,['ETB', 'ES'],https://collectorcenter.cl/collections/ver-todo-pokemon,1756958265443</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" t="s">
         <v>27</v>
       </c>
-      <c r="B10" t="s">
-        <v>39</v>
-      </c>
-      <c r="C10" t="s">
-        <v>28</v>
-      </c>
-      <c r="D10" t="s">
-        <v>31</v>
-      </c>
       <c r="E10" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="F10">
         <v>54990</v>
@@ -1016,17 +987,17 @@
         <v>img/etb-surging-sparks-en.webp</v>
       </c>
       <c r="J10" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="K10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L10">
         <v>1756612665443</v>
       </c>
       <c r="O10" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>etb-surging-sparks-en,Surging Sparks – Elite Trainer Box – Inglés,SV Surging Sparks,INGLÉS,ETB,54990,64990,10,img/etb-surging-sparks-en.webp,['ETB', 'EN'],https://collectorcenter.cl/collections/ver-todo-pokemon,1756612665443</v>
+        <v>etb-surging-sparks-en,Surging Sparks – Elite Trainer Box,ETB,INGLÉS,ETB,54990,64990,10,img/etb-surging-sparks-en.webp,['ETB', 'EN'],https://collectorcenter.cl/collections/ver-todo-pokemon,1756612665443</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ActualizaciÃ³n completa (2025-09-17 15:01)
</commit_message>
<xml_diff>
--- a/BACKUP/SUPORT IMAGEN.xlsx
+++ b/BACKUP/SUPORT IMAGEN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jorgg\OneDrive\MasterHIT\BACKUP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFDD00E4-B99E-4718-9CB4-F3FACC95ABB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6158CFFA-F2F1-44D9-88E9-B4201796AD85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="42">
   <si>
     <t>id,name,set,type,category,price,compareAtPrice,stock,image,tags,source,createdAt</t>
   </si>
@@ -78,12 +78,6 @@
     <t>createdAt</t>
   </si>
   <si>
-    <t>spc-prismatic-es</t>
-  </si>
-  <si>
-    <t>['SPC', 'ES']</t>
-  </si>
-  <si>
     <t>https://collectorcenter.cl/collections/ver-todo-pokemon</t>
   </si>
   <si>
@@ -111,9 +105,6 @@
     <t>etb-white-flare-es</t>
   </si>
   <si>
-    <t>etb-surging-sparks-en</t>
-  </si>
-  <si>
     <t>etb-prismatic-en</t>
   </si>
   <si>
@@ -123,55 +114,55 @@
     <t>INGLÉS</t>
   </si>
   <si>
-    <t>SPC</t>
-  </si>
-  <si>
     <t>ETB</t>
   </si>
   <si>
-    <t>Evoluciones Prismáticas – Super Premium Collection</t>
-  </si>
-  <si>
-    <t>Evoluciones Prismáticas – Elite Trainer Box</t>
-  </si>
-  <si>
-    <t>White Flare – Elite Trainer Box</t>
-  </si>
-  <si>
-    <t>Black Bolt – Elite Trainer Box</t>
-  </si>
-  <si>
-    <t>Aventuras Compartidas – Elite Trainer Box</t>
-  </si>
-  <si>
-    <t>Llama Blanca – Elite Trainer Box</t>
-  </si>
-  <si>
-    <t>Surging Sparks – Elite Trainer Box</t>
-  </si>
-  <si>
-    <t>spc-prismatic-es,Evoluciones Prismáticas – Super Premium Collection,SPC,ESPAÑOL,SPC,99990,129990,10,img/spc-prismatic-es.webp,['SPC', 'ES'],https://collectorcenter.cl/collections/ver-todo-pokemon,1757822265443</t>
-  </si>
-  <si>
-    <t>etb-prismatic-es,Evoluciones Prismáticas – Elite Trainer Box,ETB,ESPAÑOL,ETB,49990,69990,10,img/etb-prismatic-es.webp,['ETB', 'ES'],https://collectorcenter.cl/collections/ver-todo-pokemon,1757735865443</t>
-  </si>
-  <si>
-    <t>etb-prismatic-en,Evoluciones Prismáticas – Elite Trainer Box,ETB,INGLÉS,ETB,49990,69990,10,img/etb-prismatic-en.webp,['ETB', 'ES'],https://collectorcenter.cl/collections/ver-todo-pokemon,1757735865443</t>
-  </si>
-  <si>
-    <t>etb-white-flare-en,White Flare – Elite Trainer Box,ETB,INGLÉS,ETB,59990,67990,10,img/etb-white-flare-en.webp,['ETB', 'EN'],https://collectorcenter.cl/collections/ver-todo-pokemon,1757649465443</t>
-  </si>
-  <si>
-    <t>etb-black-bolt-en,Black Bolt – Elite Trainer Box,ETB,INGLÉS,ETB,59990,67990,10,img/etb-black-bolt-en.webp,['ETB', 'EN'],https://collectorcenter.cl/collections/ver-todo-pokemon,1757563065443</t>
-  </si>
-  <si>
-    <t>etb-black-bolt-es,Black Bolt – Elite Trainer Box,ETB,ESPAÑOL,ETB,49990,54990,10,img/etb-black-bolt-es.webp,['ETB', 'ES'],https://collectorcenter.cl/collections/ver-todo-pokemon,1757390265443</t>
-  </si>
-  <si>
-    <t>etb-aventuras-es,Aventuras Compartidas – Elite Trainer Box,ETB,ESPAÑOL,ETB,42990,59990,10,img/etb-aventuras-es.webp,['ETB', 'ES'],https://collectorcenter.cl/collections/ver-todo-pokemon,1757044665443</t>
-  </si>
-  <si>
-    <t>etb-white-flare-es,Llama Blanca – Elite Trainer Box,ETB,ESPAÑOL,ETB,49990,54990,10,img/etb-white-flare-es.webp,['ETB', 'ES'],https://collectorcenter.cl/collections/ver-todo-pokemon,1756958265443</t>
+    <t>Prismatic Evolutions</t>
+  </si>
+  <si>
+    <t>Evoluciones Prismáticas</t>
+  </si>
+  <si>
+    <t>White Flare</t>
+  </si>
+  <si>
+    <t>Black Bolt</t>
+  </si>
+  <si>
+    <t>Aventuras Compartidas</t>
+  </si>
+  <si>
+    <t>Llama Blanca</t>
+  </si>
+  <si>
+    <t>Journey Together</t>
+  </si>
+  <si>
+    <t>Fulgor Negro</t>
+  </si>
+  <si>
+    <t>etb-prismatic-en,Prismatic Evolutions,ETB,INGLÉS,ETB,49990,69990,10,img/etb-prismatic-en.webp,['ETB', 'ES'],https://collectorcenter.cl/collections/ver-todo-pokemon,1757735865443</t>
+  </si>
+  <si>
+    <t>etb-prismatic-es,Evoluciones Prismáticas,ETB,ESPAÑOL,ETB,49990,69990,10,img/etb-prismatic-es.webp,['ETB', 'ES'],https://collectorcenter.cl/collections/ver-todo-pokemon,1757735865443</t>
+  </si>
+  <si>
+    <t>etb-white-flare-en,White Flare,ETB,INGLÉS,ETB,49990,67990,10,img/etb-white-flare-en.webp,['ETB', 'EN'],https://collectorcenter.cl/collections/ver-todo-pokemon,1757649465443</t>
+  </si>
+  <si>
+    <t>etb-white-flare-en,Llama Blanca,ETB,ESPAÑOL,ETB,49990,67990,10,img/etb-white-flare-en.webp,['ETB', 'EN'],https://collectorcenter.cl/collections/ver-todo-pokemon,1757563065443</t>
+  </si>
+  <si>
+    <t>etb-black-bolt-en,Black Bolt,ETB,INGLÉS,ETB,49990,54990,10,img/etb-black-bolt-en.webp,['ETB', 'ES'],https://collectorcenter.cl/collections/ver-todo-pokemon,1757390265443</t>
+  </si>
+  <si>
+    <t>etb-black-bolt-es,Fulgor Negro,ETB,ESPAÑOL,ETB,49990,59990,10,img/etb-black-bolt-es.webp,['ETB', 'ES'],https://collectorcenter.cl/collections/ver-todo-pokemon,1757044665443</t>
+  </si>
+  <si>
+    <t>etb-white-flare-es,Journey Together,ETB,INGLÉS,ETB,49990,54990,10,img/etb-white-flare-es.webp,['ETB', 'ES'],https://collectorcenter.cl/collections/ver-todo-pokemon,1756958265443</t>
+  </si>
+  <si>
+    <t>etb-aventuras-es,Aventuras Compartidas,ETB,ESPAÑOL,ETB,49990,54990,10,img/etb-aventuras-es.webp,['ETB', 'ES'],https://collectorcenter.cl/collections/ver-todo-pokemon,1756958265443</t>
   </si>
 </sst>
 </file>
@@ -511,42 +502,42 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -556,10 +547,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3CA635C-1DF7-4EEC-B0B8-3FA5C80D03DF}">
-  <dimension ref="A1:O10"/>
+  <dimension ref="A1:O9"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1:O10"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="O9" sqref="O1:O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -568,6 +559,7 @@
     <col min="2" max="2" width="53" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.7265625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.1796875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11.81640625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="11.1796875" bestFit="1" customWidth="1"/>
   </cols>
@@ -615,62 +607,62 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F2">
-        <v>99990</v>
+        <v>49990</v>
       </c>
       <c r="G2">
-        <v>129990</v>
+        <v>69990</v>
       </c>
       <c r="H2">
         <v>10</v>
       </c>
       <c r="I2" t="str">
         <f>CONCATENATE("img/",A2,".webp")</f>
-        <v>img/spc-prismatic-es.webp</v>
+        <v>img/etb-prismatic-en.webp</v>
       </c>
       <c r="J2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="K2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="L2">
-        <v>1757822265443</v>
+        <v>1757735865443</v>
       </c>
       <c r="O2" s="1" t="str">
-        <f t="shared" ref="O2:O10" si="0">CONCATENATE(A2,",",B2,",",C2,",",D2,",",E2,",",F2,",",G2,",",H2,",",I2,",",J2,",",K2,",",L2)</f>
-        <v>spc-prismatic-es,Evoluciones Prismáticas – Super Premium Collection,SPC,ESPAÑOL,SPC,99990,129990,10,img/spc-prismatic-es.webp,['SPC', 'ES'],https://collectorcenter.cl/collections/ver-todo-pokemon,1757822265443</v>
+        <f>CONCATENATE(A2,",",B2,",",C2,",",D2,",",E2,",",F2,",",G2,",",H2,",",I2,",",J2,",",K2,",",L2)</f>
+        <v>etb-prismatic-en,Prismatic Evolutions,ETB,INGLÉS,ETB,49990,69990,10,img/etb-prismatic-en.webp,['ETB', 'ES'],https://collectorcenter.cl/collections/ver-todo-pokemon,1757735865443</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="F3">
         <v>49990</v>
@@ -682,84 +674,84 @@
         <v>10</v>
       </c>
       <c r="I3" t="str">
-        <f t="shared" ref="I3:I10" si="1">CONCATENATE("img/",A3,".webp")</f>
+        <f t="shared" ref="I3:I9" si="0">CONCATENATE("img/",A3,".webp")</f>
         <v>img/etb-prismatic-es.webp</v>
       </c>
       <c r="J3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="K3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="L3">
         <v>1757735865443</v>
       </c>
       <c r="O3" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>etb-prismatic-es,Evoluciones Prismáticas – Elite Trainer Box,ETB,ESPAÑOL,ETB,49990,69990,10,img/etb-prismatic-es.webp,['ETB', 'ES'],https://collectorcenter.cl/collections/ver-todo-pokemon,1757735865443</v>
+        <f t="shared" ref="O3:O9" si="1">CONCATENATE(A3,",",B3,",",C3,",",D3,",",E3,",",F3,",",G3,",",H3,",",I3,",",J3,",",K3,",",L3)</f>
+        <v>etb-prismatic-es,Evoluciones Prismáticas,ETB,ESPAÑOL,ETB,49990,69990,10,img/etb-prismatic-es.webp,['ETB', 'ES'],https://collectorcenter.cl/collections/ver-todo-pokemon,1757735865443</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C4" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E4" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="F4">
         <v>49990</v>
       </c>
       <c r="G4">
-        <v>69990</v>
+        <v>67990</v>
       </c>
       <c r="H4">
         <v>10</v>
       </c>
       <c r="I4" t="str">
-        <f t="shared" si="1"/>
-        <v>img/etb-prismatic-en.webp</v>
+        <f t="shared" si="0"/>
+        <v>img/etb-white-flare-en.webp</v>
       </c>
       <c r="J4" t="s">
         <v>17</v>
       </c>
       <c r="K4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="L4">
-        <v>1757735865443</v>
+        <v>1757649465443</v>
       </c>
       <c r="O4" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>etb-prismatic-en,Evoluciones Prismáticas – Elite Trainer Box,ETB,INGLÉS,ETB,49990,69990,10,img/etb-prismatic-en.webp,['ETB', 'ES'],https://collectorcenter.cl/collections/ver-todo-pokemon,1757735865443</v>
+        <f t="shared" si="1"/>
+        <v>etb-white-flare-en,White Flare,ETB,INGLÉS,ETB,49990,67990,10,img/etb-white-flare-en.webp,['ETB', 'EN'],https://collectorcenter.cl/collections/ver-todo-pokemon,1757649465443</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C5" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D5" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="E5" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="F5">
-        <v>59990</v>
+        <v>49990</v>
       </c>
       <c r="G5">
         <v>67990</v>
@@ -768,167 +760,167 @@
         <v>10</v>
       </c>
       <c r="I5" t="str">
+        <f t="shared" si="0"/>
+        <v>img/etb-white-flare-en.webp</v>
+      </c>
+      <c r="J5" t="s">
+        <v>17</v>
+      </c>
+      <c r="K5" t="s">
+        <v>13</v>
+      </c>
+      <c r="L5">
+        <v>1757563065443</v>
+      </c>
+      <c r="O5" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>img/etb-white-flare-en.webp</v>
-      </c>
-      <c r="J5" t="s">
-        <v>19</v>
-      </c>
-      <c r="K5" t="s">
-        <v>15</v>
-      </c>
-      <c r="L5">
-        <v>1757649465443</v>
-      </c>
-      <c r="O5" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>etb-white-flare-en,White Flare – Elite Trainer Box,ETB,INGLÉS,ETB,59990,67990,10,img/etb-white-flare-en.webp,['ETB', 'EN'],https://collectorcenter.cl/collections/ver-todo-pokemon,1757649465443</v>
+        <v>etb-white-flare-en,Llama Blanca,ETB,ESPAÑOL,ETB,49990,67990,10,img/etb-white-flare-en.webp,['ETB', 'EN'],https://collectorcenter.cl/collections/ver-todo-pokemon,1757563065443</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C6" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D6" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E6" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="F6">
-        <v>59990</v>
+        <v>49990</v>
       </c>
       <c r="G6">
-        <v>67990</v>
+        <v>54990</v>
       </c>
       <c r="H6">
         <v>10</v>
       </c>
       <c r="I6" t="str">
+        <f t="shared" si="0"/>
+        <v>img/etb-black-bolt-en.webp</v>
+      </c>
+      <c r="J6" t="s">
+        <v>15</v>
+      </c>
+      <c r="K6" t="s">
+        <v>13</v>
+      </c>
+      <c r="L6">
+        <v>1757390265443</v>
+      </c>
+      <c r="O6" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>img/etb-black-bolt-en.webp</v>
-      </c>
-      <c r="J6" t="s">
-        <v>19</v>
-      </c>
-      <c r="K6" t="s">
-        <v>15</v>
-      </c>
-      <c r="L6">
-        <v>1757563065443</v>
-      </c>
-      <c r="O6" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>etb-black-bolt-en,Black Bolt – Elite Trainer Box,ETB,INGLÉS,ETB,59990,67990,10,img/etb-black-bolt-en.webp,['ETB', 'EN'],https://collectorcenter.cl/collections/ver-todo-pokemon,1757563065443</v>
+        <v>etb-black-bolt-en,Black Bolt,ETB,INGLÉS,ETB,49990,54990,10,img/etb-black-bolt-en.webp,['ETB', 'ES'],https://collectorcenter.cl/collections/ver-todo-pokemon,1757390265443</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B7" t="s">
         <v>33</v>
       </c>
       <c r="C7" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D7" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E7" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="F7">
         <v>49990</v>
       </c>
       <c r="G7">
-        <v>54990</v>
+        <v>59990</v>
       </c>
       <c r="H7">
         <v>10</v>
       </c>
       <c r="I7" t="str">
+        <f t="shared" si="0"/>
+        <v>img/etb-black-bolt-es.webp</v>
+      </c>
+      <c r="J7" t="s">
+        <v>15</v>
+      </c>
+      <c r="K7" t="s">
+        <v>13</v>
+      </c>
+      <c r="L7">
+        <v>1757044665443</v>
+      </c>
+      <c r="O7" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>img/etb-black-bolt-es.webp</v>
-      </c>
-      <c r="J7" t="s">
-        <v>17</v>
-      </c>
-      <c r="K7" t="s">
-        <v>15</v>
-      </c>
-      <c r="L7">
-        <v>1757390265443</v>
-      </c>
-      <c r="O7" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>etb-black-bolt-es,Black Bolt – Elite Trainer Box,ETB,ESPAÑOL,ETB,49990,54990,10,img/etb-black-bolt-es.webp,['ETB', 'ES'],https://collectorcenter.cl/collections/ver-todo-pokemon,1757390265443</v>
+        <v>etb-black-bolt-es,Fulgor Negro,ETB,ESPAÑOL,ETB,49990,59990,10,img/etb-black-bolt-es.webp,['ETB', 'ES'],https://collectorcenter.cl/collections/ver-todo-pokemon,1757044665443</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B8" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C8" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E8" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="F8">
-        <v>42990</v>
+        <v>49990</v>
       </c>
       <c r="G8">
-        <v>59990</v>
+        <v>54990</v>
       </c>
       <c r="H8">
         <v>10</v>
       </c>
       <c r="I8" t="str">
+        <f t="shared" si="0"/>
+        <v>img/etb-white-flare-es.webp</v>
+      </c>
+      <c r="J8" t="s">
+        <v>15</v>
+      </c>
+      <c r="K8" t="s">
+        <v>13</v>
+      </c>
+      <c r="L8">
+        <v>1756958265443</v>
+      </c>
+      <c r="O8" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>img/etb-aventuras-es.webp</v>
-      </c>
-      <c r="J8" t="s">
-        <v>17</v>
-      </c>
-      <c r="K8" t="s">
-        <v>15</v>
-      </c>
-      <c r="L8">
-        <v>1757044665443</v>
-      </c>
-      <c r="O8" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>etb-aventuras-es,Aventuras Compartidas – Elite Trainer Box,ETB,ESPAÑOL,ETB,42990,59990,10,img/etb-aventuras-es.webp,['ETB', 'ES'],https://collectorcenter.cl/collections/ver-todo-pokemon,1757044665443</v>
+        <v>etb-white-flare-es,Journey Together,ETB,INGLÉS,ETB,49990,54990,10,img/etb-white-flare-es.webp,['ETB', 'ES'],https://collectorcenter.cl/collections/ver-todo-pokemon,1756958265443</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" t="s">
         <v>23</v>
       </c>
-      <c r="B9" t="s">
-        <v>35</v>
-      </c>
-      <c r="C9" t="s">
-        <v>29</v>
-      </c>
-      <c r="D9" t="s">
-        <v>26</v>
-      </c>
       <c r="E9" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="F9">
         <v>49990</v>
@@ -940,64 +932,21 @@
         <v>10</v>
       </c>
       <c r="I9" t="str">
-        <f t="shared" si="1"/>
-        <v>img/etb-white-flare-es.webp</v>
+        <f t="shared" si="0"/>
+        <v>img/etb-aventuras-es.webp</v>
       </c>
       <c r="J9" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="K9" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="L9">
         <v>1756958265443</v>
       </c>
       <c r="O9" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>etb-white-flare-es,Llama Blanca – Elite Trainer Box,ETB,ESPAÑOL,ETB,49990,54990,10,img/etb-white-flare-es.webp,['ETB', 'ES'],https://collectorcenter.cl/collections/ver-todo-pokemon,1756958265443</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>24</v>
-      </c>
-      <c r="B10" t="s">
-        <v>36</v>
-      </c>
-      <c r="C10" t="s">
-        <v>29</v>
-      </c>
-      <c r="D10" t="s">
-        <v>27</v>
-      </c>
-      <c r="E10" t="s">
-        <v>29</v>
-      </c>
-      <c r="F10">
-        <v>54990</v>
-      </c>
-      <c r="G10">
-        <v>64990</v>
-      </c>
-      <c r="H10">
-        <v>10</v>
-      </c>
-      <c r="I10" t="str">
         <f t="shared" si="1"/>
-        <v>img/etb-surging-sparks-en.webp</v>
-      </c>
-      <c r="J10" t="s">
-        <v>19</v>
-      </c>
-      <c r="K10" t="s">
-        <v>15</v>
-      </c>
-      <c r="L10">
-        <v>1756612665443</v>
-      </c>
-      <c r="O10" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>etb-surging-sparks-en,Surging Sparks – Elite Trainer Box,ETB,INGLÉS,ETB,54990,64990,10,img/etb-surging-sparks-en.webp,['ETB', 'EN'],https://collectorcenter.cl/collections/ver-todo-pokemon,1756612665443</v>
+        <v>etb-aventuras-es,Aventuras Compartidas,ETB,ESPAÑOL,ETB,49990,54990,10,img/etb-aventuras-es.webp,['ETB', 'ES'],https://collectorcenter.cl/collections/ver-todo-pokemon,1756958265443</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ActualizaciÃ³n completa (2025-09-17 15:04)
</commit_message>
<xml_diff>
--- a/BACKUP/SUPORT IMAGEN.xlsx
+++ b/BACKUP/SUPORT IMAGEN.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jorgg\OneDrive\MasterHIT\BACKUP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6158CFFA-F2F1-44D9-88E9-B4201796AD85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD65CA7B-AC40-418E-9578-69F1A53BBDEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="41">
   <si>
     <t>id,name,set,type,category,price,compareAtPrice,stock,image,tags,source,createdAt</t>
   </si>
@@ -102,9 +102,6 @@
     <t>etb-aventuras-es</t>
   </si>
   <si>
-    <t>etb-white-flare-es</t>
-  </si>
-  <si>
     <t>etb-prismatic-en</t>
   </si>
   <si>
@@ -159,10 +156,10 @@
     <t>etb-black-bolt-es,Fulgor Negro,ETB,ESPAÑOL,ETB,49990,59990,10,img/etb-black-bolt-es.webp,['ETB', 'ES'],https://collectorcenter.cl/collections/ver-todo-pokemon,1757044665443</t>
   </si>
   <si>
-    <t>etb-white-flare-es,Journey Together,ETB,INGLÉS,ETB,49990,54990,10,img/etb-white-flare-es.webp,['ETB', 'ES'],https://collectorcenter.cl/collections/ver-todo-pokemon,1756958265443</t>
-  </si>
-  <si>
     <t>etb-aventuras-es,Aventuras Compartidas,ETB,ESPAÑOL,ETB,49990,54990,10,img/etb-aventuras-es.webp,['ETB', 'ES'],https://collectorcenter.cl/collections/ver-todo-pokemon,1756958265443</t>
+  </si>
+  <si>
+    <t>etb-aventuras-es,Journey Together,ETB,INGLÉS,ETB,49990,54990,10,img/etb-aventuras-es.webp,['ETB', 'ES'],https://collectorcenter.cl/collections/ver-todo-pokemon,1756958265443</t>
   </si>
 </sst>
 </file>
@@ -489,8 +486,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A1:A9"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -502,32 +499,32 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.35">
@@ -537,7 +534,7 @@
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -549,8 +546,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3CA635C-1DF7-4EEC-B0B8-3FA5C80D03DF}">
   <dimension ref="A1:O9"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O9" sqref="O1:O9"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -607,19 +604,19 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F2">
         <v>49990</v>
@@ -653,16 +650,16 @@
         <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F3">
         <v>49990</v>
@@ -696,16 +693,16 @@
         <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F4">
         <v>49990</v>
@@ -739,16 +736,16 @@
         <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F5">
         <v>49990</v>
@@ -782,16 +779,16 @@
         <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F6">
         <v>49990</v>
@@ -825,16 +822,16 @@
         <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F7">
         <v>49990</v>
@@ -865,19 +862,19 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F8">
         <v>49990</v>
@@ -890,7 +887,7 @@
       </c>
       <c r="I8" t="str">
         <f t="shared" si="0"/>
-        <v>img/etb-white-flare-es.webp</v>
+        <v>img/etb-aventuras-es.webp</v>
       </c>
       <c r="J8" t="s">
         <v>15</v>
@@ -903,7 +900,7 @@
       </c>
       <c r="O8" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>etb-white-flare-es,Journey Together,ETB,INGLÉS,ETB,49990,54990,10,img/etb-white-flare-es.webp,['ETB', 'ES'],https://collectorcenter.cl/collections/ver-todo-pokemon,1756958265443</v>
+        <v>etb-aventuras-es,Journey Together,ETB,INGLÉS,ETB,49990,54990,10,img/etb-aventuras-es.webp,['ETB', 'ES'],https://collectorcenter.cl/collections/ver-todo-pokemon,1756958265443</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.35">
@@ -911,16 +908,16 @@
         <v>20</v>
       </c>
       <c r="B9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F9">
         <v>49990</v>

</xml_diff>

<commit_message>
ActualizaciÃ³n completa (2025-09-21 16:46)
</commit_message>
<xml_diff>
--- a/BACKUP/SUPORT IMAGEN.xlsx
+++ b/BACKUP/SUPORT IMAGEN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jorgg\OneDrive\MasterHIT\BACKUP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD65CA7B-AC40-418E-9578-69F1A53BBDEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30E6D466-2AAE-4DC2-BB85-8630B1937942}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="55">
   <si>
     <t>id,name,set,type,category,price,compareAtPrice,stock,image,tags,source,createdAt</t>
   </si>
@@ -78,21 +78,12 @@
     <t>createdAt</t>
   </si>
   <si>
-    <t>https://collectorcenter.cl/collections/ver-todo-pokemon</t>
-  </si>
-  <si>
     <t>etb-prismatic-es</t>
   </si>
   <si>
-    <t>['ETB', 'ES']</t>
-  </si>
-  <si>
     <t>etb-white-flare-en</t>
   </si>
   <si>
-    <t>['ETB', 'EN']</t>
-  </si>
-  <si>
     <t>etb-black-bolt-en</t>
   </si>
   <si>
@@ -160,6 +151,57 @@
   </si>
   <si>
     <t>etb-aventuras-es,Journey Together,ETB,INGLÉS,ETB,49990,54990,10,img/etb-aventuras-es.webp,['ETB', 'ES'],https://collectorcenter.cl/collections/ver-todo-pokemon,1756958265443</t>
+  </si>
+  <si>
+    <t>etb-destined-es</t>
+  </si>
+  <si>
+    <t>Rivales Predestinados</t>
+  </si>
+  <si>
+    <t>bin-white-flare-es</t>
+  </si>
+  <si>
+    <t>bin-black-bolt-es</t>
+  </si>
+  <si>
+    <t>BINDER</t>
+  </si>
+  <si>
+    <t>special-charizardex-en</t>
+  </si>
+  <si>
+    <t>Charizard EX</t>
+  </si>
+  <si>
+    <t>SPECIAL</t>
+  </si>
+  <si>
+    <t>poster-prismatic-en</t>
+  </si>
+  <si>
+    <t>POSTER</t>
+  </si>
+  <si>
+    <t>special-garchomp-en</t>
+  </si>
+  <si>
+    <t>Garchomp EX</t>
+  </si>
+  <si>
+    <t>surprisebox-en</t>
+  </si>
+  <si>
+    <t>SURPRISE BOX</t>
+  </si>
+  <si>
+    <t>etb-megagardevoir-en</t>
+  </si>
+  <si>
+    <t>etb-megalucario-en</t>
+  </si>
+  <si>
+    <t>Mega Evolutions</t>
   </si>
 </sst>
 </file>
@@ -499,42 +541,42 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -544,21 +586,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3CA635C-1DF7-4EEC-B0B8-3FA5C80D03DF}">
-  <dimension ref="A1:O9"/>
+  <dimension ref="A1:O23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="22.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="53" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.453125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25.1796875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.08984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="28.7265625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.36328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.36328125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.90625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="105.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.35">
@@ -604,19 +650,19 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F2">
         <v>49990</v>
@@ -631,35 +677,36 @@
         <f>CONCATENATE("img/",A2,".webp")</f>
         <v>img/etb-prismatic-en.webp</v>
       </c>
-      <c r="J2" t="s">
-        <v>15</v>
-      </c>
-      <c r="K2" t="s">
-        <v>13</v>
+      <c r="J2" t="str">
+        <f t="shared" ref="J2:J10" si="0">CONCATENATE("['",C2,",'",D2,"']")</f>
+        <v>['ETB,'INGLÉS']</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
       </c>
       <c r="L2">
-        <v>1757735865443</v>
+        <v>1</v>
       </c>
       <c r="O2" s="1" t="str">
         <f>CONCATENATE(A2,",",B2,",",C2,",",D2,",",E2,",",F2,",",G2,",",H2,",",I2,",",J2,",",K2,",",L2)</f>
-        <v>etb-prismatic-en,Prismatic Evolutions,ETB,INGLÉS,ETB,49990,69990,10,img/etb-prismatic-en.webp,['ETB', 'ES'],https://collectorcenter.cl/collections/ver-todo-pokemon,1757735865443</v>
+        <v>etb-prismatic-en,Prismatic Evolutions,ETB,INGLÉS,ETB,49990,69990,10,img/etb-prismatic-en.webp,['ETB,'INGLÉS'],1,1</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F3">
         <v>49990</v>
@@ -671,38 +718,39 @@
         <v>10</v>
       </c>
       <c r="I3" t="str">
-        <f t="shared" ref="I3:I9" si="0">CONCATENATE("img/",A3,".webp")</f>
+        <f t="shared" ref="I3:I9" si="1">CONCATENATE("img/",A3,".webp")</f>
         <v>img/etb-prismatic-es.webp</v>
       </c>
-      <c r="J3" t="s">
-        <v>15</v>
-      </c>
-      <c r="K3" t="s">
-        <v>13</v>
+      <c r="J3" t="str">
+        <f t="shared" si="0"/>
+        <v>['ETB,'ESPAÑOL']</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
       </c>
       <c r="L3">
-        <v>1757735865443</v>
+        <v>1</v>
       </c>
       <c r="O3" s="1" t="str">
-        <f t="shared" ref="O3:O9" si="1">CONCATENATE(A3,",",B3,",",C3,",",D3,",",E3,",",F3,",",G3,",",H3,",",I3,",",J3,",",K3,",",L3)</f>
-        <v>etb-prismatic-es,Evoluciones Prismáticas,ETB,ESPAÑOL,ETB,49990,69990,10,img/etb-prismatic-es.webp,['ETB', 'ES'],https://collectorcenter.cl/collections/ver-todo-pokemon,1757735865443</v>
+        <f t="shared" ref="O3:O9" si="2">CONCATENATE(A3,",",B3,",",C3,",",D3,",",E3,",",F3,",",G3,",",H3,",",I3,",",J3,",",K3,",",L3)</f>
+        <v>etb-prismatic-es,Evoluciones Prismáticas,ETB,ESPAÑOL,ETB,49990,69990,10,img/etb-prismatic-es.webp,['ETB,'ESPAÑOL'],1,1</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F4">
         <v>49990</v>
@@ -714,38 +762,39 @@
         <v>10</v>
       </c>
       <c r="I4" t="str">
+        <f t="shared" si="1"/>
+        <v>img/etb-white-flare-en.webp</v>
+      </c>
+      <c r="J4" t="str">
         <f t="shared" si="0"/>
-        <v>img/etb-white-flare-en.webp</v>
-      </c>
-      <c r="J4" t="s">
-        <v>17</v>
-      </c>
-      <c r="K4" t="s">
-        <v>13</v>
+        <v>['ETB,'INGLÉS']</v>
+      </c>
+      <c r="K4">
+        <v>1</v>
       </c>
       <c r="L4">
-        <v>1757649465443</v>
+        <v>1</v>
       </c>
       <c r="O4" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>etb-white-flare-en,White Flare,ETB,INGLÉS,ETB,49990,67990,10,img/etb-white-flare-en.webp,['ETB', 'EN'],https://collectorcenter.cl/collections/ver-todo-pokemon,1757649465443</v>
+        <f t="shared" si="2"/>
+        <v>etb-white-flare-en,White Flare,ETB,INGLÉS,ETB,49990,67990,10,img/etb-white-flare-en.webp,['ETB,'INGLÉS'],1,1</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D5" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F5">
         <v>49990</v>
@@ -757,38 +806,39 @@
         <v>10</v>
       </c>
       <c r="I5" t="str">
+        <f t="shared" si="1"/>
+        <v>img/etb-white-flare-en.webp</v>
+      </c>
+      <c r="J5" t="str">
         <f t="shared" si="0"/>
-        <v>img/etb-white-flare-en.webp</v>
-      </c>
-      <c r="J5" t="s">
-        <v>17</v>
-      </c>
-      <c r="K5" t="s">
-        <v>13</v>
+        <v>['ETB,'ESPAÑOL']</v>
+      </c>
+      <c r="K5">
+        <v>1</v>
       </c>
       <c r="L5">
-        <v>1757563065443</v>
+        <v>1</v>
       </c>
       <c r="O5" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>etb-white-flare-en,Llama Blanca,ETB,ESPAÑOL,ETB,49990,67990,10,img/etb-white-flare-en.webp,['ETB', 'EN'],https://collectorcenter.cl/collections/ver-todo-pokemon,1757563065443</v>
+        <f t="shared" si="2"/>
+        <v>etb-white-flare-en,Llama Blanca,ETB,ESPAÑOL,ETB,49990,67990,10,img/etb-white-flare-en.webp,['ETB,'ESPAÑOL'],1,1</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C6" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D6" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E6" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F6">
         <v>49990</v>
@@ -800,38 +850,39 @@
         <v>10</v>
       </c>
       <c r="I6" t="str">
+        <f t="shared" si="1"/>
+        <v>img/etb-black-bolt-en.webp</v>
+      </c>
+      <c r="J6" t="str">
         <f t="shared" si="0"/>
-        <v>img/etb-black-bolt-en.webp</v>
-      </c>
-      <c r="J6" t="s">
-        <v>15</v>
-      </c>
-      <c r="K6" t="s">
-        <v>13</v>
+        <v>['ETB,'INGLÉS']</v>
+      </c>
+      <c r="K6">
+        <v>1</v>
       </c>
       <c r="L6">
-        <v>1757390265443</v>
+        <v>1</v>
       </c>
       <c r="O6" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>etb-black-bolt-en,Black Bolt,ETB,INGLÉS,ETB,49990,54990,10,img/etb-black-bolt-en.webp,['ETB', 'ES'],https://collectorcenter.cl/collections/ver-todo-pokemon,1757390265443</v>
+        <f t="shared" si="2"/>
+        <v>etb-black-bolt-en,Black Bolt,ETB,INGLÉS,ETB,49990,54990,10,img/etb-black-bolt-en.webp,['ETB,'INGLÉS'],1,1</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" t="s">
         <v>19</v>
       </c>
-      <c r="B7" t="s">
-        <v>32</v>
-      </c>
-      <c r="C7" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7" t="s">
-        <v>22</v>
-      </c>
       <c r="E7" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F7">
         <v>49990</v>
@@ -843,38 +894,39 @@
         <v>10</v>
       </c>
       <c r="I7" t="str">
+        <f t="shared" si="1"/>
+        <v>img/etb-black-bolt-es.webp</v>
+      </c>
+      <c r="J7" t="str">
         <f t="shared" si="0"/>
-        <v>img/etb-black-bolt-es.webp</v>
-      </c>
-      <c r="J7" t="s">
-        <v>15</v>
-      </c>
-      <c r="K7" t="s">
-        <v>13</v>
+        <v>['ETB,'ESPAÑOL']</v>
+      </c>
+      <c r="K7">
+        <v>1</v>
       </c>
       <c r="L7">
-        <v>1757044665443</v>
+        <v>1</v>
       </c>
       <c r="O7" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>etb-black-bolt-es,Fulgor Negro,ETB,ESPAÑOL,ETB,49990,59990,10,img/etb-black-bolt-es.webp,['ETB', 'ES'],https://collectorcenter.cl/collections/ver-todo-pokemon,1757044665443</v>
+        <f t="shared" si="2"/>
+        <v>etb-black-bolt-es,Fulgor Negro,ETB,ESPAÑOL,ETB,49990,59990,10,img/etb-black-bolt-es.webp,['ETB,'ESPAÑOL'],1,1</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" t="s">
         <v>20</v>
       </c>
-      <c r="B8" t="s">
-        <v>31</v>
-      </c>
-      <c r="C8" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" t="s">
-        <v>23</v>
-      </c>
       <c r="E8" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F8">
         <v>49990</v>
@@ -886,38 +938,39 @@
         <v>10</v>
       </c>
       <c r="I8" t="str">
+        <f t="shared" si="1"/>
+        <v>img/etb-aventuras-es.webp</v>
+      </c>
+      <c r="J8" t="str">
         <f t="shared" si="0"/>
-        <v>img/etb-aventuras-es.webp</v>
-      </c>
-      <c r="J8" t="s">
-        <v>15</v>
-      </c>
-      <c r="K8" t="s">
-        <v>13</v>
+        <v>['ETB,'INGLÉS']</v>
+      </c>
+      <c r="K8">
+        <v>1</v>
       </c>
       <c r="L8">
-        <v>1756958265443</v>
+        <v>1</v>
       </c>
       <c r="O8" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>etb-aventuras-es,Journey Together,ETB,INGLÉS,ETB,49990,54990,10,img/etb-aventuras-es.webp,['ETB', 'ES'],https://collectorcenter.cl/collections/ver-todo-pokemon,1756958265443</v>
+        <f t="shared" si="2"/>
+        <v>etb-aventuras-es,Journey Together,ETB,INGLÉS,ETB,49990,54990,10,img/etb-aventuras-es.webp,['ETB,'INGLÉS'],1,1</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B9" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C9" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D9" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E9" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F9">
         <v>49990</v>
@@ -929,21 +982,470 @@
         <v>10</v>
       </c>
       <c r="I9" t="str">
+        <f t="shared" si="1"/>
+        <v>img/etb-aventuras-es.webp</v>
+      </c>
+      <c r="J9" t="str">
         <f t="shared" si="0"/>
-        <v>img/etb-aventuras-es.webp</v>
-      </c>
-      <c r="J9" t="s">
-        <v>15</v>
-      </c>
-      <c r="K9" t="s">
-        <v>13</v>
+        <v>['ETB,'ESPAÑOL']</v>
+      </c>
+      <c r="K9">
+        <v>1</v>
       </c>
       <c r="L9">
-        <v>1756958265443</v>
+        <v>1</v>
       </c>
       <c r="O9" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>etb-aventuras-es,Aventuras Compartidas,ETB,ESPAÑOL,ETB,49990,54990,10,img/etb-aventuras-es.webp,['ETB', 'ES'],https://collectorcenter.cl/collections/ver-todo-pokemon,1756958265443</v>
+        <f t="shared" si="2"/>
+        <v>etb-aventuras-es,Aventuras Compartidas,ETB,ESPAÑOL,ETB,49990,54990,10,img/etb-aventuras-es.webp,['ETB,'ESPAÑOL'],1,1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" t="s">
+        <v>21</v>
+      </c>
+      <c r="F10">
+        <v>39990</v>
+      </c>
+      <c r="G10">
+        <v>54990</v>
+      </c>
+      <c r="H10">
+        <v>10</v>
+      </c>
+      <c r="I10" t="str">
+        <f t="shared" ref="I10:I15" si="3">CONCATENATE("img/",A10,".webp")</f>
+        <v>img/etb-destined-es.webp</v>
+      </c>
+      <c r="J10" t="str">
+        <f t="shared" si="0"/>
+        <v>['ETB,'ESPAÑOL']</v>
+      </c>
+      <c r="K10">
+        <v>1</v>
+      </c>
+      <c r="L10">
+        <v>1</v>
+      </c>
+      <c r="O10" s="1" t="str">
+        <f t="shared" ref="O10" si="4">CONCATENATE(A10,",",B10,",",C10,",",D10,",",E10,",",F10,",",G10,",",H10,",",I10,",",J10,",",K10,",",L10)</f>
+        <v>etb-destined-es,Rivales Predestinados,ETB,ESPAÑOL,ETB,39990,54990,10,img/etb-destined-es.webp,['ETB,'ESPAÑOL'],1,1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" t="s">
+        <v>42</v>
+      </c>
+      <c r="F11">
+        <v>34990</v>
+      </c>
+      <c r="G11">
+        <v>34990</v>
+      </c>
+      <c r="H11">
+        <v>10</v>
+      </c>
+      <c r="I11" t="str">
+        <f t="shared" si="3"/>
+        <v>img/bin-white-flare-es.webp</v>
+      </c>
+      <c r="J11" t="str">
+        <f>CONCATENATE("['",C11,",'",D11,"']")</f>
+        <v>['BINDER,'ESPAÑOL']</v>
+      </c>
+      <c r="K11">
+        <v>1</v>
+      </c>
+      <c r="L11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" t="s">
+        <v>42</v>
+      </c>
+      <c r="F12">
+        <v>34990</v>
+      </c>
+      <c r="G12">
+        <v>34990</v>
+      </c>
+      <c r="H12">
+        <v>10</v>
+      </c>
+      <c r="I12" t="str">
+        <f t="shared" si="3"/>
+        <v>img/bin-black-bolt-es.webp</v>
+      </c>
+      <c r="J12" t="str">
+        <f t="shared" ref="J12:J15" si="5">CONCATENATE("['",C12,",'",D12,"']")</f>
+        <v>['BINDER,'ESPAÑOL']</v>
+      </c>
+      <c r="K12">
+        <v>1</v>
+      </c>
+      <c r="L12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13" t="s">
+        <v>44</v>
+      </c>
+      <c r="C13" t="s">
+        <v>45</v>
+      </c>
+      <c r="D13" t="s">
+        <v>20</v>
+      </c>
+      <c r="E13" t="s">
+        <v>45</v>
+      </c>
+      <c r="F13">
+        <v>29990</v>
+      </c>
+      <c r="G13">
+        <v>29990</v>
+      </c>
+      <c r="H13">
+        <v>10</v>
+      </c>
+      <c r="I13" t="str">
+        <f t="shared" si="3"/>
+        <v>img/special-charizardex-en.webp</v>
+      </c>
+      <c r="J13" t="str">
+        <f t="shared" si="5"/>
+        <v>['SPECIAL,'INGLÉS']</v>
+      </c>
+      <c r="K13">
+        <v>1</v>
+      </c>
+      <c r="L13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14" t="s">
+        <v>45</v>
+      </c>
+      <c r="D14" t="s">
+        <v>19</v>
+      </c>
+      <c r="E14" t="s">
+        <v>45</v>
+      </c>
+      <c r="F14">
+        <v>29990</v>
+      </c>
+      <c r="G14">
+        <v>29990</v>
+      </c>
+      <c r="H14">
+        <v>10</v>
+      </c>
+      <c r="I14" t="str">
+        <f t="shared" si="3"/>
+        <v>img/special-charizardex-en.webp</v>
+      </c>
+      <c r="J14" t="str">
+        <f t="shared" si="5"/>
+        <v>['SPECIAL,'ESPAÑOL']</v>
+      </c>
+      <c r="K14">
+        <v>1</v>
+      </c>
+      <c r="L14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>46</v>
+      </c>
+      <c r="B15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" t="s">
+        <v>47</v>
+      </c>
+      <c r="D15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E15" t="s">
+        <v>47</v>
+      </c>
+      <c r="F15">
+        <v>19990</v>
+      </c>
+      <c r="G15">
+        <v>19990</v>
+      </c>
+      <c r="H15">
+        <v>10</v>
+      </c>
+      <c r="I15" t="str">
+        <f t="shared" si="3"/>
+        <v>img/poster-prismatic-en.webp</v>
+      </c>
+      <c r="J15" t="str">
+        <f t="shared" si="5"/>
+        <v>['POSTER,'ESPAÑOL']</v>
+      </c>
+      <c r="K15">
+        <v>1</v>
+      </c>
+      <c r="L15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>48</v>
+      </c>
+      <c r="B16" t="s">
+        <v>49</v>
+      </c>
+      <c r="C16" t="s">
+        <v>45</v>
+      </c>
+      <c r="D16" t="s">
+        <v>20</v>
+      </c>
+      <c r="E16" t="s">
+        <v>45</v>
+      </c>
+      <c r="F16">
+        <v>29990</v>
+      </c>
+      <c r="G16">
+        <v>29990</v>
+      </c>
+      <c r="H16">
+        <v>10</v>
+      </c>
+      <c r="I16" t="str">
+        <f t="shared" ref="I16:I17" si="6">CONCATENATE("img/",A16,".webp")</f>
+        <v>img/special-garchomp-en.webp</v>
+      </c>
+      <c r="J16" t="str">
+        <f t="shared" ref="J16:J17" si="7">CONCATENATE("['",C16,",'",D16,"']")</f>
+        <v>['SPECIAL,'INGLÉS']</v>
+      </c>
+      <c r="K16">
+        <v>1</v>
+      </c>
+      <c r="L16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>48</v>
+      </c>
+      <c r="B17" t="s">
+        <v>49</v>
+      </c>
+      <c r="C17" t="s">
+        <v>45</v>
+      </c>
+      <c r="D17" t="s">
+        <v>19</v>
+      </c>
+      <c r="E17" t="s">
+        <v>45</v>
+      </c>
+      <c r="F17">
+        <v>29990</v>
+      </c>
+      <c r="G17">
+        <v>29990</v>
+      </c>
+      <c r="H17">
+        <v>10</v>
+      </c>
+      <c r="I17" t="str">
+        <f t="shared" si="6"/>
+        <v>img/special-garchomp-en.webp</v>
+      </c>
+      <c r="J17" t="str">
+        <f t="shared" si="7"/>
+        <v>['SPECIAL,'ESPAÑOL']</v>
+      </c>
+      <c r="K17">
+        <v>1</v>
+      </c>
+      <c r="L17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>50</v>
+      </c>
+      <c r="B18" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" t="s">
+        <v>51</v>
+      </c>
+      <c r="D18" t="s">
+        <v>20</v>
+      </c>
+      <c r="E18" t="s">
+        <v>51</v>
+      </c>
+      <c r="F18">
+        <v>34990</v>
+      </c>
+      <c r="G18">
+        <v>34990</v>
+      </c>
+      <c r="H18">
+        <v>10</v>
+      </c>
+      <c r="I18" t="str">
+        <f t="shared" ref="I18:I19" si="8">CONCATENATE("img/",A18,".webp")</f>
+        <v>img/surprisebox-en.webp</v>
+      </c>
+      <c r="J18" t="str">
+        <f t="shared" ref="J18:J19" si="9">CONCATENATE("['",C18,",'",D18,"']")</f>
+        <v>['SURPRISE BOX,'INGLÉS']</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>50</v>
+      </c>
+      <c r="B19" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19" t="s">
+        <v>51</v>
+      </c>
+      <c r="D19" t="s">
+        <v>19</v>
+      </c>
+      <c r="E19" t="s">
+        <v>51</v>
+      </c>
+      <c r="F19">
+        <v>29990</v>
+      </c>
+      <c r="G19">
+        <v>29990</v>
+      </c>
+      <c r="H19">
+        <v>10</v>
+      </c>
+      <c r="I19" t="str">
+        <f t="shared" si="8"/>
+        <v>img/surprisebox-en.webp</v>
+      </c>
+      <c r="J19" t="str">
+        <f t="shared" si="9"/>
+        <v>['SURPRISE BOX,'ESPAÑOL']</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>53</v>
+      </c>
+      <c r="B20" t="s">
+        <v>54</v>
+      </c>
+      <c r="C20" t="s">
+        <v>21</v>
+      </c>
+      <c r="D20" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>53</v>
+      </c>
+      <c r="B21" t="s">
+        <v>54</v>
+      </c>
+      <c r="C21" t="s">
+        <v>21</v>
+      </c>
+      <c r="D21" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>52</v>
+      </c>
+      <c r="B22" t="s">
+        <v>54</v>
+      </c>
+      <c r="C22" t="s">
+        <v>21</v>
+      </c>
+      <c r="D22" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>52</v>
+      </c>
+      <c r="B23" t="s">
+        <v>54</v>
+      </c>
+      <c r="C23" t="s">
+        <v>21</v>
+      </c>
+      <c r="D23" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ActualizaciÃ³n completa (2025-09-21 17:45)
</commit_message>
<xml_diff>
--- a/BACKUP/SUPORT IMAGEN.xlsx
+++ b/BACKUP/SUPORT IMAGEN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jorgg\OneDrive\MasterHIT\BACKUP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30E6D466-2AAE-4DC2-BB85-8630B1937942}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A88C2211-A2C4-45B6-81EA-46935E73614A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="57">
   <si>
     <t>id,name,set,type,category,price,compareAtPrice,stock,image,tags,source,createdAt</t>
   </si>
@@ -93,9 +93,6 @@
     <t>etb-aventuras-es</t>
   </si>
   <si>
-    <t>etb-prismatic-en</t>
-  </si>
-  <si>
     <t>ESPAÑOL</t>
   </si>
   <si>
@@ -202,6 +199,15 @@
   </si>
   <si>
     <t>Mega Evolutions</t>
+  </si>
+  <si>
+    <t>Megaevolución</t>
+  </si>
+  <si>
+    <t>SPC</t>
+  </si>
+  <si>
+    <t>spc-prismatic-en</t>
   </si>
 </sst>
 </file>
@@ -529,7 +535,7 @@
   <dimension ref="A1:A9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A9"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -541,42 +547,42 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -588,7 +594,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3CA635C-1DF7-4EEC-B0B8-3FA5C80D03DF}">
   <dimension ref="A1:O23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -597,7 +605,7 @@
     <col min="3" max="3" width="12.54296875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.36328125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.81640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="5.08984375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="28.7265625" bestFit="1" customWidth="1"/>
@@ -650,36 +658,36 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>56</v>
       </c>
       <c r="B2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C2" t="s">
-        <v>21</v>
+        <v>55</v>
       </c>
       <c r="D2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E2" t="s">
-        <v>21</v>
+        <v>55</v>
       </c>
       <c r="F2">
-        <v>49990</v>
+        <v>139990</v>
       </c>
       <c r="G2">
-        <v>69990</v>
+        <v>139990</v>
       </c>
       <c r="H2">
         <v>10</v>
       </c>
       <c r="I2" t="str">
         <f>CONCATENATE("img/",A2,".webp")</f>
-        <v>img/etb-prismatic-en.webp</v>
+        <v>img/spc-prismatic-en.webp</v>
       </c>
       <c r="J2" t="str">
         <f t="shared" ref="J2:J10" si="0">CONCATENATE("['",C2,",'",D2,"']")</f>
-        <v>['ETB,'INGLÉS']</v>
+        <v>['SPC,'INGLÉS']</v>
       </c>
       <c r="K2">
         <v>1</v>
@@ -689,7 +697,7 @@
       </c>
       <c r="O2" s="1" t="str">
         <f>CONCATENATE(A2,",",B2,",",C2,",",D2,",",E2,",",F2,",",G2,",",H2,",",I2,",",J2,",",K2,",",L2)</f>
-        <v>etb-prismatic-en,Prismatic Evolutions,ETB,INGLÉS,ETB,49990,69990,10,img/etb-prismatic-en.webp,['ETB,'INGLÉS'],1,1</v>
+        <v>spc-prismatic-en,Prismatic Evolutions,SPC,INGLÉS,SPC,139990,139990,10,img/spc-prismatic-en.webp,['SPC,'INGLÉS'],1,1</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.35">
@@ -697,16 +705,16 @@
         <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F3">
         <v>49990</v>
@@ -741,16 +749,16 @@
         <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F4">
         <v>49990</v>
@@ -785,16 +793,16 @@
         <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F5">
         <v>49990</v>
@@ -829,16 +837,16 @@
         <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F6">
         <v>49990</v>
@@ -873,16 +881,16 @@
         <v>16</v>
       </c>
       <c r="B7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F7">
         <v>49990</v>
@@ -917,16 +925,16 @@
         <v>17</v>
       </c>
       <c r="B8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F8">
         <v>49990</v>
@@ -961,16 +969,16 @@
         <v>17</v>
       </c>
       <c r="B9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F9">
         <v>49990</v>
@@ -1002,19 +1010,19 @@
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" t="s">
         <v>38</v>
       </c>
-      <c r="B10" t="s">
-        <v>39</v>
-      </c>
       <c r="C10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F10">
         <v>39990</v>
@@ -1040,25 +1048,25 @@
         <v>1</v>
       </c>
       <c r="O10" s="1" t="str">
-        <f t="shared" ref="O10" si="4">CONCATENATE(A10,",",B10,",",C10,",",D10,",",E10,",",F10,",",G10,",",H10,",",I10,",",J10,",",K10,",",L10)</f>
+        <f t="shared" ref="O10:O23" si="4">CONCATENATE(A10,",",B10,",",C10,",",D10,",",E10,",",F10,",",G10,",",H10,",",I10,",",J10,",",K10,",",L10)</f>
         <v>etb-destined-es,Rivales Predestinados,ETB,ESPAÑOL,ETB,39990,54990,10,img/etb-destined-es.webp,['ETB,'ESPAÑOL'],1,1</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F11">
         <v>34990</v>
@@ -1083,22 +1091,26 @@
       <c r="L11">
         <v>1</v>
       </c>
+      <c r="O11" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>bin-white-flare-es,Llama Blanca,BINDER,ESPAÑOL,BINDER,34990,34990,10,img/bin-white-flare-es.webp,['BINDER,'ESPAÑOL'],1,1</v>
+      </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" t="s">
         <v>41</v>
       </c>
-      <c r="B12" t="s">
-        <v>29</v>
-      </c>
-      <c r="C12" t="s">
-        <v>42</v>
-      </c>
       <c r="D12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F12">
         <v>34990</v>
@@ -1123,22 +1135,26 @@
       <c r="L12">
         <v>1</v>
       </c>
+      <c r="O12" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>bin-black-bolt-es,Fulgor Negro,BINDER,ESPAÑOL,BINDER,34990,34990,10,img/bin-black-bolt-es.webp,['BINDER,'ESPAÑOL'],1,1</v>
+      </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" t="s">
         <v>43</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>44</v>
       </c>
-      <c r="C13" t="s">
-        <v>45</v>
-      </c>
       <c r="D13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F13">
         <v>29990</v>
@@ -1163,22 +1179,26 @@
       <c r="L13">
         <v>1</v>
       </c>
+      <c r="O13" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>special-charizardex-en,Charizard EX,SPECIAL,INGLÉS,SPECIAL,29990,29990,10,img/special-charizardex-en.webp,['SPECIAL,'INGLÉS'],1,1</v>
+      </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
+        <v>42</v>
+      </c>
+      <c r="B14" t="s">
         <v>43</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>44</v>
       </c>
-      <c r="C14" t="s">
-        <v>45</v>
-      </c>
       <c r="D14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F14">
         <v>29990</v>
@@ -1203,22 +1223,26 @@
       <c r="L14">
         <v>1</v>
       </c>
+      <c r="O14" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>special-charizardex-en,Charizard EX,SPECIAL,ESPAÑOL,SPECIAL,29990,29990,10,img/special-charizardex-en.webp,['SPECIAL,'ESPAÑOL'],1,1</v>
+      </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
+        <v>45</v>
+      </c>
+      <c r="B15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" t="s">
         <v>46</v>
       </c>
-      <c r="B15" t="s">
-        <v>22</v>
-      </c>
-      <c r="C15" t="s">
-        <v>47</v>
-      </c>
       <c r="D15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F15">
         <v>19990</v>
@@ -1243,22 +1267,26 @@
       <c r="L15">
         <v>1</v>
       </c>
+      <c r="O15" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>poster-prismatic-en,Prismatic Evolutions,POSTER,ESPAÑOL,POSTER,19990,19990,10,img/poster-prismatic-en.webp,['POSTER,'ESPAÑOL'],1,1</v>
+      </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16" t="s">
         <v>48</v>
       </c>
-      <c r="B16" t="s">
-        <v>49</v>
-      </c>
       <c r="C16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F16">
         <v>29990</v>
@@ -1283,22 +1311,26 @@
       <c r="L16">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="O16" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>special-garchomp-en,Garchomp EX,SPECIAL,INGLÉS,SPECIAL,29990,29990,10,img/special-garchomp-en.webp,['SPECIAL,'INGLÉS'],1,1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
+        <v>47</v>
+      </c>
+      <c r="B17" t="s">
         <v>48</v>
       </c>
-      <c r="B17" t="s">
-        <v>49</v>
-      </c>
       <c r="C17" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E17" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F17">
         <v>29990</v>
@@ -1323,22 +1355,26 @@
       <c r="L17">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="O17" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>special-garchomp-en,Garchomp EX,SPECIAL,ESPAÑOL,SPECIAL,29990,29990,10,img/special-garchomp-en.webp,['SPECIAL,'ESPAÑOL'],1,1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
+        <v>49</v>
+      </c>
+      <c r="B18" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" t="s">
         <v>50</v>
       </c>
-      <c r="B18" t="s">
-        <v>22</v>
-      </c>
-      <c r="C18" t="s">
-        <v>51</v>
-      </c>
       <c r="D18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E18" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F18">
         <v>34990</v>
@@ -1357,22 +1393,32 @@
         <f t="shared" ref="J18:J19" si="9">CONCATENATE("['",C18,",'",D18,"']")</f>
         <v>['SURPRISE BOX,'INGLÉS']</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="K18">
+        <v>1</v>
+      </c>
+      <c r="L18">
+        <v>1</v>
+      </c>
+      <c r="O18" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>surprisebox-en,Prismatic Evolutions,SURPRISE BOX,INGLÉS,SURPRISE BOX,34990,34990,10,img/surprisebox-en.webp,['SURPRISE BOX,'INGLÉS'],1,1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
+        <v>49</v>
+      </c>
+      <c r="B19" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19" t="s">
         <v>50</v>
       </c>
-      <c r="B19" t="s">
-        <v>22</v>
-      </c>
-      <c r="C19" t="s">
-        <v>51</v>
-      </c>
       <c r="D19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F19">
         <v>29990</v>
@@ -1391,61 +1437,191 @@
         <f t="shared" si="9"/>
         <v>['SURPRISE BOX,'ESPAÑOL']</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="K19">
+        <v>1</v>
+      </c>
+      <c r="L19">
+        <v>1</v>
+      </c>
+      <c r="O19" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>surprisebox-en,Prismatic Evolutions,SURPRISE BOX,ESPAÑOL,SURPRISE BOX,29990,29990,10,img/surprisebox-en.webp,['SURPRISE BOX,'ESPAÑOL'],1,1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
+        <v>52</v>
+      </c>
+      <c r="B20" t="s">
         <v>53</v>
       </c>
-      <c r="B20" t="s">
-        <v>54</v>
-      </c>
       <c r="C20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D20" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
+        <v>19</v>
+      </c>
+      <c r="E20" t="s">
+        <v>20</v>
+      </c>
+      <c r="F20">
+        <v>64990</v>
+      </c>
+      <c r="G20">
+        <v>29990</v>
+      </c>
+      <c r="H20">
+        <v>10</v>
+      </c>
+      <c r="I20" t="str">
+        <f t="shared" ref="I20:I23" si="10">CONCATENATE("img/",A20,".webp")</f>
+        <v>img/etb-megalucario-en.webp</v>
+      </c>
+      <c r="J20" t="str">
+        <f t="shared" ref="J20:J23" si="11">CONCATENATE("['",C20,",'",D20,"']")</f>
+        <v>['ETB,'INGLÉS']</v>
+      </c>
+      <c r="K20">
+        <v>1</v>
+      </c>
+      <c r="L20">
+        <v>1</v>
+      </c>
+      <c r="O20" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>etb-megalucario-en,Mega Evolutions,ETB,INGLÉS,ETB,64990,29990,10,img/etb-megalucario-en.webp,['ETB,'INGLÉS'],1,1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B21" t="s">
         <v>54</v>
       </c>
       <c r="C21" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D21" t="s">
+        <v>18</v>
+      </c>
+      <c r="E21" t="s">
+        <v>20</v>
+      </c>
+      <c r="F21">
+        <v>54990</v>
+      </c>
+      <c r="G21">
+        <v>29990</v>
+      </c>
+      <c r="H21">
+        <v>10</v>
+      </c>
+      <c r="I21" t="str">
+        <f t="shared" si="10"/>
+        <v>img/etb-megalucario-en.webp</v>
+      </c>
+      <c r="J21" t="str">
+        <f t="shared" si="11"/>
+        <v>['ETB,'ESPAÑOL']</v>
+      </c>
+      <c r="K21">
+        <v>1</v>
+      </c>
+      <c r="L21">
+        <v>1</v>
+      </c>
+      <c r="O21" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>etb-megalucario-en,Megaevolución,ETB,ESPAÑOL,ETB,54990,29990,10,img/etb-megalucario-en.webp,['ETB,'ESPAÑOL'],1,1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>51</v>
+      </c>
+      <c r="B22" t="s">
+        <v>53</v>
+      </c>
+      <c r="C22" t="s">
+        <v>20</v>
+      </c>
+      <c r="D22" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
-        <v>52</v>
-      </c>
-      <c r="B22" t="s">
-        <v>54</v>
-      </c>
-      <c r="C22" t="s">
-        <v>21</v>
-      </c>
-      <c r="D22" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="E22" t="s">
+        <v>20</v>
+      </c>
+      <c r="F22">
+        <v>64990</v>
+      </c>
+      <c r="G22">
+        <v>29990</v>
+      </c>
+      <c r="H22">
+        <v>10</v>
+      </c>
+      <c r="I22" t="str">
+        <f t="shared" si="10"/>
+        <v>img/etb-megagardevoir-en.webp</v>
+      </c>
+      <c r="J22" t="str">
+        <f t="shared" si="11"/>
+        <v>['ETB,'INGLÉS']</v>
+      </c>
+      <c r="K22">
+        <v>1</v>
+      </c>
+      <c r="L22">
+        <v>1</v>
+      </c>
+      <c r="O22" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>etb-megagardevoir-en,Mega Evolutions,ETB,INGLÉS,ETB,64990,29990,10,img/etb-megagardevoir-en.webp,['ETB,'INGLÉS'],1,1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B23" t="s">
         <v>54</v>
       </c>
       <c r="C23" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D23" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="E23" t="s">
+        <v>20</v>
+      </c>
+      <c r="F23">
+        <v>54990</v>
+      </c>
+      <c r="G23">
+        <v>29990</v>
+      </c>
+      <c r="H23">
+        <v>10</v>
+      </c>
+      <c r="I23" t="str">
+        <f t="shared" si="10"/>
+        <v>img/etb-megagardevoir-en.webp</v>
+      </c>
+      <c r="J23" t="str">
+        <f t="shared" si="11"/>
+        <v>['ETB,'ESPAÑOL']</v>
+      </c>
+      <c r="K23">
+        <v>1</v>
+      </c>
+      <c r="L23">
+        <v>1</v>
+      </c>
+      <c r="O23" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>etb-megagardevoir-en,Megaevolución,ETB,ESPAÑOL,ETB,54990,29990,10,img/etb-megagardevoir-en.webp,['ETB,'ESPAÑOL'],1,1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ActualizaciÃ³n completa (2025-09-21 17:57)
</commit_message>
<xml_diff>
--- a/BACKUP/SUPORT IMAGEN.xlsx
+++ b/BACKUP/SUPORT IMAGEN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jorgg\OneDrive\MasterHIT\BACKUP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A88C2211-A2C4-45B6-81EA-46935E73614A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C89FE8FA-AEF4-4DF1-9225-01E3E97AE094}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="57">
   <si>
     <t>id,name,set,type,category,price,compareAtPrice,stock,image,tags,source,createdAt</t>
   </si>
@@ -592,11 +592,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3CA635C-1DF7-4EEC-B0B8-3FA5C80D03DF}">
-  <dimension ref="A1:O23"/>
+  <dimension ref="A1:O24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -673,10 +671,10 @@
         <v>55</v>
       </c>
       <c r="F2">
-        <v>139990</v>
+        <v>140000</v>
       </c>
       <c r="G2">
-        <v>139990</v>
+        <v>179990</v>
       </c>
       <c r="H2">
         <v>10</v>
@@ -686,7 +684,7 @@
         <v>img/spc-prismatic-en.webp</v>
       </c>
       <c r="J2" t="str">
-        <f t="shared" ref="J2:J10" si="0">CONCATENATE("['",C2,",'",D2,"']")</f>
+        <f t="shared" ref="J2:J4" si="0">CONCATENATE("['",C2,",'",D2,"']")</f>
         <v>['SPC,'INGLÉS']</v>
       </c>
       <c r="K2">
@@ -697,86 +695,86 @@
       </c>
       <c r="O2" s="1" t="str">
         <f>CONCATENATE(A2,",",B2,",",C2,",",D2,",",E2,",",F2,",",G2,",",H2,",",I2,",",J2,",",K2,",",L2)</f>
-        <v>spc-prismatic-en,Prismatic Evolutions,SPC,INGLÉS,SPC,139990,139990,10,img/spc-prismatic-en.webp,['SPC,'INGLÉS'],1,1</v>
+        <v>spc-prismatic-en,Prismatic Evolutions,SPC,INGLÉS,SPC,140000,179990,10,img/spc-prismatic-en.webp,['SPC,'INGLÉS'],1,1</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>47</v>
       </c>
       <c r="B3" t="s">
-        <v>22</v>
+        <v>48</v>
       </c>
       <c r="C3" t="s">
-        <v>20</v>
+        <v>44</v>
       </c>
       <c r="D3" t="s">
         <v>18</v>
       </c>
       <c r="E3" t="s">
-        <v>20</v>
+        <v>44</v>
       </c>
       <c r="F3">
-        <v>49990</v>
+        <v>25000</v>
       </c>
       <c r="G3">
-        <v>69990</v>
+        <v>34990</v>
       </c>
       <c r="H3">
         <v>10</v>
       </c>
       <c r="I3" t="str">
-        <f t="shared" ref="I3:I9" si="1">CONCATENATE("img/",A3,".webp")</f>
-        <v>img/etb-prismatic-es.webp</v>
+        <f>CONCATENATE("img/",A3,".webp")</f>
+        <v>img/special-garchomp-en.webp</v>
       </c>
       <c r="J3" t="str">
+        <f>CONCATENATE("['",C3,",'",D3,"']")</f>
+        <v>['SPECIAL,'ESPAÑOL']</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3">
+        <v>1</v>
+      </c>
+      <c r="O3" s="1" t="str">
+        <f>CONCATENATE(A3,",",B3,",",C3,",",D3,",",E3,",",F3,",",G3,",",H3,",",I3,",",J3,",",K3,",",L3)</f>
+        <v>special-garchomp-en,Garchomp EX,SPECIAL,ESPAÑOL,SPECIAL,25000,34990,10,img/special-garchomp-en.webp,['SPECIAL,'ESPAÑOL'],1,1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4">
+        <v>40000</v>
+      </c>
+      <c r="G4">
+        <v>54990</v>
+      </c>
+      <c r="H4">
+        <v>10</v>
+      </c>
+      <c r="I4" t="str">
+        <f t="shared" ref="I4:I8" si="1">CONCATENATE("img/",A4,".webp")</f>
+        <v>img/etb-destined-es.webp</v>
+      </c>
+      <c r="J4" t="str">
         <f t="shared" si="0"/>
         <v>['ETB,'ESPAÑOL']</v>
       </c>
-      <c r="K3">
-        <v>1</v>
-      </c>
-      <c r="L3">
-        <v>1</v>
-      </c>
-      <c r="O3" s="1" t="str">
-        <f t="shared" ref="O3:O9" si="2">CONCATENATE(A3,",",B3,",",C3,",",D3,",",E3,",",F3,",",G3,",",H3,",",I3,",",J3,",",K3,",",L3)</f>
-        <v>etb-prismatic-es,Evoluciones Prismáticas,ETB,ESPAÑOL,ETB,49990,69990,10,img/etb-prismatic-es.webp,['ETB,'ESPAÑOL'],1,1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4">
-        <v>49990</v>
-      </c>
-      <c r="G4">
-        <v>67990</v>
-      </c>
-      <c r="H4">
-        <v>10</v>
-      </c>
-      <c r="I4" t="str">
-        <f t="shared" si="1"/>
-        <v>img/etb-white-flare-en.webp</v>
-      </c>
-      <c r="J4" t="str">
-        <f t="shared" si="0"/>
-        <v>['ETB,'INGLÉS']</v>
-      </c>
       <c r="K4">
         <v>1</v>
       </c>
@@ -784,42 +782,42 @@
         <v>1</v>
       </c>
       <c r="O4" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>etb-white-flare-en,White Flare,ETB,INGLÉS,ETB,49990,67990,10,img/etb-white-flare-en.webp,['ETB,'INGLÉS'],1,1</v>
+        <f t="shared" ref="O4:O16" si="2">CONCATENATE(A4,",",B4,",",C4,",",D4,",",E4,",",F4,",",G4,",",H4,",",I4,",",J4,",",K4,",",L4)</f>
+        <v>etb-destined-es,Rivales Predestinados,ETB,ESPAÑOL,ETB,40000,54990,10,img/etb-destined-es.webp,['ETB,'ESPAÑOL'],1,1</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>42</v>
       </c>
       <c r="B5" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
+        <v>44</v>
       </c>
       <c r="D5" t="s">
         <v>18</v>
       </c>
       <c r="E5" t="s">
-        <v>20</v>
+        <v>44</v>
       </c>
       <c r="F5">
-        <v>49990</v>
+        <v>25000</v>
       </c>
       <c r="G5">
-        <v>67990</v>
+        <v>34990</v>
       </c>
       <c r="H5">
         <v>10</v>
       </c>
       <c r="I5" t="str">
-        <f t="shared" si="1"/>
-        <v>img/etb-white-flare-en.webp</v>
+        <f>CONCATENATE("img/",A5,".webp")</f>
+        <v>img/special-charizardex-en.webp</v>
       </c>
       <c r="J5" t="str">
-        <f t="shared" si="0"/>
-        <v>['ETB,'ESPAÑOL']</v>
+        <f>CONCATENATE("['",C5,",'",D5,"']")</f>
+        <v>['SPECIAL,'ESPAÑOL']</v>
       </c>
       <c r="K5">
         <v>1</v>
@@ -828,42 +826,42 @@
         <v>1</v>
       </c>
       <c r="O5" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>etb-white-flare-en,Llama Blanca,ETB,ESPAÑOL,ETB,49990,67990,10,img/etb-white-flare-en.webp,['ETB,'ESPAÑOL'],1,1</v>
+        <f>CONCATENATE(A5,",",B5,",",C5,",",D5,",",E5,",",F5,",",G5,",",H5,",",I5,",",J5,",",K5,",",L5)</f>
+        <v>special-charizardex-en,Charizard EX,SPECIAL,ESPAÑOL,SPECIAL,25000,34990,10,img/special-charizardex-en.webp,['SPECIAL,'ESPAÑOL'],1,1</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C6" t="s">
         <v>20</v>
       </c>
       <c r="D6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E6" t="s">
         <v>20</v>
       </c>
       <c r="F6">
-        <v>49990</v>
+        <v>55000</v>
       </c>
       <c r="G6">
-        <v>54990</v>
+        <v>69990</v>
       </c>
       <c r="H6">
         <v>10</v>
       </c>
       <c r="I6" t="str">
-        <f t="shared" si="1"/>
-        <v>img/etb-black-bolt-en.webp</v>
+        <f t="shared" ref="I6" si="3">CONCATENATE("img/",A6,".webp")</f>
+        <v>img/etb-prismatic-es.webp</v>
       </c>
       <c r="J6" t="str">
-        <f t="shared" si="0"/>
-        <v>['ETB,'INGLÉS']</v>
+        <f>CONCATENATE("['",C6,",'",D6,"']")</f>
+        <v>['ETB,'ESPAÑOL']</v>
       </c>
       <c r="K6">
         <v>1</v>
@@ -872,42 +870,42 @@
         <v>1</v>
       </c>
       <c r="O6" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>etb-black-bolt-en,Black Bolt,ETB,INGLÉS,ETB,49990,54990,10,img/etb-black-bolt-en.webp,['ETB,'INGLÉS'],1,1</v>
+        <f t="shared" ref="O6" si="4">CONCATENATE(A6,",",B6,",",C6,",",D6,",",E6,",",F6,",",G6,",",H6,",",I6,",",J6,",",K6,",",L6)</f>
+        <v>etb-prismatic-es,Evoluciones Prismáticas,ETB,ESPAÑOL,ETB,55000,69990,10,img/etb-prismatic-es.webp,['ETB,'ESPAÑOL'],1,1</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>42</v>
       </c>
       <c r="B7" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="C7" t="s">
-        <v>20</v>
+        <v>44</v>
       </c>
       <c r="D7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E7" t="s">
-        <v>20</v>
+        <v>44</v>
       </c>
       <c r="F7">
-        <v>49990</v>
+        <v>28000</v>
       </c>
       <c r="G7">
-        <v>59990</v>
+        <v>34990</v>
       </c>
       <c r="H7">
         <v>10</v>
       </c>
       <c r="I7" t="str">
         <f t="shared" si="1"/>
-        <v>img/etb-black-bolt-es.webp</v>
+        <v>img/special-charizardex-en.webp</v>
       </c>
       <c r="J7" t="str">
-        <f t="shared" si="0"/>
-        <v>['ETB,'ESPAÑOL']</v>
+        <f t="shared" ref="J7:J8" si="5">CONCATENATE("['",C7,",'",D7,"']")</f>
+        <v>['SPECIAL,'INGLÉS']</v>
       </c>
       <c r="K7">
         <v>1</v>
@@ -917,41 +915,41 @@
       </c>
       <c r="O7" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>etb-black-bolt-es,Fulgor Negro,ETB,ESPAÑOL,ETB,49990,59990,10,img/etb-black-bolt-es.webp,['ETB,'ESPAÑOL'],1,1</v>
+        <v>special-charizardex-en,Charizard EX,SPECIAL,INGLÉS,SPECIAL,28000,34990,10,img/special-charizardex-en.webp,['SPECIAL,'INGLÉS'],1,1</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>45</v>
       </c>
       <c r="B8" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C8" t="s">
-        <v>20</v>
+        <v>46</v>
       </c>
       <c r="D8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E8" t="s">
-        <v>20</v>
+        <v>46</v>
       </c>
       <c r="F8">
-        <v>49990</v>
+        <v>18000</v>
       </c>
       <c r="G8">
-        <v>54990</v>
+        <v>19990</v>
       </c>
       <c r="H8">
         <v>10</v>
       </c>
       <c r="I8" t="str">
         <f t="shared" si="1"/>
-        <v>img/etb-aventuras-es.webp</v>
+        <v>img/poster-prismatic-en.webp</v>
       </c>
       <c r="J8" t="str">
-        <f t="shared" si="0"/>
-        <v>['ETB,'INGLÉS']</v>
+        <f t="shared" si="5"/>
+        <v>['POSTER,'ESPAÑOL']</v>
       </c>
       <c r="K8">
         <v>1</v>
@@ -961,41 +959,41 @@
       </c>
       <c r="O8" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>etb-aventuras-es,Journey Together,ETB,INGLÉS,ETB,49990,54990,10,img/etb-aventuras-es.webp,['ETB,'INGLÉS'],1,1</v>
+        <v>poster-prismatic-en,Prismatic Evolutions,POSTER,ESPAÑOL,POSTER,18000,19990,10,img/poster-prismatic-en.webp,['POSTER,'ESPAÑOL'],1,1</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
       <c r="B9" t="s">
-        <v>25</v>
+        <v>48</v>
       </c>
       <c r="C9" t="s">
-        <v>20</v>
+        <v>44</v>
       </c>
       <c r="D9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E9" t="s">
-        <v>20</v>
+        <v>44</v>
       </c>
       <c r="F9">
-        <v>49990</v>
+        <v>28000</v>
       </c>
       <c r="G9">
-        <v>54990</v>
+        <v>35990</v>
       </c>
       <c r="H9">
         <v>10</v>
       </c>
       <c r="I9" t="str">
-        <f t="shared" si="1"/>
-        <v>img/etb-aventuras-es.webp</v>
+        <f t="shared" ref="I9" si="6">CONCATENATE("img/",A9,".webp")</f>
+        <v>img/special-garchomp-en.webp</v>
       </c>
       <c r="J9" t="str">
-        <f t="shared" si="0"/>
-        <v>['ETB,'ESPAÑOL']</v>
+        <f t="shared" ref="J9:J10" si="7">CONCATENATE("['",C9,",'",D9,"']")</f>
+        <v>['SPECIAL,'INGLÉS']</v>
       </c>
       <c r="K9">
         <v>1</v>
@@ -1005,41 +1003,41 @@
       </c>
       <c r="O9" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>etb-aventuras-es,Aventuras Compartidas,ETB,ESPAÑOL,ETB,49990,54990,10,img/etb-aventuras-es.webp,['ETB,'ESPAÑOL'],1,1</v>
+        <v>special-garchomp-en,Garchomp EX,SPECIAL,INGLÉS,SPECIAL,28000,35990,10,img/special-garchomp-en.webp,['SPECIAL,'INGLÉS'],1,1</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>37</v>
+        <v>56</v>
       </c>
       <c r="B10" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="C10" t="s">
-        <v>20</v>
+        <v>55</v>
       </c>
       <c r="D10" t="s">
         <v>18</v>
       </c>
       <c r="E10" t="s">
-        <v>20</v>
+        <v>55</v>
       </c>
       <c r="F10">
-        <v>39990</v>
+        <v>120000</v>
       </c>
       <c r="G10">
-        <v>54990</v>
+        <v>179990</v>
       </c>
       <c r="H10">
         <v>10</v>
       </c>
       <c r="I10" t="str">
-        <f t="shared" ref="I10:I15" si="3">CONCATENATE("img/",A10,".webp")</f>
-        <v>img/etb-destined-es.webp</v>
+        <f>CONCATENATE("img/",A10,".webp")</f>
+        <v>img/spc-prismatic-en.webp</v>
       </c>
       <c r="J10" t="str">
-        <f t="shared" si="0"/>
-        <v>['ETB,'ESPAÑOL']</v>
+        <f t="shared" si="7"/>
+        <v>['SPC,'ESPAÑOL']</v>
       </c>
       <c r="K10">
         <v>1</v>
@@ -1048,42 +1046,42 @@
         <v>1</v>
       </c>
       <c r="O10" s="1" t="str">
-        <f t="shared" ref="O10:O23" si="4">CONCATENATE(A10,",",B10,",",C10,",",D10,",",E10,",",F10,",",G10,",",H10,",",I10,",",J10,",",K10,",",L10)</f>
-        <v>etb-destined-es,Rivales Predestinados,ETB,ESPAÑOL,ETB,39990,54990,10,img/etb-destined-es.webp,['ETB,'ESPAÑOL'],1,1</v>
+        <f>CONCATENATE(A10,",",B10,",",C10,",",D10,",",E10,",",F10,",",G10,",",H10,",",I10,",",J10,",",K10,",",L10)</f>
+        <v>spc-prismatic-en,Evoluciones Prismáticas,SPC,ESPAÑOL,SPC,120000,179990,10,img/spc-prismatic-en.webp,['SPC,'ESPAÑOL'],1,1</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="B11" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C11" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="D11" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E11" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="F11">
-        <v>34990</v>
+        <v>35000</v>
       </c>
       <c r="G11">
-        <v>34990</v>
+        <v>39990</v>
       </c>
       <c r="H11">
         <v>10</v>
       </c>
       <c r="I11" t="str">
-        <f t="shared" si="3"/>
-        <v>img/bin-white-flare-es.webp</v>
+        <f t="shared" ref="I11:I12" si="8">CONCATENATE("img/",A11,".webp")</f>
+        <v>img/surprisebox-en.webp</v>
       </c>
       <c r="J11" t="str">
-        <f>CONCATENATE("['",C11,",'",D11,"']")</f>
-        <v>['BINDER,'ESPAÑOL']</v>
+        <f t="shared" ref="J11:J12" si="9">CONCATENATE("['",C11,",'",D11,"']")</f>
+        <v>['SURPRISE BOX,'INGLÉS']</v>
       </c>
       <c r="K11">
         <v>1</v>
@@ -1092,28 +1090,28 @@
         <v>1</v>
       </c>
       <c r="O11" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>bin-white-flare-es,Llama Blanca,BINDER,ESPAÑOL,BINDER,34990,34990,10,img/bin-white-flare-es.webp,['BINDER,'ESPAÑOL'],1,1</v>
+        <f t="shared" si="2"/>
+        <v>surprisebox-en,Prismatic Evolutions,SURPRISE BOX,INGLÉS,SURPRISE BOX,35000,39990,10,img/surprisebox-en.webp,['SURPRISE BOX,'INGLÉS'],1,1</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="B12" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="C12" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="D12" t="s">
         <v>18</v>
       </c>
       <c r="E12" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="F12">
-        <v>34990</v>
+        <v>30000</v>
       </c>
       <c r="G12">
         <v>34990</v>
@@ -1122,12 +1120,12 @@
         <v>10</v>
       </c>
       <c r="I12" t="str">
-        <f t="shared" si="3"/>
-        <v>img/bin-black-bolt-es.webp</v>
+        <f t="shared" si="8"/>
+        <v>img/surprisebox-en.webp</v>
       </c>
       <c r="J12" t="str">
-        <f t="shared" ref="J12:J15" si="5">CONCATENATE("['",C12,",'",D12,"']")</f>
-        <v>['BINDER,'ESPAÑOL']</v>
+        <f t="shared" si="9"/>
+        <v>['SURPRISE BOX,'ESPAÑOL']</v>
       </c>
       <c r="K12">
         <v>1</v>
@@ -1136,28 +1134,28 @@
         <v>1</v>
       </c>
       <c r="O12" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>bin-black-bolt-es,Fulgor Negro,BINDER,ESPAÑOL,BINDER,34990,34990,10,img/bin-black-bolt-es.webp,['BINDER,'ESPAÑOL'],1,1</v>
+        <f t="shared" si="2"/>
+        <v>surprisebox-en,Prismatic Evolutions,SURPRISE BOX,ESPAÑOL,SURPRISE BOX,30000,34990,10,img/surprisebox-en.webp,['SURPRISE BOX,'ESPAÑOL'],1,1</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="B13" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="C13" t="s">
-        <v>44</v>
+        <v>20</v>
       </c>
       <c r="D13" t="s">
         <v>19</v>
       </c>
       <c r="E13" t="s">
-        <v>44</v>
+        <v>20</v>
       </c>
       <c r="F13">
-        <v>29990</v>
+        <v>64990</v>
       </c>
       <c r="G13">
         <v>29990</v>
@@ -1166,12 +1164,12 @@
         <v>10</v>
       </c>
       <c r="I13" t="str">
-        <f t="shared" si="3"/>
-        <v>img/special-charizardex-en.webp</v>
+        <f t="shared" ref="I13:I16" si="10">CONCATENATE("img/",A13,".webp")</f>
+        <v>img/etb-megalucario-en.webp</v>
       </c>
       <c r="J13" t="str">
-        <f t="shared" si="5"/>
-        <v>['SPECIAL,'INGLÉS']</v>
+        <f t="shared" ref="J13:J16" si="11">CONCATENATE("['",C13,",'",D13,"']")</f>
+        <v>['ETB,'INGLÉS']</v>
       </c>
       <c r="K13">
         <v>1</v>
@@ -1180,28 +1178,28 @@
         <v>1</v>
       </c>
       <c r="O13" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>special-charizardex-en,Charizard EX,SPECIAL,INGLÉS,SPECIAL,29990,29990,10,img/special-charizardex-en.webp,['SPECIAL,'INGLÉS'],1,1</v>
+        <f t="shared" si="2"/>
+        <v>etb-megalucario-en,Mega Evolutions,ETB,INGLÉS,ETB,64990,29990,10,img/etb-megalucario-en.webp,['ETB,'INGLÉS'],1,1</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="B14" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="C14" t="s">
-        <v>44</v>
+        <v>20</v>
       </c>
       <c r="D14" t="s">
         <v>18</v>
       </c>
       <c r="E14" t="s">
-        <v>44</v>
+        <v>20</v>
       </c>
       <c r="F14">
-        <v>29990</v>
+        <v>54990</v>
       </c>
       <c r="G14">
         <v>29990</v>
@@ -1210,12 +1208,12 @@
         <v>10</v>
       </c>
       <c r="I14" t="str">
-        <f t="shared" si="3"/>
-        <v>img/special-charizardex-en.webp</v>
+        <f t="shared" si="10"/>
+        <v>img/etb-megalucario-en.webp</v>
       </c>
       <c r="J14" t="str">
-        <f t="shared" si="5"/>
-        <v>['SPECIAL,'ESPAÑOL']</v>
+        <f t="shared" si="11"/>
+        <v>['ETB,'ESPAÑOL']</v>
       </c>
       <c r="K14">
         <v>1</v>
@@ -1224,42 +1222,42 @@
         <v>1</v>
       </c>
       <c r="O14" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>special-charizardex-en,Charizard EX,SPECIAL,ESPAÑOL,SPECIAL,29990,29990,10,img/special-charizardex-en.webp,['SPECIAL,'ESPAÑOL'],1,1</v>
+        <f t="shared" si="2"/>
+        <v>etb-megalucario-en,Megaevolución,ETB,ESPAÑOL,ETB,54990,29990,10,img/etb-megalucario-en.webp,['ETB,'ESPAÑOL'],1,1</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="B15" t="s">
-        <v>21</v>
+        <v>53</v>
       </c>
       <c r="C15" t="s">
-        <v>46</v>
+        <v>20</v>
       </c>
       <c r="D15" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E15" t="s">
-        <v>46</v>
+        <v>20</v>
       </c>
       <c r="F15">
-        <v>19990</v>
+        <v>64990</v>
       </c>
       <c r="G15">
-        <v>19990</v>
+        <v>29990</v>
       </c>
       <c r="H15">
         <v>10</v>
       </c>
       <c r="I15" t="str">
-        <f t="shared" si="3"/>
-        <v>img/poster-prismatic-en.webp</v>
+        <f t="shared" si="10"/>
+        <v>img/etb-megagardevoir-en.webp</v>
       </c>
       <c r="J15" t="str">
-        <f t="shared" si="5"/>
-        <v>['POSTER,'ESPAÑOL']</v>
+        <f t="shared" si="11"/>
+        <v>['ETB,'INGLÉS']</v>
       </c>
       <c r="K15">
         <v>1</v>
@@ -1268,28 +1266,28 @@
         <v>1</v>
       </c>
       <c r="O15" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>poster-prismatic-en,Prismatic Evolutions,POSTER,ESPAÑOL,POSTER,19990,19990,10,img/poster-prismatic-en.webp,['POSTER,'ESPAÑOL'],1,1</v>
+        <f t="shared" si="2"/>
+        <v>etb-megagardevoir-en,Mega Evolutions,ETB,INGLÉS,ETB,64990,29990,10,img/etb-megagardevoir-en.webp,['ETB,'INGLÉS'],1,1</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="B16" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="C16" t="s">
-        <v>44</v>
+        <v>20</v>
       </c>
       <c r="D16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E16" t="s">
-        <v>44</v>
+        <v>20</v>
       </c>
       <c r="F16">
-        <v>29990</v>
+        <v>54990</v>
       </c>
       <c r="G16">
         <v>29990</v>
@@ -1298,12 +1296,12 @@
         <v>10</v>
       </c>
       <c r="I16" t="str">
-        <f t="shared" ref="I16:I17" si="6">CONCATENATE("img/",A16,".webp")</f>
-        <v>img/special-garchomp-en.webp</v>
+        <f t="shared" si="10"/>
+        <v>img/etb-megagardevoir-en.webp</v>
       </c>
       <c r="J16" t="str">
-        <f t="shared" ref="J16:J17" si="7">CONCATENATE("['",C16,",'",D16,"']")</f>
-        <v>['SPECIAL,'INGLÉS']</v>
+        <f t="shared" si="11"/>
+        <v>['ETB,'ESPAÑOL']</v>
       </c>
       <c r="K16">
         <v>1</v>
@@ -1312,42 +1310,42 @@
         <v>1</v>
       </c>
       <c r="O16" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>special-garchomp-en,Garchomp EX,SPECIAL,INGLÉS,SPECIAL,29990,29990,10,img/special-garchomp-en.webp,['SPECIAL,'INGLÉS'],1,1</v>
+        <f t="shared" si="2"/>
+        <v>etb-megagardevoir-en,Megaevolución,ETB,ESPAÑOL,ETB,54990,29990,10,img/etb-megagardevoir-en.webp,['ETB,'ESPAÑOL'],1,1</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>47</v>
+        <v>14</v>
       </c>
       <c r="B17" t="s">
-        <v>48</v>
+        <v>23</v>
       </c>
       <c r="C17" t="s">
-        <v>44</v>
+        <v>20</v>
       </c>
       <c r="D17" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E17" t="s">
-        <v>44</v>
+        <v>20</v>
       </c>
       <c r="F17">
-        <v>29990</v>
+        <v>74990</v>
       </c>
       <c r="G17">
-        <v>29990</v>
+        <v>79990</v>
       </c>
       <c r="H17">
         <v>10</v>
       </c>
       <c r="I17" t="str">
-        <f t="shared" si="6"/>
-        <v>img/special-garchomp-en.webp</v>
+        <f>CONCATENATE("img/",A17,".webp")</f>
+        <v>img/etb-white-flare-en.webp</v>
       </c>
       <c r="J17" t="str">
-        <f t="shared" si="7"/>
-        <v>['SPECIAL,'ESPAÑOL']</v>
+        <f>CONCATENATE("['",C17,",'",D17,"']")</f>
+        <v>['ETB,'INGLÉS']</v>
       </c>
       <c r="K17">
         <v>1</v>
@@ -1356,42 +1354,42 @@
         <v>1</v>
       </c>
       <c r="O17" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>special-garchomp-en,Garchomp EX,SPECIAL,ESPAÑOL,SPECIAL,29990,29990,10,img/special-garchomp-en.webp,['SPECIAL,'ESPAÑOL'],1,1</v>
+        <f>CONCATENATE(A17,",",B17,",",C17,",",D17,",",E17,",",F17,",",G17,",",H17,",",I17,",",J17,",",K17,",",L17)</f>
+        <v>etb-white-flare-en,White Flare,ETB,INGLÉS,ETB,74990,79990,10,img/etb-white-flare-en.webp,['ETB,'INGLÉS'],1,1</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>49</v>
+        <v>14</v>
       </c>
       <c r="B18" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="C18" t="s">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="D18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E18" t="s">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="F18">
-        <v>34990</v>
+        <v>69990</v>
       </c>
       <c r="G18">
-        <v>34990</v>
+        <v>79990</v>
       </c>
       <c r="H18">
         <v>10</v>
       </c>
       <c r="I18" t="str">
-        <f t="shared" ref="I18:I19" si="8">CONCATENATE("img/",A18,".webp")</f>
-        <v>img/surprisebox-en.webp</v>
+        <f>CONCATENATE("img/",A18,".webp")</f>
+        <v>img/etb-white-flare-en.webp</v>
       </c>
       <c r="J18" t="str">
-        <f t="shared" ref="J18:J19" si="9">CONCATENATE("['",C18,",'",D18,"']")</f>
-        <v>['SURPRISE BOX,'INGLÉS']</v>
+        <f>CONCATENATE("['",C18,",'",D18,"']")</f>
+        <v>['ETB,'ESPAÑOL']</v>
       </c>
       <c r="K18">
         <v>1</v>
@@ -1400,42 +1398,42 @@
         <v>1</v>
       </c>
       <c r="O18" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>surprisebox-en,Prismatic Evolutions,SURPRISE BOX,INGLÉS,SURPRISE BOX,34990,34990,10,img/surprisebox-en.webp,['SURPRISE BOX,'INGLÉS'],1,1</v>
+        <f>CONCATENATE(A18,",",B18,",",C18,",",D18,",",E18,",",F18,",",G18,",",H18,",",I18,",",J18,",",K18,",",L18)</f>
+        <v>etb-white-flare-en,Llama Blanca,ETB,ESPAÑOL,ETB,69990,79990,10,img/etb-white-flare-en.webp,['ETB,'ESPAÑOL'],1,1</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>49</v>
+        <v>15</v>
       </c>
       <c r="B19" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C19" t="s">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="D19" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E19" t="s">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="F19">
-        <v>29990</v>
+        <v>74990</v>
       </c>
       <c r="G19">
-        <v>29990</v>
+        <v>79990</v>
       </c>
       <c r="H19">
         <v>10</v>
       </c>
       <c r="I19" t="str">
-        <f t="shared" si="8"/>
-        <v>img/surprisebox-en.webp</v>
+        <f>CONCATENATE("img/",A19,".webp")</f>
+        <v>img/etb-black-bolt-en.webp</v>
       </c>
       <c r="J19" t="str">
-        <f t="shared" si="9"/>
-        <v>['SURPRISE BOX,'ESPAÑOL']</v>
+        <f>CONCATENATE("['",C19,",'",D19,"']")</f>
+        <v>['ETB,'INGLÉS']</v>
       </c>
       <c r="K19">
         <v>1</v>
@@ -1444,42 +1442,42 @@
         <v>1</v>
       </c>
       <c r="O19" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>surprisebox-en,Prismatic Evolutions,SURPRISE BOX,ESPAÑOL,SURPRISE BOX,29990,29990,10,img/surprisebox-en.webp,['SURPRISE BOX,'ESPAÑOL'],1,1</v>
+        <f>CONCATENATE(A19,",",B19,",",C19,",",D19,",",E19,",",F19,",",G19,",",H19,",",I19,",",J19,",",K19,",",L19)</f>
+        <v>etb-black-bolt-en,Black Bolt,ETB,INGLÉS,ETB,74990,79990,10,img/etb-black-bolt-en.webp,['ETB,'INGLÉS'],1,1</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>52</v>
+        <v>16</v>
       </c>
       <c r="B20" t="s">
-        <v>53</v>
+        <v>28</v>
       </c>
       <c r="C20" t="s">
         <v>20</v>
       </c>
       <c r="D20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E20" t="s">
         <v>20</v>
       </c>
       <c r="F20">
-        <v>64990</v>
+        <v>69990</v>
       </c>
       <c r="G20">
-        <v>29990</v>
+        <v>79990</v>
       </c>
       <c r="H20">
         <v>10</v>
       </c>
       <c r="I20" t="str">
-        <f t="shared" ref="I20:I23" si="10">CONCATENATE("img/",A20,".webp")</f>
-        <v>img/etb-megalucario-en.webp</v>
+        <f>CONCATENATE("img/",A20,".webp")</f>
+        <v>img/etb-black-bolt-es.webp</v>
       </c>
       <c r="J20" t="str">
-        <f t="shared" ref="J20:J23" si="11">CONCATENATE("['",C20,",'",D20,"']")</f>
-        <v>['ETB,'INGLÉS']</v>
+        <f>CONCATENATE("['",C20,",'",D20,"']")</f>
+        <v>['ETB,'ESPAÑOL']</v>
       </c>
       <c r="K20">
         <v>1</v>
@@ -1488,42 +1486,42 @@
         <v>1</v>
       </c>
       <c r="O20" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>etb-megalucario-en,Mega Evolutions,ETB,INGLÉS,ETB,64990,29990,10,img/etb-megalucario-en.webp,['ETB,'INGLÉS'],1,1</v>
+        <f>CONCATENATE(A20,",",B20,",",C20,",",D20,",",E20,",",F20,",",G20,",",H20,",",I20,",",J20,",",K20,",",L20)</f>
+        <v>etb-black-bolt-es,Fulgor Negro,ETB,ESPAÑOL,ETB,69990,79990,10,img/etb-black-bolt-es.webp,['ETB,'ESPAÑOL'],1,1</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>52</v>
+        <v>17</v>
       </c>
       <c r="B21" t="s">
-        <v>54</v>
+        <v>27</v>
       </c>
       <c r="C21" t="s">
         <v>20</v>
       </c>
       <c r="D21" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E21" t="s">
         <v>20</v>
       </c>
       <c r="F21">
-        <v>54990</v>
+        <v>74990</v>
       </c>
       <c r="G21">
-        <v>29990</v>
+        <v>79990</v>
       </c>
       <c r="H21">
         <v>10</v>
       </c>
       <c r="I21" t="str">
-        <f t="shared" si="10"/>
-        <v>img/etb-megalucario-en.webp</v>
+        <f>CONCATENATE("img/",A21,".webp")</f>
+        <v>img/etb-aventuras-es.webp</v>
       </c>
       <c r="J21" t="str">
-        <f t="shared" si="11"/>
-        <v>['ETB,'ESPAÑOL']</v>
+        <f>CONCATENATE("['",C21,",'",D21,"']")</f>
+        <v>['ETB,'INGLÉS']</v>
       </c>
       <c r="K21">
         <v>1</v>
@@ -1532,42 +1530,42 @@
         <v>1</v>
       </c>
       <c r="O21" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>etb-megalucario-en,Megaevolución,ETB,ESPAÑOL,ETB,54990,29990,10,img/etb-megalucario-en.webp,['ETB,'ESPAÑOL'],1,1</v>
+        <f>CONCATENATE(A21,",",B21,",",C21,",",D21,",",E21,",",F21,",",G21,",",H21,",",I21,",",J21,",",K21,",",L21)</f>
+        <v>etb-aventuras-es,Journey Together,ETB,INGLÉS,ETB,74990,79990,10,img/etb-aventuras-es.webp,['ETB,'INGLÉS'],1,1</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>51</v>
+        <v>17</v>
       </c>
       <c r="B22" t="s">
-        <v>53</v>
+        <v>25</v>
       </c>
       <c r="C22" t="s">
         <v>20</v>
       </c>
       <c r="D22" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E22" t="s">
         <v>20</v>
       </c>
       <c r="F22">
-        <v>64990</v>
+        <v>69990</v>
       </c>
       <c r="G22">
-        <v>29990</v>
+        <v>79990</v>
       </c>
       <c r="H22">
         <v>10</v>
       </c>
       <c r="I22" t="str">
-        <f t="shared" si="10"/>
-        <v>img/etb-megagardevoir-en.webp</v>
+        <f>CONCATENATE("img/",A22,".webp")</f>
+        <v>img/etb-aventuras-es.webp</v>
       </c>
       <c r="J22" t="str">
-        <f t="shared" si="11"/>
-        <v>['ETB,'INGLÉS']</v>
+        <f>CONCATENATE("['",C22,",'",D22,"']")</f>
+        <v>['ETB,'ESPAÑOL']</v>
       </c>
       <c r="K22">
         <v>1</v>
@@ -1576,42 +1574,42 @@
         <v>1</v>
       </c>
       <c r="O22" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>etb-megagardevoir-en,Mega Evolutions,ETB,INGLÉS,ETB,64990,29990,10,img/etb-megagardevoir-en.webp,['ETB,'INGLÉS'],1,1</v>
+        <f>CONCATENATE(A22,",",B22,",",C22,",",D22,",",E22,",",F22,",",G22,",",H22,",",I22,",",J22,",",K22,",",L22)</f>
+        <v>etb-aventuras-es,Aventuras Compartidas,ETB,ESPAÑOL,ETB,69990,79990,10,img/etb-aventuras-es.webp,['ETB,'ESPAÑOL'],1,1</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="B23" t="s">
-        <v>54</v>
+        <v>26</v>
       </c>
       <c r="C23" t="s">
-        <v>20</v>
+        <v>41</v>
       </c>
       <c r="D23" t="s">
         <v>18</v>
       </c>
       <c r="E23" t="s">
-        <v>20</v>
+        <v>41</v>
       </c>
       <c r="F23">
-        <v>54990</v>
+        <v>34990</v>
       </c>
       <c r="G23">
-        <v>29990</v>
+        <v>34990</v>
       </c>
       <c r="H23">
         <v>10</v>
       </c>
       <c r="I23" t="str">
-        <f t="shared" si="10"/>
-        <v>img/etb-megagardevoir-en.webp</v>
+        <f>CONCATENATE("img/",A23,".webp")</f>
+        <v>img/bin-white-flare-es.webp</v>
       </c>
       <c r="J23" t="str">
-        <f t="shared" si="11"/>
-        <v>['ETB,'ESPAÑOL']</v>
+        <f>CONCATENATE("['",C23,",'",D23,"']")</f>
+        <v>['BINDER,'ESPAÑOL']</v>
       </c>
       <c r="K23">
         <v>1</v>
@@ -1620,8 +1618,52 @@
         <v>1</v>
       </c>
       <c r="O23" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>etb-megagardevoir-en,Megaevolución,ETB,ESPAÑOL,ETB,54990,29990,10,img/etb-megagardevoir-en.webp,['ETB,'ESPAÑOL'],1,1</v>
+        <f>CONCATENATE(A23,",",B23,",",C23,",",D23,",",E23,",",F23,",",G23,",",H23,",",I23,",",J23,",",K23,",",L23)</f>
+        <v>bin-white-flare-es,Llama Blanca,BINDER,ESPAÑOL,BINDER,34990,34990,10,img/bin-white-flare-es.webp,['BINDER,'ESPAÑOL'],1,1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>40</v>
+      </c>
+      <c r="B24" t="s">
+        <v>28</v>
+      </c>
+      <c r="C24" t="s">
+        <v>41</v>
+      </c>
+      <c r="D24" t="s">
+        <v>18</v>
+      </c>
+      <c r="E24" t="s">
+        <v>41</v>
+      </c>
+      <c r="F24">
+        <v>34990</v>
+      </c>
+      <c r="G24">
+        <v>34990</v>
+      </c>
+      <c r="H24">
+        <v>10</v>
+      </c>
+      <c r="I24" t="str">
+        <f>CONCATENATE("img/",A24,".webp")</f>
+        <v>img/bin-black-bolt-es.webp</v>
+      </c>
+      <c r="J24" t="str">
+        <f>CONCATENATE("['",C24,",'",D24,"']")</f>
+        <v>['BINDER,'ESPAÑOL']</v>
+      </c>
+      <c r="K24">
+        <v>1</v>
+      </c>
+      <c r="L24">
+        <v>1</v>
+      </c>
+      <c r="O24" s="1" t="str">
+        <f>CONCATENATE(A24,",",B24,",",C24,",",D24,",",E24,",",F24,",",G24,",",H24,",",I24,",",J24,",",K24,",",L24)</f>
+        <v>bin-black-bolt-es,Fulgor Negro,BINDER,ESPAÑOL,BINDER,34990,34990,10,img/bin-black-bolt-es.webp,['BINDER,'ESPAÑOL'],1,1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ActualizaciÃ³n completa (2025-09-21 22:31)
</commit_message>
<xml_diff>
--- a/BACKUP/SUPORT IMAGEN.xlsx
+++ b/BACKUP/SUPORT IMAGEN.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jorgg\OneDrive\MasterHIT\BACKUP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C89FE8FA-AEF4-4DF1-9225-01E3E97AE094}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1937DB8D-50E5-4194-9FD5-E5E4DEBD9379}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="78">
   <si>
     <t>id,name,set,type,category,price,compareAtPrice,stock,image,tags,source,createdAt</t>
   </si>
@@ -126,30 +126,6 @@
     <t>Fulgor Negro</t>
   </si>
   <si>
-    <t>etb-prismatic-en,Prismatic Evolutions,ETB,INGLÉS,ETB,49990,69990,10,img/etb-prismatic-en.webp,['ETB', 'ES'],https://collectorcenter.cl/collections/ver-todo-pokemon,1757735865443</t>
-  </si>
-  <si>
-    <t>etb-prismatic-es,Evoluciones Prismáticas,ETB,ESPAÑOL,ETB,49990,69990,10,img/etb-prismatic-es.webp,['ETB', 'ES'],https://collectorcenter.cl/collections/ver-todo-pokemon,1757735865443</t>
-  </si>
-  <si>
-    <t>etb-white-flare-en,White Flare,ETB,INGLÉS,ETB,49990,67990,10,img/etb-white-flare-en.webp,['ETB', 'EN'],https://collectorcenter.cl/collections/ver-todo-pokemon,1757649465443</t>
-  </si>
-  <si>
-    <t>etb-white-flare-en,Llama Blanca,ETB,ESPAÑOL,ETB,49990,67990,10,img/etb-white-flare-en.webp,['ETB', 'EN'],https://collectorcenter.cl/collections/ver-todo-pokemon,1757563065443</t>
-  </si>
-  <si>
-    <t>etb-black-bolt-en,Black Bolt,ETB,INGLÉS,ETB,49990,54990,10,img/etb-black-bolt-en.webp,['ETB', 'ES'],https://collectorcenter.cl/collections/ver-todo-pokemon,1757390265443</t>
-  </si>
-  <si>
-    <t>etb-black-bolt-es,Fulgor Negro,ETB,ESPAÑOL,ETB,49990,59990,10,img/etb-black-bolt-es.webp,['ETB', 'ES'],https://collectorcenter.cl/collections/ver-todo-pokemon,1757044665443</t>
-  </si>
-  <si>
-    <t>etb-aventuras-es,Aventuras Compartidas,ETB,ESPAÑOL,ETB,49990,54990,10,img/etb-aventuras-es.webp,['ETB', 'ES'],https://collectorcenter.cl/collections/ver-todo-pokemon,1756958265443</t>
-  </si>
-  <si>
-    <t>etb-aventuras-es,Journey Together,ETB,INGLÉS,ETB,49990,54990,10,img/etb-aventuras-es.webp,['ETB', 'ES'],https://collectorcenter.cl/collections/ver-todo-pokemon,1756958265443</t>
-  </si>
-  <si>
     <t>etb-destined-es</t>
   </si>
   <si>
@@ -208,16 +184,109 @@
   </si>
   <si>
     <t>spc-prismatic-en</t>
+  </si>
+  <si>
+    <t>Oferta Flash</t>
+  </si>
+  <si>
+    <t>Preventa 26/09</t>
+  </si>
+  <si>
+    <t>Preventa 26/10</t>
+  </si>
+  <si>
+    <t>Preventa 26/11</t>
+  </si>
+  <si>
+    <t>Preventa 26/12</t>
+  </si>
+  <si>
+    <t>Últimas Unidades</t>
+  </si>
+  <si>
+    <t>spc-prismatic-en,Prismatic Evolutions,SPC,INGLÉS,SPC,140000,179990,10,img/spc-prismatic-en.webp,['SPC,'INGLÉS'],Oferta Flash,</t>
+  </si>
+  <si>
+    <t>special-garchomp-en,Garchomp EX,SPECIAL,ESPAÑOL,SPECIAL,25000,34990,5,img/special-garchomp-en.webp,['SPECIAL,'ESPAÑOL'],Oferta Flash,</t>
+  </si>
+  <si>
+    <t>etb-destined-es,Rivales Predestinados,ETB,ESPAÑOL,ETB,40000,54990,10,img/etb-destined-es.webp,['ETB,'ESPAÑOL'],Oferta Flash,</t>
+  </si>
+  <si>
+    <t>special-charizardex-en,Charizard EX,SPECIAL,ESPAÑOL,SPECIAL,25000,34990,5,img/special-charizardex-en.webp,['SPECIAL,'ESPAÑOL'],Oferta Flash,</t>
+  </si>
+  <si>
+    <t>etb-prismatic-es,Evoluciones Prismáticas,ETB,ESPAÑOL,ETB,55000,69990,2,img/etb-prismatic-es.webp,['ETB,'ESPAÑOL'],Últimas Unidades,</t>
+  </si>
+  <si>
+    <t>special-charizardex-en,Charizard EX,SPECIAL,INGLÉS,SPECIAL,28000,34990,5,img/special-charizardex-en.webp,['SPECIAL,'INGLÉS'],Últimas Unidades,</t>
+  </si>
+  <si>
+    <t>poster-prismatic-en,Prismatic Evolutions,POSTER,ESPAÑOL,POSTER,18000,19990,2,img/poster-prismatic-en.webp,['POSTER,'ESPAÑOL'],Últimas Unidades,</t>
+  </si>
+  <si>
+    <t>special-garchomp-en,Garchomp EX,SPECIAL,INGLÉS,SPECIAL,28000,35990,5,img/special-garchomp-en.webp,['SPECIAL,'INGLÉS'],Últimas Unidades,</t>
+  </si>
+  <si>
+    <t>spc-prismatic-en,Evoluciones Prismáticas,SPC,ESPAÑOL,SPC,120000,179990,2,img/spc-prismatic-en.webp,['SPC,'ESPAÑOL'],Últimas Unidades,</t>
+  </si>
+  <si>
+    <t>surprisebox-en,Prismatic Evolutions,SURPRISE BOX,INGLÉS,SURPRISE BOX,35000,39990,2,img/surprisebox-en.webp,['SURPRISE BOX,'INGLÉS'],Últimas Unidades,</t>
+  </si>
+  <si>
+    <t>surprisebox-en,Prismatic Evolutions,SURPRISE BOX,ESPAÑOL,SURPRISE BOX,30000,34990,2,img/surprisebox-en.webp,['SURPRISE BOX,'ESPAÑOL'],Últimas Unidades,</t>
+  </si>
+  <si>
+    <t>etb-megalucario-en,Mega Evolutions,ETB,INGLÉS,ETB,64990,29990,10,img/etb-megalucario-en.webp,['ETB,'INGLÉS'],Preventa 26/09,</t>
+  </si>
+  <si>
+    <t>etb-megalucario-en,Megaevolución,ETB,ESPAÑOL,ETB,54990,29990,10,img/etb-megalucario-en.webp,['ETB,'ESPAÑOL'],Preventa 26/10,</t>
+  </si>
+  <si>
+    <t>etb-megagardevoir-en,Mega Evolutions,ETB,INGLÉS,ETB,64990,29990,10,img/etb-megagardevoir-en.webp,['ETB,'INGLÉS'],Preventa 26/11,</t>
+  </si>
+  <si>
+    <t>etb-megagardevoir-en,Megaevolución,ETB,ESPAÑOL,ETB,54990,29990,10,img/etb-megagardevoir-en.webp,['ETB,'ESPAÑOL'],Preventa 26/12,</t>
+  </si>
+  <si>
+    <t>etb-white-flare-en,White Flare,ETB,INGLÉS,ETB,74990,79990,2,img/etb-white-flare-en.webp,['ETB,'INGLÉS'],Últimas Unidades,</t>
+  </si>
+  <si>
+    <t>etb-white-flare-en,Llama Blanca,ETB,ESPAÑOL,ETB,69990,79990,2,img/etb-white-flare-en.webp,['ETB,'ESPAÑOL'],Últimas Unidades,</t>
+  </si>
+  <si>
+    <t>etb-black-bolt-en,Black Bolt,ETB,INGLÉS,ETB,74990,79990,2,img/etb-black-bolt-en.webp,['ETB,'INGLÉS'],Últimas Unidades,</t>
+  </si>
+  <si>
+    <t>etb-black-bolt-es,Fulgor Negro,ETB,ESPAÑOL,ETB,69990,79990,2,img/etb-black-bolt-es.webp,['ETB,'ESPAÑOL'],Últimas Unidades,</t>
+  </si>
+  <si>
+    <t>etb-aventuras-es,Journey Together,ETB,INGLÉS,ETB,74990,79990,2,img/etb-aventuras-es.webp,['ETB,'INGLÉS'],Últimas Unidades,</t>
+  </si>
+  <si>
+    <t>etb-aventuras-es,Aventuras Compartidas,ETB,ESPAÑOL,ETB,69990,79990,2,img/etb-aventuras-es.webp,['ETB,'ESPAÑOL'],Últimas Unidades,</t>
+  </si>
+  <si>
+    <t>bin-white-flare-es,Llama Blanca,BINDER,ESPAÑOL,BINDER,34990,34990,2,img/bin-white-flare-es.webp,['BINDER,'ESPAÑOL'],Últimas Unidades,</t>
+  </si>
+  <si>
+    <t>bin-black-bolt-es,Fulgor Negro,BINDER,ESPAÑOL,BINDER,34990,34990,2,img/bin-black-bolt-es.webp,['BINDER,'ESPAÑOL'],Últimas Unidades,</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -532,10 +601,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A9"/>
+  <dimension ref="A1:A24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -547,42 +616,117 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>30</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>31</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>32</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>33</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>36</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>35</v>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -594,7 +738,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3CA635C-1DF7-4EEC-B0B8-3FA5C80D03DF}">
   <dimension ref="A1:O24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O1" sqref="O1:O24"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -608,7 +754,7 @@
     <col min="8" max="8" width="5.08984375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="28.7265625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="23.36328125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.36328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.7265625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="8.90625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="105.6328125" bestFit="1" customWidth="1"/>
   </cols>
@@ -656,19 +802,19 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="B2" t="s">
         <v>21</v>
       </c>
       <c r="C2" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="D2" t="s">
         <v>19</v>
       </c>
       <c r="E2" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="F2">
         <v>140000</v>
@@ -687,32 +833,29 @@
         <f t="shared" ref="J2:J4" si="0">CONCATENATE("['",C2,",'",D2,"']")</f>
         <v>['SPC,'INGLÉS']</v>
       </c>
-      <c r="K2">
-        <v>1</v>
-      </c>
-      <c r="L2">
-        <v>1</v>
+      <c r="K2" t="s">
+        <v>49</v>
       </c>
       <c r="O2" s="1" t="str">
         <f>CONCATENATE(A2,",",B2,",",C2,",",D2,",",E2,",",F2,",",G2,",",H2,",",I2,",",J2,",",K2,",",L2)</f>
-        <v>spc-prismatic-en,Prismatic Evolutions,SPC,INGLÉS,SPC,140000,179990,10,img/spc-prismatic-en.webp,['SPC,'INGLÉS'],1,1</v>
+        <v>spc-prismatic-en,Prismatic Evolutions,SPC,INGLÉS,SPC,140000,179990,10,img/spc-prismatic-en.webp,['SPC,'INGLÉS'],Oferta Flash,</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="B3" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="C3" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D3" t="s">
         <v>18</v>
       </c>
       <c r="E3" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="F3">
         <v>25000</v>
@@ -721,7 +864,7 @@
         <v>34990</v>
       </c>
       <c r="H3">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="I3" t="str">
         <f>CONCATENATE("img/",A3,".webp")</f>
@@ -731,23 +874,20 @@
         <f>CONCATENATE("['",C3,",'",D3,"']")</f>
         <v>['SPECIAL,'ESPAÑOL']</v>
       </c>
-      <c r="K3">
-        <v>1</v>
-      </c>
-      <c r="L3">
-        <v>1</v>
+      <c r="K3" t="s">
+        <v>49</v>
       </c>
       <c r="O3" s="1" t="str">
         <f>CONCATENATE(A3,",",B3,",",C3,",",D3,",",E3,",",F3,",",G3,",",H3,",",I3,",",J3,",",K3,",",L3)</f>
-        <v>special-garchomp-en,Garchomp EX,SPECIAL,ESPAÑOL,SPECIAL,25000,34990,10,img/special-garchomp-en.webp,['SPECIAL,'ESPAÑOL'],1,1</v>
+        <v>special-garchomp-en,Garchomp EX,SPECIAL,ESPAÑOL,SPECIAL,25000,34990,5,img/special-garchomp-en.webp,['SPECIAL,'ESPAÑOL'],Oferta Flash,</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="B4" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="C4" t="s">
         <v>20</v>
@@ -775,32 +915,29 @@
         <f t="shared" si="0"/>
         <v>['ETB,'ESPAÑOL']</v>
       </c>
-      <c r="K4">
-        <v>1</v>
-      </c>
-      <c r="L4">
-        <v>1</v>
+      <c r="K4" t="s">
+        <v>49</v>
       </c>
       <c r="O4" s="1" t="str">
-        <f t="shared" ref="O4:O16" si="2">CONCATENATE(A4,",",B4,",",C4,",",D4,",",E4,",",F4,",",G4,",",H4,",",I4,",",J4,",",K4,",",L4)</f>
-        <v>etb-destined-es,Rivales Predestinados,ETB,ESPAÑOL,ETB,40000,54990,10,img/etb-destined-es.webp,['ETB,'ESPAÑOL'],1,1</v>
+        <f>CONCATENATE(A4,",",B4,",",C4,",",D4,",",E4,",",F4,",",G4,",",H4,",",I4,",",J4,",",K4,",",L4)</f>
+        <v>etb-destined-es,Rivales Predestinados,ETB,ESPAÑOL,ETB,40000,54990,10,img/etb-destined-es.webp,['ETB,'ESPAÑOL'],Oferta Flash,</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="B5" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="C5" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D5" t="s">
         <v>18</v>
       </c>
       <c r="E5" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="F5">
         <v>25000</v>
@@ -809,7 +946,7 @@
         <v>34990</v>
       </c>
       <c r="H5">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="I5" t="str">
         <f>CONCATENATE("img/",A5,".webp")</f>
@@ -819,15 +956,12 @@
         <f>CONCATENATE("['",C5,",'",D5,"']")</f>
         <v>['SPECIAL,'ESPAÑOL']</v>
       </c>
-      <c r="K5">
-        <v>1</v>
-      </c>
-      <c r="L5">
-        <v>1</v>
+      <c r="K5" t="s">
+        <v>49</v>
       </c>
       <c r="O5" s="1" t="str">
         <f>CONCATENATE(A5,",",B5,",",C5,",",D5,",",E5,",",F5,",",G5,",",H5,",",I5,",",J5,",",K5,",",L5)</f>
-        <v>special-charizardex-en,Charizard EX,SPECIAL,ESPAÑOL,SPECIAL,25000,34990,10,img/special-charizardex-en.webp,['SPECIAL,'ESPAÑOL'],1,1</v>
+        <v>special-charizardex-en,Charizard EX,SPECIAL,ESPAÑOL,SPECIAL,25000,34990,5,img/special-charizardex-en.webp,['SPECIAL,'ESPAÑOL'],Oferta Flash,</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.35">
@@ -853,42 +987,39 @@
         <v>69990</v>
       </c>
       <c r="H6">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="I6" t="str">
-        <f t="shared" ref="I6" si="3">CONCATENATE("img/",A6,".webp")</f>
+        <f t="shared" ref="I6" si="2">CONCATENATE("img/",A6,".webp")</f>
         <v>img/etb-prismatic-es.webp</v>
       </c>
       <c r="J6" t="str">
         <f>CONCATENATE("['",C6,",'",D6,"']")</f>
         <v>['ETB,'ESPAÑOL']</v>
       </c>
-      <c r="K6">
-        <v>1</v>
-      </c>
-      <c r="L6">
-        <v>1</v>
+      <c r="K6" t="s">
+        <v>54</v>
       </c>
       <c r="O6" s="1" t="str">
-        <f t="shared" ref="O6" si="4">CONCATENATE(A6,",",B6,",",C6,",",D6,",",E6,",",F6,",",G6,",",H6,",",I6,",",J6,",",K6,",",L6)</f>
-        <v>etb-prismatic-es,Evoluciones Prismáticas,ETB,ESPAÑOL,ETB,55000,69990,10,img/etb-prismatic-es.webp,['ETB,'ESPAÑOL'],1,1</v>
+        <f>CONCATENATE(A6,",",B6,",",C6,",",D6,",",E6,",",F6,",",G6,",",H6,",",I6,",",J6,",",K6,",",L6)</f>
+        <v>etb-prismatic-es,Evoluciones Prismáticas,ETB,ESPAÑOL,ETB,55000,69990,2,img/etb-prismatic-es.webp,['ETB,'ESPAÑOL'],Últimas Unidades,</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="B7" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="C7" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D7" t="s">
         <v>19</v>
       </c>
       <c r="E7" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="F7">
         <v>28000</v>
@@ -897,42 +1028,39 @@
         <v>34990</v>
       </c>
       <c r="H7">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="I7" t="str">
         <f t="shared" si="1"/>
         <v>img/special-charizardex-en.webp</v>
       </c>
       <c r="J7" t="str">
-        <f t="shared" ref="J7:J8" si="5">CONCATENATE("['",C7,",'",D7,"']")</f>
+        <f t="shared" ref="J7:J8" si="3">CONCATENATE("['",C7,",'",D7,"']")</f>
         <v>['SPECIAL,'INGLÉS']</v>
       </c>
-      <c r="K7">
-        <v>1</v>
-      </c>
-      <c r="L7">
-        <v>1</v>
+      <c r="K7" t="s">
+        <v>54</v>
       </c>
       <c r="O7" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>special-charizardex-en,Charizard EX,SPECIAL,INGLÉS,SPECIAL,28000,34990,10,img/special-charizardex-en.webp,['SPECIAL,'INGLÉS'],1,1</v>
+        <f>CONCATENATE(A7,",",B7,",",C7,",",D7,",",E7,",",F7,",",G7,",",H7,",",I7,",",J7,",",K7,",",L7)</f>
+        <v>special-charizardex-en,Charizard EX,SPECIAL,INGLÉS,SPECIAL,28000,34990,5,img/special-charizardex-en.webp,['SPECIAL,'INGLÉS'],Últimas Unidades,</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="B8" t="s">
         <v>21</v>
       </c>
       <c r="C8" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="D8" t="s">
         <v>18</v>
       </c>
       <c r="E8" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="F8">
         <v>18000</v>
@@ -941,42 +1069,39 @@
         <v>19990</v>
       </c>
       <c r="H8">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="I8" t="str">
         <f t="shared" si="1"/>
         <v>img/poster-prismatic-en.webp</v>
       </c>
       <c r="J8" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>['POSTER,'ESPAÑOL']</v>
       </c>
-      <c r="K8">
-        <v>1</v>
-      </c>
-      <c r="L8">
-        <v>1</v>
+      <c r="K8" t="s">
+        <v>54</v>
       </c>
       <c r="O8" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>poster-prismatic-en,Prismatic Evolutions,POSTER,ESPAÑOL,POSTER,18000,19990,10,img/poster-prismatic-en.webp,['POSTER,'ESPAÑOL'],1,1</v>
+        <f>CONCATENATE(A8,",",B8,",",C8,",",D8,",",E8,",",F8,",",G8,",",H8,",",I8,",",J8,",",K8,",",L8)</f>
+        <v>poster-prismatic-en,Prismatic Evolutions,POSTER,ESPAÑOL,POSTER,18000,19990,2,img/poster-prismatic-en.webp,['POSTER,'ESPAÑOL'],Últimas Unidades,</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="B9" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="C9" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D9" t="s">
         <v>19</v>
       </c>
       <c r="E9" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="F9">
         <v>28000</v>
@@ -985,42 +1110,39 @@
         <v>35990</v>
       </c>
       <c r="H9">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="I9" t="str">
-        <f t="shared" ref="I9" si="6">CONCATENATE("img/",A9,".webp")</f>
+        <f t="shared" ref="I9" si="4">CONCATENATE("img/",A9,".webp")</f>
         <v>img/special-garchomp-en.webp</v>
       </c>
       <c r="J9" t="str">
-        <f t="shared" ref="J9:J10" si="7">CONCATENATE("['",C9,",'",D9,"']")</f>
+        <f t="shared" ref="J9:J10" si="5">CONCATENATE("['",C9,",'",D9,"']")</f>
         <v>['SPECIAL,'INGLÉS']</v>
       </c>
-      <c r="K9">
-        <v>1</v>
-      </c>
-      <c r="L9">
-        <v>1</v>
+      <c r="K9" t="s">
+        <v>54</v>
       </c>
       <c r="O9" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>special-garchomp-en,Garchomp EX,SPECIAL,INGLÉS,SPECIAL,28000,35990,10,img/special-garchomp-en.webp,['SPECIAL,'INGLÉS'],1,1</v>
+        <f>CONCATENATE(A9,",",B9,",",C9,",",D9,",",E9,",",F9,",",G9,",",H9,",",I9,",",J9,",",K9,",",L9)</f>
+        <v>special-garchomp-en,Garchomp EX,SPECIAL,INGLÉS,SPECIAL,28000,35990,5,img/special-garchomp-en.webp,['SPECIAL,'INGLÉS'],Últimas Unidades,</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="B10" t="s">
         <v>22</v>
       </c>
       <c r="C10" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="D10" t="s">
         <v>18</v>
       </c>
       <c r="E10" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="F10">
         <v>120000</v>
@@ -1029,42 +1151,39 @@
         <v>179990</v>
       </c>
       <c r="H10">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="I10" t="str">
         <f>CONCATENATE("img/",A10,".webp")</f>
         <v>img/spc-prismatic-en.webp</v>
       </c>
       <c r="J10" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>['SPC,'ESPAÑOL']</v>
       </c>
-      <c r="K10">
-        <v>1</v>
-      </c>
-      <c r="L10">
-        <v>1</v>
+      <c r="K10" t="s">
+        <v>54</v>
       </c>
       <c r="O10" s="1" t="str">
         <f>CONCATENATE(A10,",",B10,",",C10,",",D10,",",E10,",",F10,",",G10,",",H10,",",I10,",",J10,",",K10,",",L10)</f>
-        <v>spc-prismatic-en,Evoluciones Prismáticas,SPC,ESPAÑOL,SPC,120000,179990,10,img/spc-prismatic-en.webp,['SPC,'ESPAÑOL'],1,1</v>
+        <v>spc-prismatic-en,Evoluciones Prismáticas,SPC,ESPAÑOL,SPC,120000,179990,2,img/spc-prismatic-en.webp,['SPC,'ESPAÑOL'],Últimas Unidades,</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="B11" t="s">
         <v>21</v>
       </c>
       <c r="C11" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="D11" t="s">
         <v>19</v>
       </c>
       <c r="E11" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="F11">
         <v>35000</v>
@@ -1073,42 +1192,39 @@
         <v>39990</v>
       </c>
       <c r="H11">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="I11" t="str">
-        <f t="shared" ref="I11:I12" si="8">CONCATENATE("img/",A11,".webp")</f>
+        <f t="shared" ref="I11:I12" si="6">CONCATENATE("img/",A11,".webp")</f>
         <v>img/surprisebox-en.webp</v>
       </c>
       <c r="J11" t="str">
-        <f t="shared" ref="J11:J12" si="9">CONCATENATE("['",C11,",'",D11,"']")</f>
+        <f t="shared" ref="J11:J12" si="7">CONCATENATE("['",C11,",'",D11,"']")</f>
         <v>['SURPRISE BOX,'INGLÉS']</v>
       </c>
-      <c r="K11">
-        <v>1</v>
-      </c>
-      <c r="L11">
-        <v>1</v>
+      <c r="K11" t="s">
+        <v>54</v>
       </c>
       <c r="O11" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>surprisebox-en,Prismatic Evolutions,SURPRISE BOX,INGLÉS,SURPRISE BOX,35000,39990,10,img/surprisebox-en.webp,['SURPRISE BOX,'INGLÉS'],1,1</v>
+        <f>CONCATENATE(A11,",",B11,",",C11,",",D11,",",E11,",",F11,",",G11,",",H11,",",I11,",",J11,",",K11,",",L11)</f>
+        <v>surprisebox-en,Prismatic Evolutions,SURPRISE BOX,INGLÉS,SURPRISE BOX,35000,39990,2,img/surprisebox-en.webp,['SURPRISE BOX,'INGLÉS'],Últimas Unidades,</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="B12" t="s">
         <v>21</v>
       </c>
       <c r="C12" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="D12" t="s">
         <v>18</v>
       </c>
       <c r="E12" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="F12">
         <v>30000</v>
@@ -1117,33 +1233,30 @@
         <v>34990</v>
       </c>
       <c r="H12">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="I12" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>img/surprisebox-en.webp</v>
       </c>
       <c r="J12" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>['SURPRISE BOX,'ESPAÑOL']</v>
       </c>
-      <c r="K12">
-        <v>1</v>
-      </c>
-      <c r="L12">
-        <v>1</v>
+      <c r="K12" t="s">
+        <v>54</v>
       </c>
       <c r="O12" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>surprisebox-en,Prismatic Evolutions,SURPRISE BOX,ESPAÑOL,SURPRISE BOX,30000,34990,10,img/surprisebox-en.webp,['SURPRISE BOX,'ESPAÑOL'],1,1</v>
+        <f>CONCATENATE(A12,",",B12,",",C12,",",D12,",",E12,",",F12,",",G12,",",H12,",",I12,",",J12,",",K12,",",L12)</f>
+        <v>surprisebox-en,Prismatic Evolutions,SURPRISE BOX,ESPAÑOL,SURPRISE BOX,30000,34990,2,img/surprisebox-en.webp,['SURPRISE BOX,'ESPAÑOL'],Últimas Unidades,</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="B13" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="C13" t="s">
         <v>20</v>
@@ -1164,30 +1277,27 @@
         <v>10</v>
       </c>
       <c r="I13" t="str">
-        <f t="shared" ref="I13:I16" si="10">CONCATENATE("img/",A13,".webp")</f>
+        <f t="shared" ref="I13:I16" si="8">CONCATENATE("img/",A13,".webp")</f>
         <v>img/etb-megalucario-en.webp</v>
       </c>
       <c r="J13" t="str">
-        <f t="shared" ref="J13:J16" si="11">CONCATENATE("['",C13,",'",D13,"']")</f>
+        <f t="shared" ref="J13:J16" si="9">CONCATENATE("['",C13,",'",D13,"']")</f>
         <v>['ETB,'INGLÉS']</v>
       </c>
-      <c r="K13">
-        <v>1</v>
-      </c>
-      <c r="L13">
-        <v>1</v>
+      <c r="K13" t="s">
+        <v>50</v>
       </c>
       <c r="O13" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>etb-megalucario-en,Mega Evolutions,ETB,INGLÉS,ETB,64990,29990,10,img/etb-megalucario-en.webp,['ETB,'INGLÉS'],1,1</v>
+        <f>CONCATENATE(A13,",",B13,",",C13,",",D13,",",E13,",",F13,",",G13,",",H13,",",I13,",",J13,",",K13,",",L13)</f>
+        <v>etb-megalucario-en,Mega Evolutions,ETB,INGLÉS,ETB,64990,29990,10,img/etb-megalucario-en.webp,['ETB,'INGLÉS'],Preventa 26/09,</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="B14" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="C14" t="s">
         <v>20</v>
@@ -1208,30 +1318,27 @@
         <v>10</v>
       </c>
       <c r="I14" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>img/etb-megalucario-en.webp</v>
       </c>
       <c r="J14" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>['ETB,'ESPAÑOL']</v>
       </c>
-      <c r="K14">
-        <v>1</v>
-      </c>
-      <c r="L14">
-        <v>1</v>
+      <c r="K14" t="s">
+        <v>51</v>
       </c>
       <c r="O14" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>etb-megalucario-en,Megaevolución,ETB,ESPAÑOL,ETB,54990,29990,10,img/etb-megalucario-en.webp,['ETB,'ESPAÑOL'],1,1</v>
+        <f>CONCATENATE(A14,",",B14,",",C14,",",D14,",",E14,",",F14,",",G14,",",H14,",",I14,",",J14,",",K14,",",L14)</f>
+        <v>etb-megalucario-en,Megaevolución,ETB,ESPAÑOL,ETB,54990,29990,10,img/etb-megalucario-en.webp,['ETB,'ESPAÑOL'],Preventa 26/10,</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="B15" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="C15" t="s">
         <v>20</v>
@@ -1252,30 +1359,27 @@
         <v>10</v>
       </c>
       <c r="I15" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>img/etb-megagardevoir-en.webp</v>
       </c>
       <c r="J15" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>['ETB,'INGLÉS']</v>
       </c>
-      <c r="K15">
-        <v>1</v>
-      </c>
-      <c r="L15">
-        <v>1</v>
+      <c r="K15" t="s">
+        <v>52</v>
       </c>
       <c r="O15" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>etb-megagardevoir-en,Mega Evolutions,ETB,INGLÉS,ETB,64990,29990,10,img/etb-megagardevoir-en.webp,['ETB,'INGLÉS'],1,1</v>
+        <f>CONCATENATE(A15,",",B15,",",C15,",",D15,",",E15,",",F15,",",G15,",",H15,",",I15,",",J15,",",K15,",",L15)</f>
+        <v>etb-megagardevoir-en,Mega Evolutions,ETB,INGLÉS,ETB,64990,29990,10,img/etb-megagardevoir-en.webp,['ETB,'INGLÉS'],Preventa 26/11,</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="B16" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="C16" t="s">
         <v>20</v>
@@ -1296,22 +1400,19 @@
         <v>10</v>
       </c>
       <c r="I16" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>img/etb-megagardevoir-en.webp</v>
       </c>
       <c r="J16" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>['ETB,'ESPAÑOL']</v>
       </c>
-      <c r="K16">
-        <v>1</v>
-      </c>
-      <c r="L16">
-        <v>1</v>
+      <c r="K16" t="s">
+        <v>53</v>
       </c>
       <c r="O16" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>etb-megagardevoir-en,Megaevolución,ETB,ESPAÑOL,ETB,54990,29990,10,img/etb-megagardevoir-en.webp,['ETB,'ESPAÑOL'],1,1</v>
+        <f>CONCATENATE(A16,",",B16,",",C16,",",D16,",",E16,",",F16,",",G16,",",H16,",",I16,",",J16,",",K16,",",L16)</f>
+        <v>etb-megagardevoir-en,Megaevolución,ETB,ESPAÑOL,ETB,54990,29990,10,img/etb-megagardevoir-en.webp,['ETB,'ESPAÑOL'],Preventa 26/12,</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.35">
@@ -1337,25 +1438,22 @@
         <v>79990</v>
       </c>
       <c r="H17">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="I17" t="str">
-        <f>CONCATENATE("img/",A17,".webp")</f>
+        <f t="shared" ref="I17:I24" si="10">CONCATENATE("img/",A17,".webp")</f>
         <v>img/etb-white-flare-en.webp</v>
       </c>
       <c r="J17" t="str">
-        <f>CONCATENATE("['",C17,",'",D17,"']")</f>
+        <f t="shared" ref="J17:J24" si="11">CONCATENATE("['",C17,",'",D17,"']")</f>
         <v>['ETB,'INGLÉS']</v>
       </c>
-      <c r="K17">
-        <v>1</v>
-      </c>
-      <c r="L17">
-        <v>1</v>
+      <c r="K17" t="s">
+        <v>54</v>
       </c>
       <c r="O17" s="1" t="str">
         <f>CONCATENATE(A17,",",B17,",",C17,",",D17,",",E17,",",F17,",",G17,",",H17,",",I17,",",J17,",",K17,",",L17)</f>
-        <v>etb-white-flare-en,White Flare,ETB,INGLÉS,ETB,74990,79990,10,img/etb-white-flare-en.webp,['ETB,'INGLÉS'],1,1</v>
+        <v>etb-white-flare-en,White Flare,ETB,INGLÉS,ETB,74990,79990,2,img/etb-white-flare-en.webp,['ETB,'INGLÉS'],Últimas Unidades,</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.35">
@@ -1381,25 +1479,22 @@
         <v>79990</v>
       </c>
       <c r="H18">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="I18" t="str">
-        <f>CONCATENATE("img/",A18,".webp")</f>
+        <f t="shared" si="10"/>
         <v>img/etb-white-flare-en.webp</v>
       </c>
       <c r="J18" t="str">
-        <f>CONCATENATE("['",C18,",'",D18,"']")</f>
+        <f t="shared" si="11"/>
         <v>['ETB,'ESPAÑOL']</v>
       </c>
-      <c r="K18">
-        <v>1</v>
-      </c>
-      <c r="L18">
-        <v>1</v>
+      <c r="K18" t="s">
+        <v>54</v>
       </c>
       <c r="O18" s="1" t="str">
         <f>CONCATENATE(A18,",",B18,",",C18,",",D18,",",E18,",",F18,",",G18,",",H18,",",I18,",",J18,",",K18,",",L18)</f>
-        <v>etb-white-flare-en,Llama Blanca,ETB,ESPAÑOL,ETB,69990,79990,10,img/etb-white-flare-en.webp,['ETB,'ESPAÑOL'],1,1</v>
+        <v>etb-white-flare-en,Llama Blanca,ETB,ESPAÑOL,ETB,69990,79990,2,img/etb-white-flare-en.webp,['ETB,'ESPAÑOL'],Últimas Unidades,</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.35">
@@ -1425,25 +1520,22 @@
         <v>79990</v>
       </c>
       <c r="H19">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="I19" t="str">
-        <f>CONCATENATE("img/",A19,".webp")</f>
+        <f t="shared" si="10"/>
         <v>img/etb-black-bolt-en.webp</v>
       </c>
       <c r="J19" t="str">
-        <f>CONCATENATE("['",C19,",'",D19,"']")</f>
+        <f t="shared" si="11"/>
         <v>['ETB,'INGLÉS']</v>
       </c>
-      <c r="K19">
-        <v>1</v>
-      </c>
-      <c r="L19">
-        <v>1</v>
+      <c r="K19" t="s">
+        <v>54</v>
       </c>
       <c r="O19" s="1" t="str">
         <f>CONCATENATE(A19,",",B19,",",C19,",",D19,",",E19,",",F19,",",G19,",",H19,",",I19,",",J19,",",K19,",",L19)</f>
-        <v>etb-black-bolt-en,Black Bolt,ETB,INGLÉS,ETB,74990,79990,10,img/etb-black-bolt-en.webp,['ETB,'INGLÉS'],1,1</v>
+        <v>etb-black-bolt-en,Black Bolt,ETB,INGLÉS,ETB,74990,79990,2,img/etb-black-bolt-en.webp,['ETB,'INGLÉS'],Últimas Unidades,</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.35">
@@ -1469,25 +1561,22 @@
         <v>79990</v>
       </c>
       <c r="H20">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="I20" t="str">
-        <f>CONCATENATE("img/",A20,".webp")</f>
+        <f t="shared" si="10"/>
         <v>img/etb-black-bolt-es.webp</v>
       </c>
       <c r="J20" t="str">
-        <f>CONCATENATE("['",C20,",'",D20,"']")</f>
+        <f t="shared" si="11"/>
         <v>['ETB,'ESPAÑOL']</v>
       </c>
-      <c r="K20">
-        <v>1</v>
-      </c>
-      <c r="L20">
-        <v>1</v>
+      <c r="K20" t="s">
+        <v>54</v>
       </c>
       <c r="O20" s="1" t="str">
         <f>CONCATENATE(A20,",",B20,",",C20,",",D20,",",E20,",",F20,",",G20,",",H20,",",I20,",",J20,",",K20,",",L20)</f>
-        <v>etb-black-bolt-es,Fulgor Negro,ETB,ESPAÑOL,ETB,69990,79990,10,img/etb-black-bolt-es.webp,['ETB,'ESPAÑOL'],1,1</v>
+        <v>etb-black-bolt-es,Fulgor Negro,ETB,ESPAÑOL,ETB,69990,79990,2,img/etb-black-bolt-es.webp,['ETB,'ESPAÑOL'],Últimas Unidades,</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.35">
@@ -1513,25 +1602,22 @@
         <v>79990</v>
       </c>
       <c r="H21">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="I21" t="str">
-        <f>CONCATENATE("img/",A21,".webp")</f>
+        <f t="shared" si="10"/>
         <v>img/etb-aventuras-es.webp</v>
       </c>
       <c r="J21" t="str">
-        <f>CONCATENATE("['",C21,",'",D21,"']")</f>
+        <f t="shared" si="11"/>
         <v>['ETB,'INGLÉS']</v>
       </c>
-      <c r="K21">
-        <v>1</v>
-      </c>
-      <c r="L21">
-        <v>1</v>
+      <c r="K21" t="s">
+        <v>54</v>
       </c>
       <c r="O21" s="1" t="str">
         <f>CONCATENATE(A21,",",B21,",",C21,",",D21,",",E21,",",F21,",",G21,",",H21,",",I21,",",J21,",",K21,",",L21)</f>
-        <v>etb-aventuras-es,Journey Together,ETB,INGLÉS,ETB,74990,79990,10,img/etb-aventuras-es.webp,['ETB,'INGLÉS'],1,1</v>
+        <v>etb-aventuras-es,Journey Together,ETB,INGLÉS,ETB,74990,79990,2,img/etb-aventuras-es.webp,['ETB,'INGLÉS'],Últimas Unidades,</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.35">
@@ -1557,42 +1643,39 @@
         <v>79990</v>
       </c>
       <c r="H22">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="I22" t="str">
-        <f>CONCATENATE("img/",A22,".webp")</f>
+        <f t="shared" si="10"/>
         <v>img/etb-aventuras-es.webp</v>
       </c>
       <c r="J22" t="str">
-        <f>CONCATENATE("['",C22,",'",D22,"']")</f>
+        <f t="shared" si="11"/>
         <v>['ETB,'ESPAÑOL']</v>
       </c>
-      <c r="K22">
-        <v>1</v>
-      </c>
-      <c r="L22">
-        <v>1</v>
+      <c r="K22" t="s">
+        <v>54</v>
       </c>
       <c r="O22" s="1" t="str">
         <f>CONCATENATE(A22,",",B22,",",C22,",",D22,",",E22,",",F22,",",G22,",",H22,",",I22,",",J22,",",K22,",",L22)</f>
-        <v>etb-aventuras-es,Aventuras Compartidas,ETB,ESPAÑOL,ETB,69990,79990,10,img/etb-aventuras-es.webp,['ETB,'ESPAÑOL'],1,1</v>
+        <v>etb-aventuras-es,Aventuras Compartidas,ETB,ESPAÑOL,ETB,69990,79990,2,img/etb-aventuras-es.webp,['ETB,'ESPAÑOL'],Últimas Unidades,</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="B23" t="s">
         <v>26</v>
       </c>
       <c r="C23" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="D23" t="s">
         <v>18</v>
       </c>
       <c r="E23" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="F23">
         <v>34990</v>
@@ -1601,42 +1684,39 @@
         <v>34990</v>
       </c>
       <c r="H23">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="I23" t="str">
-        <f>CONCATENATE("img/",A23,".webp")</f>
+        <f t="shared" si="10"/>
         <v>img/bin-white-flare-es.webp</v>
       </c>
       <c r="J23" t="str">
-        <f>CONCATENATE("['",C23,",'",D23,"']")</f>
+        <f t="shared" si="11"/>
         <v>['BINDER,'ESPAÑOL']</v>
       </c>
-      <c r="K23">
-        <v>1</v>
-      </c>
-      <c r="L23">
-        <v>1</v>
+      <c r="K23" t="s">
+        <v>54</v>
       </c>
       <c r="O23" s="1" t="str">
         <f>CONCATENATE(A23,",",B23,",",C23,",",D23,",",E23,",",F23,",",G23,",",H23,",",I23,",",J23,",",K23,",",L23)</f>
-        <v>bin-white-flare-es,Llama Blanca,BINDER,ESPAÑOL,BINDER,34990,34990,10,img/bin-white-flare-es.webp,['BINDER,'ESPAÑOL'],1,1</v>
+        <v>bin-white-flare-es,Llama Blanca,BINDER,ESPAÑOL,BINDER,34990,34990,2,img/bin-white-flare-es.webp,['BINDER,'ESPAÑOL'],Últimas Unidades,</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="B24" t="s">
         <v>28</v>
       </c>
       <c r="C24" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="D24" t="s">
         <v>18</v>
       </c>
       <c r="E24" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="F24">
         <v>34990</v>
@@ -1645,28 +1725,26 @@
         <v>34990</v>
       </c>
       <c r="H24">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="I24" t="str">
-        <f>CONCATENATE("img/",A24,".webp")</f>
+        <f t="shared" si="10"/>
         <v>img/bin-black-bolt-es.webp</v>
       </c>
       <c r="J24" t="str">
-        <f>CONCATENATE("['",C24,",'",D24,"']")</f>
+        <f t="shared" si="11"/>
         <v>['BINDER,'ESPAÑOL']</v>
       </c>
-      <c r="K24">
-        <v>1</v>
-      </c>
-      <c r="L24">
-        <v>1</v>
+      <c r="K24" t="s">
+        <v>54</v>
       </c>
       <c r="O24" s="1" t="str">
         <f>CONCATENATE(A24,",",B24,",",C24,",",D24,",",E24,",",F24,",",G24,",",H24,",",I24,",",J24,",",K24,",",L24)</f>
-        <v>bin-black-bolt-es,Fulgor Negro,BINDER,ESPAÑOL,BINDER,34990,34990,10,img/bin-black-bolt-es.webp,['BINDER,'ESPAÑOL'],1,1</v>
+        <v>bin-black-bolt-es,Fulgor Negro,BINDER,ESPAÑOL,BINDER,34990,34990,2,img/bin-black-bolt-es.webp,['BINDER,'ESPAÑOL'],Últimas Unidades,</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
ActualizaciÃ³n completa (2025-09-21 22:36)
</commit_message>
<xml_diff>
--- a/BACKUP/SUPORT IMAGEN.xlsx
+++ b/BACKUP/SUPORT IMAGEN.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jorgg\OneDrive\MasterHIT\BACKUP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1937DB8D-50E5-4194-9FD5-E5E4DEBD9379}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04328B6C-63D7-448F-9F44-27BCD2EFACEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="74">
   <si>
     <t>id,name,set,type,category,price,compareAtPrice,stock,image,tags,source,createdAt</t>
   </si>
@@ -190,18 +190,6 @@
   </si>
   <si>
     <t>Preventa 26/09</t>
-  </si>
-  <si>
-    <t>Preventa 26/10</t>
-  </si>
-  <si>
-    <t>Preventa 26/11</t>
-  </si>
-  <si>
-    <t>Preventa 26/12</t>
-  </si>
-  <si>
-    <t>Últimas Unidades</t>
   </si>
   <si>
     <t>spc-prismatic-en,Prismatic Evolutions,SPC,INGLÉS,SPC,140000,179990,10,img/spc-prismatic-en.webp,['SPC,'INGLÉS'],Oferta Flash,</t>
@@ -603,7 +591,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:A24"/>
     </sheetView>
   </sheetViews>
@@ -616,117 +604,117 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -738,9 +726,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3CA635C-1DF7-4EEC-B0B8-3FA5C80D03DF}">
   <dimension ref="A1:O24"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1:O24"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -837,7 +823,7 @@
         <v>49</v>
       </c>
       <c r="O2" s="1" t="str">
-        <f>CONCATENATE(A2,",",B2,",",C2,",",D2,",",E2,",",F2,",",G2,",",H2,",",I2,",",J2,",",K2,",",L2)</f>
+        <f t="shared" ref="O2:O24" si="1">CONCATENATE(A2,",",B2,",",C2,",",D2,",",E2,",",F2,",",G2,",",H2,",",I2,",",J2,",",K2,",",L2)</f>
         <v>spc-prismatic-en,Prismatic Evolutions,SPC,INGLÉS,SPC,140000,179990,10,img/spc-prismatic-en.webp,['SPC,'INGLÉS'],Oferta Flash,</v>
       </c>
     </row>
@@ -878,7 +864,7 @@
         <v>49</v>
       </c>
       <c r="O3" s="1" t="str">
-        <f>CONCATENATE(A3,",",B3,",",C3,",",D3,",",E3,",",F3,",",G3,",",H3,",",I3,",",J3,",",K3,",",L3)</f>
+        <f t="shared" si="1"/>
         <v>special-garchomp-en,Garchomp EX,SPECIAL,ESPAÑOL,SPECIAL,25000,34990,5,img/special-garchomp-en.webp,['SPECIAL,'ESPAÑOL'],Oferta Flash,</v>
       </c>
     </row>
@@ -908,7 +894,7 @@
         <v>10</v>
       </c>
       <c r="I4" t="str">
-        <f t="shared" ref="I4:I8" si="1">CONCATENATE("img/",A4,".webp")</f>
+        <f t="shared" ref="I4:I8" si="2">CONCATENATE("img/",A4,".webp")</f>
         <v>img/etb-destined-es.webp</v>
       </c>
       <c r="J4" t="str">
@@ -919,7 +905,7 @@
         <v>49</v>
       </c>
       <c r="O4" s="1" t="str">
-        <f>CONCATENATE(A4,",",B4,",",C4,",",D4,",",E4,",",F4,",",G4,",",H4,",",I4,",",J4,",",K4,",",L4)</f>
+        <f t="shared" si="1"/>
         <v>etb-destined-es,Rivales Predestinados,ETB,ESPAÑOL,ETB,40000,54990,10,img/etb-destined-es.webp,['ETB,'ESPAÑOL'],Oferta Flash,</v>
       </c>
     </row>
@@ -960,7 +946,7 @@
         <v>49</v>
       </c>
       <c r="O5" s="1" t="str">
-        <f>CONCATENATE(A5,",",B5,",",C5,",",D5,",",E5,",",F5,",",G5,",",H5,",",I5,",",J5,",",K5,",",L5)</f>
+        <f t="shared" si="1"/>
         <v>special-charizardex-en,Charizard EX,SPECIAL,ESPAÑOL,SPECIAL,25000,34990,5,img/special-charizardex-en.webp,['SPECIAL,'ESPAÑOL'],Oferta Flash,</v>
       </c>
     </row>
@@ -990,19 +976,16 @@
         <v>2</v>
       </c>
       <c r="I6" t="str">
-        <f t="shared" ref="I6" si="2">CONCATENATE("img/",A6,".webp")</f>
+        <f t="shared" ref="I6" si="3">CONCATENATE("img/",A6,".webp")</f>
         <v>img/etb-prismatic-es.webp</v>
       </c>
       <c r="J6" t="str">
         <f>CONCATENATE("['",C6,",'",D6,"']")</f>
         <v>['ETB,'ESPAÑOL']</v>
       </c>
-      <c r="K6" t="s">
-        <v>54</v>
-      </c>
       <c r="O6" s="1" t="str">
-        <f>CONCATENATE(A6,",",B6,",",C6,",",D6,",",E6,",",F6,",",G6,",",H6,",",I6,",",J6,",",K6,",",L6)</f>
-        <v>etb-prismatic-es,Evoluciones Prismáticas,ETB,ESPAÑOL,ETB,55000,69990,2,img/etb-prismatic-es.webp,['ETB,'ESPAÑOL'],Últimas Unidades,</v>
+        <f t="shared" si="1"/>
+        <v>etb-prismatic-es,Evoluciones Prismáticas,ETB,ESPAÑOL,ETB,55000,69990,2,img/etb-prismatic-es.webp,['ETB,'ESPAÑOL'],,</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.35">
@@ -1031,19 +1014,16 @@
         <v>5</v>
       </c>
       <c r="I7" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>img/special-charizardex-en.webp</v>
       </c>
       <c r="J7" t="str">
-        <f t="shared" ref="J7:J8" si="3">CONCATENATE("['",C7,",'",D7,"']")</f>
+        <f t="shared" ref="J7:J8" si="4">CONCATENATE("['",C7,",'",D7,"']")</f>
         <v>['SPECIAL,'INGLÉS']</v>
       </c>
-      <c r="K7" t="s">
-        <v>54</v>
-      </c>
       <c r="O7" s="1" t="str">
-        <f>CONCATENATE(A7,",",B7,",",C7,",",D7,",",E7,",",F7,",",G7,",",H7,",",I7,",",J7,",",K7,",",L7)</f>
-        <v>special-charizardex-en,Charizard EX,SPECIAL,INGLÉS,SPECIAL,28000,34990,5,img/special-charizardex-en.webp,['SPECIAL,'INGLÉS'],Últimas Unidades,</v>
+        <f t="shared" si="1"/>
+        <v>special-charizardex-en,Charizard EX,SPECIAL,INGLÉS,SPECIAL,28000,34990,5,img/special-charizardex-en.webp,['SPECIAL,'INGLÉS'],,</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.35">
@@ -1072,19 +1052,16 @@
         <v>2</v>
       </c>
       <c r="I8" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>img/poster-prismatic-en.webp</v>
       </c>
       <c r="J8" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>['POSTER,'ESPAÑOL']</v>
       </c>
-      <c r="K8" t="s">
-        <v>54</v>
-      </c>
       <c r="O8" s="1" t="str">
-        <f>CONCATENATE(A8,",",B8,",",C8,",",D8,",",E8,",",F8,",",G8,",",H8,",",I8,",",J8,",",K8,",",L8)</f>
-        <v>poster-prismatic-en,Prismatic Evolutions,POSTER,ESPAÑOL,POSTER,18000,19990,2,img/poster-prismatic-en.webp,['POSTER,'ESPAÑOL'],Últimas Unidades,</v>
+        <f t="shared" si="1"/>
+        <v>poster-prismatic-en,Prismatic Evolutions,POSTER,ESPAÑOL,POSTER,18000,19990,2,img/poster-prismatic-en.webp,['POSTER,'ESPAÑOL'],,</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.35">
@@ -1113,19 +1090,16 @@
         <v>5</v>
       </c>
       <c r="I9" t="str">
-        <f t="shared" ref="I9" si="4">CONCATENATE("img/",A9,".webp")</f>
+        <f t="shared" ref="I9" si="5">CONCATENATE("img/",A9,".webp")</f>
         <v>img/special-garchomp-en.webp</v>
       </c>
       <c r="J9" t="str">
-        <f t="shared" ref="J9:J10" si="5">CONCATENATE("['",C9,",'",D9,"']")</f>
+        <f t="shared" ref="J9:J10" si="6">CONCATENATE("['",C9,",'",D9,"']")</f>
         <v>['SPECIAL,'INGLÉS']</v>
       </c>
-      <c r="K9" t="s">
-        <v>54</v>
-      </c>
       <c r="O9" s="1" t="str">
-        <f>CONCATENATE(A9,",",B9,",",C9,",",D9,",",E9,",",F9,",",G9,",",H9,",",I9,",",J9,",",K9,",",L9)</f>
-        <v>special-garchomp-en,Garchomp EX,SPECIAL,INGLÉS,SPECIAL,28000,35990,5,img/special-garchomp-en.webp,['SPECIAL,'INGLÉS'],Últimas Unidades,</v>
+        <f t="shared" si="1"/>
+        <v>special-garchomp-en,Garchomp EX,SPECIAL,INGLÉS,SPECIAL,28000,35990,5,img/special-garchomp-en.webp,['SPECIAL,'INGLÉS'],,</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.35">
@@ -1158,15 +1132,12 @@
         <v>img/spc-prismatic-en.webp</v>
       </c>
       <c r="J10" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>['SPC,'ESPAÑOL']</v>
       </c>
-      <c r="K10" t="s">
-        <v>54</v>
-      </c>
       <c r="O10" s="1" t="str">
-        <f>CONCATENATE(A10,",",B10,",",C10,",",D10,",",E10,",",F10,",",G10,",",H10,",",I10,",",J10,",",K10,",",L10)</f>
-        <v>spc-prismatic-en,Evoluciones Prismáticas,SPC,ESPAÑOL,SPC,120000,179990,2,img/spc-prismatic-en.webp,['SPC,'ESPAÑOL'],Últimas Unidades,</v>
+        <f t="shared" si="1"/>
+        <v>spc-prismatic-en,Evoluciones Prismáticas,SPC,ESPAÑOL,SPC,120000,179990,2,img/spc-prismatic-en.webp,['SPC,'ESPAÑOL'],,</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.35">
@@ -1195,19 +1166,16 @@
         <v>2</v>
       </c>
       <c r="I11" t="str">
-        <f t="shared" ref="I11:I12" si="6">CONCATENATE("img/",A11,".webp")</f>
+        <f t="shared" ref="I11:I12" si="7">CONCATENATE("img/",A11,".webp")</f>
         <v>img/surprisebox-en.webp</v>
       </c>
       <c r="J11" t="str">
-        <f t="shared" ref="J11:J12" si="7">CONCATENATE("['",C11,",'",D11,"']")</f>
+        <f t="shared" ref="J11:J12" si="8">CONCATENATE("['",C11,",'",D11,"']")</f>
         <v>['SURPRISE BOX,'INGLÉS']</v>
       </c>
-      <c r="K11" t="s">
-        <v>54</v>
-      </c>
       <c r="O11" s="1" t="str">
-        <f>CONCATENATE(A11,",",B11,",",C11,",",D11,",",E11,",",F11,",",G11,",",H11,",",I11,",",J11,",",K11,",",L11)</f>
-        <v>surprisebox-en,Prismatic Evolutions,SURPRISE BOX,INGLÉS,SURPRISE BOX,35000,39990,2,img/surprisebox-en.webp,['SURPRISE BOX,'INGLÉS'],Últimas Unidades,</v>
+        <f t="shared" si="1"/>
+        <v>surprisebox-en,Prismatic Evolutions,SURPRISE BOX,INGLÉS,SURPRISE BOX,35000,39990,2,img/surprisebox-en.webp,['SURPRISE BOX,'INGLÉS'],,</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.35">
@@ -1236,19 +1204,16 @@
         <v>2</v>
       </c>
       <c r="I12" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>img/surprisebox-en.webp</v>
       </c>
       <c r="J12" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>['SURPRISE BOX,'ESPAÑOL']</v>
       </c>
-      <c r="K12" t="s">
-        <v>54</v>
-      </c>
       <c r="O12" s="1" t="str">
-        <f>CONCATENATE(A12,",",B12,",",C12,",",D12,",",E12,",",F12,",",G12,",",H12,",",I12,",",J12,",",K12,",",L12)</f>
-        <v>surprisebox-en,Prismatic Evolutions,SURPRISE BOX,ESPAÑOL,SURPRISE BOX,30000,34990,2,img/surprisebox-en.webp,['SURPRISE BOX,'ESPAÑOL'],Últimas Unidades,</v>
+        <f t="shared" si="1"/>
+        <v>surprisebox-en,Prismatic Evolutions,SURPRISE BOX,ESPAÑOL,SURPRISE BOX,30000,34990,2,img/surprisebox-en.webp,['SURPRISE BOX,'ESPAÑOL'],,</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.35">
@@ -1277,18 +1242,18 @@
         <v>10</v>
       </c>
       <c r="I13" t="str">
-        <f t="shared" ref="I13:I16" si="8">CONCATENATE("img/",A13,".webp")</f>
+        <f t="shared" ref="I13:I16" si="9">CONCATENATE("img/",A13,".webp")</f>
         <v>img/etb-megalucario-en.webp</v>
       </c>
       <c r="J13" t="str">
-        <f t="shared" ref="J13:J16" si="9">CONCATENATE("['",C13,",'",D13,"']")</f>
+        <f t="shared" ref="J13:J16" si="10">CONCATENATE("['",C13,",'",D13,"']")</f>
         <v>['ETB,'INGLÉS']</v>
       </c>
       <c r="K13" t="s">
         <v>50</v>
       </c>
       <c r="O13" s="1" t="str">
-        <f>CONCATENATE(A13,",",B13,",",C13,",",D13,",",E13,",",F13,",",G13,",",H13,",",I13,",",J13,",",K13,",",L13)</f>
+        <f t="shared" si="1"/>
         <v>etb-megalucario-en,Mega Evolutions,ETB,INGLÉS,ETB,64990,29990,10,img/etb-megalucario-en.webp,['ETB,'INGLÉS'],Preventa 26/09,</v>
       </c>
     </row>
@@ -1318,19 +1283,19 @@
         <v>10</v>
       </c>
       <c r="I14" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>img/etb-megalucario-en.webp</v>
       </c>
       <c r="J14" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>['ETB,'ESPAÑOL']</v>
       </c>
       <c r="K14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="O14" s="1" t="str">
-        <f>CONCATENATE(A14,",",B14,",",C14,",",D14,",",E14,",",F14,",",G14,",",H14,",",I14,",",J14,",",K14,",",L14)</f>
-        <v>etb-megalucario-en,Megaevolución,ETB,ESPAÑOL,ETB,54990,29990,10,img/etb-megalucario-en.webp,['ETB,'ESPAÑOL'],Preventa 26/10,</v>
+        <f t="shared" si="1"/>
+        <v>etb-megalucario-en,Megaevolución,ETB,ESPAÑOL,ETB,54990,29990,10,img/etb-megalucario-en.webp,['ETB,'ESPAÑOL'],Preventa 26/09,</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.35">
@@ -1359,19 +1324,19 @@
         <v>10</v>
       </c>
       <c r="I15" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>img/etb-megagardevoir-en.webp</v>
       </c>
       <c r="J15" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>['ETB,'INGLÉS']</v>
       </c>
       <c r="K15" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="O15" s="1" t="str">
-        <f>CONCATENATE(A15,",",B15,",",C15,",",D15,",",E15,",",F15,",",G15,",",H15,",",I15,",",J15,",",K15,",",L15)</f>
-        <v>etb-megagardevoir-en,Mega Evolutions,ETB,INGLÉS,ETB,64990,29990,10,img/etb-megagardevoir-en.webp,['ETB,'INGLÉS'],Preventa 26/11,</v>
+        <f t="shared" si="1"/>
+        <v>etb-megagardevoir-en,Mega Evolutions,ETB,INGLÉS,ETB,64990,29990,10,img/etb-megagardevoir-en.webp,['ETB,'INGLÉS'],Preventa 26/09,</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.35">
@@ -1400,19 +1365,19 @@
         <v>10</v>
       </c>
       <c r="I16" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>img/etb-megagardevoir-en.webp</v>
       </c>
       <c r="J16" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>['ETB,'ESPAÑOL']</v>
       </c>
       <c r="K16" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="O16" s="1" t="str">
-        <f>CONCATENATE(A16,",",B16,",",C16,",",D16,",",E16,",",F16,",",G16,",",H16,",",I16,",",J16,",",K16,",",L16)</f>
-        <v>etb-megagardevoir-en,Megaevolución,ETB,ESPAÑOL,ETB,54990,29990,10,img/etb-megagardevoir-en.webp,['ETB,'ESPAÑOL'],Preventa 26/12,</v>
+        <f t="shared" si="1"/>
+        <v>etb-megagardevoir-en,Megaevolución,ETB,ESPAÑOL,ETB,54990,29990,10,img/etb-megagardevoir-en.webp,['ETB,'ESPAÑOL'],Preventa 26/09,</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.35">
@@ -1441,19 +1406,16 @@
         <v>2</v>
       </c>
       <c r="I17" t="str">
-        <f t="shared" ref="I17:I24" si="10">CONCATENATE("img/",A17,".webp")</f>
+        <f t="shared" ref="I17:I24" si="11">CONCATENATE("img/",A17,".webp")</f>
         <v>img/etb-white-flare-en.webp</v>
       </c>
       <c r="J17" t="str">
-        <f t="shared" ref="J17:J24" si="11">CONCATENATE("['",C17,",'",D17,"']")</f>
+        <f t="shared" ref="J17:J24" si="12">CONCATENATE("['",C17,",'",D17,"']")</f>
         <v>['ETB,'INGLÉS']</v>
       </c>
-      <c r="K17" t="s">
-        <v>54</v>
-      </c>
       <c r="O17" s="1" t="str">
-        <f>CONCATENATE(A17,",",B17,",",C17,",",D17,",",E17,",",F17,",",G17,",",H17,",",I17,",",J17,",",K17,",",L17)</f>
-        <v>etb-white-flare-en,White Flare,ETB,INGLÉS,ETB,74990,79990,2,img/etb-white-flare-en.webp,['ETB,'INGLÉS'],Últimas Unidades,</v>
+        <f t="shared" si="1"/>
+        <v>etb-white-flare-en,White Flare,ETB,INGLÉS,ETB,74990,79990,2,img/etb-white-flare-en.webp,['ETB,'INGLÉS'],,</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.35">
@@ -1482,19 +1444,16 @@
         <v>2</v>
       </c>
       <c r="I18" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>img/etb-white-flare-en.webp</v>
       </c>
       <c r="J18" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>['ETB,'ESPAÑOL']</v>
       </c>
-      <c r="K18" t="s">
-        <v>54</v>
-      </c>
       <c r="O18" s="1" t="str">
-        <f>CONCATENATE(A18,",",B18,",",C18,",",D18,",",E18,",",F18,",",G18,",",H18,",",I18,",",J18,",",K18,",",L18)</f>
-        <v>etb-white-flare-en,Llama Blanca,ETB,ESPAÑOL,ETB,69990,79990,2,img/etb-white-flare-en.webp,['ETB,'ESPAÑOL'],Últimas Unidades,</v>
+        <f t="shared" si="1"/>
+        <v>etb-white-flare-en,Llama Blanca,ETB,ESPAÑOL,ETB,69990,79990,2,img/etb-white-flare-en.webp,['ETB,'ESPAÑOL'],,</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.35">
@@ -1523,19 +1482,16 @@
         <v>2</v>
       </c>
       <c r="I19" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>img/etb-black-bolt-en.webp</v>
       </c>
       <c r="J19" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>['ETB,'INGLÉS']</v>
       </c>
-      <c r="K19" t="s">
-        <v>54</v>
-      </c>
       <c r="O19" s="1" t="str">
-        <f>CONCATENATE(A19,",",B19,",",C19,",",D19,",",E19,",",F19,",",G19,",",H19,",",I19,",",J19,",",K19,",",L19)</f>
-        <v>etb-black-bolt-en,Black Bolt,ETB,INGLÉS,ETB,74990,79990,2,img/etb-black-bolt-en.webp,['ETB,'INGLÉS'],Últimas Unidades,</v>
+        <f t="shared" si="1"/>
+        <v>etb-black-bolt-en,Black Bolt,ETB,INGLÉS,ETB,74990,79990,2,img/etb-black-bolt-en.webp,['ETB,'INGLÉS'],,</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.35">
@@ -1564,19 +1520,16 @@
         <v>2</v>
       </c>
       <c r="I20" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>img/etb-black-bolt-es.webp</v>
       </c>
       <c r="J20" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>['ETB,'ESPAÑOL']</v>
       </c>
-      <c r="K20" t="s">
-        <v>54</v>
-      </c>
       <c r="O20" s="1" t="str">
-        <f>CONCATENATE(A20,",",B20,",",C20,",",D20,",",E20,",",F20,",",G20,",",H20,",",I20,",",J20,",",K20,",",L20)</f>
-        <v>etb-black-bolt-es,Fulgor Negro,ETB,ESPAÑOL,ETB,69990,79990,2,img/etb-black-bolt-es.webp,['ETB,'ESPAÑOL'],Últimas Unidades,</v>
+        <f t="shared" si="1"/>
+        <v>etb-black-bolt-es,Fulgor Negro,ETB,ESPAÑOL,ETB,69990,79990,2,img/etb-black-bolt-es.webp,['ETB,'ESPAÑOL'],,</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.35">
@@ -1605,19 +1558,16 @@
         <v>2</v>
       </c>
       <c r="I21" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>img/etb-aventuras-es.webp</v>
       </c>
       <c r="J21" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>['ETB,'INGLÉS']</v>
       </c>
-      <c r="K21" t="s">
-        <v>54</v>
-      </c>
       <c r="O21" s="1" t="str">
-        <f>CONCATENATE(A21,",",B21,",",C21,",",D21,",",E21,",",F21,",",G21,",",H21,",",I21,",",J21,",",K21,",",L21)</f>
-        <v>etb-aventuras-es,Journey Together,ETB,INGLÉS,ETB,74990,79990,2,img/etb-aventuras-es.webp,['ETB,'INGLÉS'],Últimas Unidades,</v>
+        <f t="shared" si="1"/>
+        <v>etb-aventuras-es,Journey Together,ETB,INGLÉS,ETB,74990,79990,2,img/etb-aventuras-es.webp,['ETB,'INGLÉS'],,</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.35">
@@ -1646,19 +1596,16 @@
         <v>2</v>
       </c>
       <c r="I22" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>img/etb-aventuras-es.webp</v>
       </c>
       <c r="J22" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>['ETB,'ESPAÑOL']</v>
       </c>
-      <c r="K22" t="s">
-        <v>54</v>
-      </c>
       <c r="O22" s="1" t="str">
-        <f>CONCATENATE(A22,",",B22,",",C22,",",D22,",",E22,",",F22,",",G22,",",H22,",",I22,",",J22,",",K22,",",L22)</f>
-        <v>etb-aventuras-es,Aventuras Compartidas,ETB,ESPAÑOL,ETB,69990,79990,2,img/etb-aventuras-es.webp,['ETB,'ESPAÑOL'],Últimas Unidades,</v>
+        <f t="shared" si="1"/>
+        <v>etb-aventuras-es,Aventuras Compartidas,ETB,ESPAÑOL,ETB,69990,79990,2,img/etb-aventuras-es.webp,['ETB,'ESPAÑOL'],,</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.35">
@@ -1687,19 +1634,16 @@
         <v>2</v>
       </c>
       <c r="I23" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>img/bin-white-flare-es.webp</v>
       </c>
       <c r="J23" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>['BINDER,'ESPAÑOL']</v>
       </c>
-      <c r="K23" t="s">
-        <v>54</v>
-      </c>
       <c r="O23" s="1" t="str">
-        <f>CONCATENATE(A23,",",B23,",",C23,",",D23,",",E23,",",F23,",",G23,",",H23,",",I23,",",J23,",",K23,",",L23)</f>
-        <v>bin-white-flare-es,Llama Blanca,BINDER,ESPAÑOL,BINDER,34990,34990,2,img/bin-white-flare-es.webp,['BINDER,'ESPAÑOL'],Últimas Unidades,</v>
+        <f t="shared" si="1"/>
+        <v>bin-white-flare-es,Llama Blanca,BINDER,ESPAÑOL,BINDER,34990,34990,2,img/bin-white-flare-es.webp,['BINDER,'ESPAÑOL'],,</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.35">
@@ -1728,19 +1672,16 @@
         <v>2</v>
       </c>
       <c r="I24" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>img/bin-black-bolt-es.webp</v>
       </c>
       <c r="J24" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>['BINDER,'ESPAÑOL']</v>
       </c>
-      <c r="K24" t="s">
-        <v>54</v>
-      </c>
       <c r="O24" s="1" t="str">
-        <f>CONCATENATE(A24,",",B24,",",C24,",",D24,",",E24,",",F24,",",G24,",",H24,",",I24,",",J24,",",K24,",",L24)</f>
-        <v>bin-black-bolt-es,Fulgor Negro,BINDER,ESPAÑOL,BINDER,34990,34990,2,img/bin-black-bolt-es.webp,['BINDER,'ESPAÑOL'],Últimas Unidades,</v>
+        <f t="shared" si="1"/>
+        <v>bin-black-bolt-es,Fulgor Negro,BINDER,ESPAÑOL,BINDER,34990,34990,2,img/bin-black-bolt-es.webp,['BINDER,'ESPAÑOL'],,</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ActualizaciÃ³n completa (2025-09-21 23:11)
</commit_message>
<xml_diff>
--- a/BACKUP/SUPORT IMAGEN.xlsx
+++ b/BACKUP/SUPORT IMAGEN.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jorgg\OneDrive\MasterHIT\BACKUP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04328B6C-63D7-448F-9F44-27BCD2EFACEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70E69675-6AFF-470F-A9F6-EF0D2C28985F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="75">
   <si>
     <t>id,name,set,type,category,price,compareAtPrice,stock,image,tags,source,createdAt</t>
   </si>
@@ -195,70 +195,73 @@
     <t>spc-prismatic-en,Prismatic Evolutions,SPC,INGLÉS,SPC,140000,179990,10,img/spc-prismatic-en.webp,['SPC,'INGLÉS'],Oferta Flash,</t>
   </si>
   <si>
-    <t>special-garchomp-en,Garchomp EX,SPECIAL,ESPAÑOL,SPECIAL,25000,34990,5,img/special-garchomp-en.webp,['SPECIAL,'ESPAÑOL'],Oferta Flash,</t>
-  </si>
-  <si>
     <t>etb-destined-es,Rivales Predestinados,ETB,ESPAÑOL,ETB,40000,54990,10,img/etb-destined-es.webp,['ETB,'ESPAÑOL'],Oferta Flash,</t>
   </si>
   <si>
-    <t>special-charizardex-en,Charizard EX,SPECIAL,ESPAÑOL,SPECIAL,25000,34990,5,img/special-charizardex-en.webp,['SPECIAL,'ESPAÑOL'],Oferta Flash,</t>
-  </si>
-  <si>
-    <t>etb-prismatic-es,Evoluciones Prismáticas,ETB,ESPAÑOL,ETB,55000,69990,2,img/etb-prismatic-es.webp,['ETB,'ESPAÑOL'],Últimas Unidades,</t>
-  </si>
-  <si>
-    <t>special-charizardex-en,Charizard EX,SPECIAL,INGLÉS,SPECIAL,28000,34990,5,img/special-charizardex-en.webp,['SPECIAL,'INGLÉS'],Últimas Unidades,</t>
-  </si>
-  <si>
-    <t>poster-prismatic-en,Prismatic Evolutions,POSTER,ESPAÑOL,POSTER,18000,19990,2,img/poster-prismatic-en.webp,['POSTER,'ESPAÑOL'],Últimas Unidades,</t>
-  </si>
-  <si>
-    <t>special-garchomp-en,Garchomp EX,SPECIAL,INGLÉS,SPECIAL,28000,35990,5,img/special-garchomp-en.webp,['SPECIAL,'INGLÉS'],Últimas Unidades,</t>
-  </si>
-  <si>
-    <t>spc-prismatic-en,Evoluciones Prismáticas,SPC,ESPAÑOL,SPC,120000,179990,2,img/spc-prismatic-en.webp,['SPC,'ESPAÑOL'],Últimas Unidades,</t>
-  </si>
-  <si>
-    <t>surprisebox-en,Prismatic Evolutions,SURPRISE BOX,INGLÉS,SURPRISE BOX,35000,39990,2,img/surprisebox-en.webp,['SURPRISE BOX,'INGLÉS'],Últimas Unidades,</t>
-  </si>
-  <si>
-    <t>surprisebox-en,Prismatic Evolutions,SURPRISE BOX,ESPAÑOL,SURPRISE BOX,30000,34990,2,img/surprisebox-en.webp,['SURPRISE BOX,'ESPAÑOL'],Últimas Unidades,</t>
-  </si>
-  <si>
     <t>etb-megalucario-en,Mega Evolutions,ETB,INGLÉS,ETB,64990,29990,10,img/etb-megalucario-en.webp,['ETB,'INGLÉS'],Preventa 26/09,</t>
   </si>
   <si>
-    <t>etb-megalucario-en,Megaevolución,ETB,ESPAÑOL,ETB,54990,29990,10,img/etb-megalucario-en.webp,['ETB,'ESPAÑOL'],Preventa 26/10,</t>
-  </si>
-  <si>
-    <t>etb-megagardevoir-en,Mega Evolutions,ETB,INGLÉS,ETB,64990,29990,10,img/etb-megagardevoir-en.webp,['ETB,'INGLÉS'],Preventa 26/11,</t>
-  </si>
-  <si>
-    <t>etb-megagardevoir-en,Megaevolución,ETB,ESPAÑOL,ETB,54990,29990,10,img/etb-megagardevoir-en.webp,['ETB,'ESPAÑOL'],Preventa 26/12,</t>
-  </si>
-  <si>
-    <t>etb-white-flare-en,White Flare,ETB,INGLÉS,ETB,74990,79990,2,img/etb-white-flare-en.webp,['ETB,'INGLÉS'],Últimas Unidades,</t>
-  </si>
-  <si>
-    <t>etb-white-flare-en,Llama Blanca,ETB,ESPAÑOL,ETB,69990,79990,2,img/etb-white-flare-en.webp,['ETB,'ESPAÑOL'],Últimas Unidades,</t>
-  </si>
-  <si>
-    <t>etb-black-bolt-en,Black Bolt,ETB,INGLÉS,ETB,74990,79990,2,img/etb-black-bolt-en.webp,['ETB,'INGLÉS'],Últimas Unidades,</t>
-  </si>
-  <si>
-    <t>etb-black-bolt-es,Fulgor Negro,ETB,ESPAÑOL,ETB,69990,79990,2,img/etb-black-bolt-es.webp,['ETB,'ESPAÑOL'],Últimas Unidades,</t>
-  </si>
-  <si>
-    <t>etb-aventuras-es,Journey Together,ETB,INGLÉS,ETB,74990,79990,2,img/etb-aventuras-es.webp,['ETB,'INGLÉS'],Últimas Unidades,</t>
-  </si>
-  <si>
-    <t>etb-aventuras-es,Aventuras Compartidas,ETB,ESPAÑOL,ETB,69990,79990,2,img/etb-aventuras-es.webp,['ETB,'ESPAÑOL'],Últimas Unidades,</t>
-  </si>
-  <si>
-    <t>bin-white-flare-es,Llama Blanca,BINDER,ESPAÑOL,BINDER,34990,34990,2,img/bin-white-flare-es.webp,['BINDER,'ESPAÑOL'],Últimas Unidades,</t>
-  </si>
-  <si>
-    <t>bin-black-bolt-es,Fulgor Negro,BINDER,ESPAÑOL,BINDER,34990,34990,2,img/bin-black-bolt-es.webp,['BINDER,'ESPAÑOL'],Últimas Unidades,</t>
+    <t>etb-megalucario-en,Megaevolución,ETB,ESPAÑOL,ETB,54990,29990,10,img/etb-megalucario-en.webp,['ETB,'ESPAÑOL'],Preventa 26/09,</t>
+  </si>
+  <si>
+    <t>etb-megagardevoir-en,Mega Evolutions,ETB,INGLÉS,ETB,64990,29990,10,img/etb-megagardevoir-en.webp,['ETB,'INGLÉS'],Preventa 26/09,</t>
+  </si>
+  <si>
+    <t>etb-megagardevoir-en,Megaevolución,ETB,ESPAÑOL,ETB,54990,29990,10,img/etb-megagardevoir-en.webp,['ETB,'ESPAÑOL'],Preventa 26/09,</t>
+  </si>
+  <si>
+    <t>special-garchomp-en,Garchomp EX,SPECIAL,ESPAÑOL,SPECIAL,25000,34990,10,img/special-garchomp-en.webp,['SPECIAL,'ESPAÑOL'],Oferta Flash,</t>
+  </si>
+  <si>
+    <t>special-charizardex-en,Charizard EX,SPECIAL,ESPAÑOL,SPECIAL,25000,34990,10,img/special-charizardex-en.webp,['SPECIAL,'ESPAÑOL'],Oferta Flash,</t>
+  </si>
+  <si>
+    <t>etb-prismatic-es,Evoluciones Prismáticas,ETB,ESPAÑOL,ETB,55000,69990,10,img/etb-prismatic-es.webp,['ETB,'ESPAÑOL'],,</t>
+  </si>
+  <si>
+    <t>special-charizardex-en,Charizard EX,SPECIAL,INGLÉS,SPECIAL,28000,34990,10,img/special-charizardex-en.webp,['SPECIAL,'INGLÉS'],,</t>
+  </si>
+  <si>
+    <t>poster-prismatic-en,Prismatic Evolutions,POSTER,ESPAÑOL,POSTER,18000,19990,10,img/poster-prismatic-en.webp,['POSTER,'ESPAÑOL'],,</t>
+  </si>
+  <si>
+    <t>special-garchomp-en,Garchomp EX,SPECIAL,INGLÉS,SPECIAL,28000,35990,10,img/special-garchomp-en.webp,['SPECIAL,'INGLÉS'],,</t>
+  </si>
+  <si>
+    <t>spc-prismatic-en,Evoluciones Prismáticas,SPC,ESPAÑOL,SPC,120000,179990,10,img/spc-prismatic-en.webp,['SPC,'ESPAÑOL'],,</t>
+  </si>
+  <si>
+    <t>surprisebox-en,Prismatic Evolutions,SURPRISE BOX,INGLÉS,SURPRISE BOX,35000,39990,10,img/surprisebox-en.webp,['SURPRISE BOX,'INGLÉS'],,</t>
+  </si>
+  <si>
+    <t>surprisebox-en,Prismatic Evolutions,SURPRISE BOX,ESPAÑOL,SURPRISE BOX,30000,34990,10,img/surprisebox-en.webp,['SURPRISE BOX,'ESPAÑOL'],,</t>
+  </si>
+  <si>
+    <t>etb-white-flare-en,White Flare,ETB,INGLÉS,ETB,74990,79990,10,img/etb-white-flare-en.webp,['ETB,'INGLÉS'],,</t>
+  </si>
+  <si>
+    <t>etb-white-flare-en,Llama Blanca,ETB,ESPAÑOL,ETB,69990,79990,10,img/etb-white-flare-en.webp,['ETB,'ESPAÑOL'],,</t>
+  </si>
+  <si>
+    <t>etb-black-bolt-en,Black Bolt,ETB,INGLÉS,ETB,74990,79990,10,img/etb-black-bolt-en.webp,['ETB,'INGLÉS'],,</t>
+  </si>
+  <si>
+    <t>etb-black-bolt-es,Fulgor Negro,ETB,ESPAÑOL,ETB,69990,79990,10,img/etb-black-bolt-es.webp,['ETB,'ESPAÑOL'],,</t>
+  </si>
+  <si>
+    <t>etb-aventuras-es,Journey Together,ETB,INGLÉS,ETB,74990,79990,10,img/etb-aventuras-es.webp,['ETB,'INGLÉS'],,</t>
+  </si>
+  <si>
+    <t>etb-aventuras-es,Aventuras Compartidas,ETB,ESPAÑOL,ETB,69990,79990,10,img/etb-aventuras-es.webp,['ETB,'ESPAÑOL'],,</t>
+  </si>
+  <si>
+    <t>bin-white-flare-es,Llama Blanca,BINDER,ESPAÑOL,BINDER,34990,34990,10,img/bin-white-flare-es.webp,['BINDER,'ESPAÑOL'],,</t>
+  </si>
+  <si>
+    <t>bin-black-bolt-es,Fulgor Negro,BINDER,ESPAÑOL,BINDER,34990,34990,10,img/bin-black-bolt-es.webp,['BINDER,'ESPAÑOL'],,</t>
+  </si>
+  <si>
+    <t>poster-prismatic-en,Prismatic Evolutions,POSTER,INGLÉS,POSTER,29990,34990,10,img/poster-prismatic-en.webp,['POSTER,'INGLÉS'],,</t>
   </si>
 </sst>
 </file>
@@ -589,13 +592,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A24"/>
+  <dimension ref="A1:A25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A24"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="124.453125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
@@ -609,112 +613,117 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>73</v>
+        <v>74</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -724,9 +733,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3CA635C-1DF7-4EEC-B0B8-3FA5C80D03DF}">
-  <dimension ref="A1:O24"/>
+  <dimension ref="A1:O25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O2" sqref="O2:O25"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -823,7 +834,7 @@
         <v>49</v>
       </c>
       <c r="O2" s="1" t="str">
-        <f t="shared" ref="O2:O24" si="1">CONCATENATE(A2,",",B2,",",C2,",",D2,",",E2,",",F2,",",G2,",",H2,",",I2,",",J2,",",K2,",",L2)</f>
+        <f t="shared" ref="O2:O25" si="1">CONCATENATE(A2,",",B2,",",C2,",",D2,",",E2,",",F2,",",G2,",",H2,",",I2,",",J2,",",K2,",",L2)</f>
         <v>spc-prismatic-en,Prismatic Evolutions,SPC,INGLÉS,SPC,140000,179990,10,img/spc-prismatic-en.webp,['SPC,'INGLÉS'],Oferta Flash,</v>
       </c>
     </row>
@@ -850,7 +861,7 @@
         <v>34990</v>
       </c>
       <c r="H3">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I3" t="str">
         <f>CONCATENATE("img/",A3,".webp")</f>
@@ -865,7 +876,7 @@
       </c>
       <c r="O3" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>special-garchomp-en,Garchomp EX,SPECIAL,ESPAÑOL,SPECIAL,25000,34990,5,img/special-garchomp-en.webp,['SPECIAL,'ESPAÑOL'],Oferta Flash,</v>
+        <v>special-garchomp-en,Garchomp EX,SPECIAL,ESPAÑOL,SPECIAL,25000,34990,10,img/special-garchomp-en.webp,['SPECIAL,'ESPAÑOL'],Oferta Flash,</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.35">
@@ -894,7 +905,7 @@
         <v>10</v>
       </c>
       <c r="I4" t="str">
-        <f t="shared" ref="I4:I8" si="2">CONCATENATE("img/",A4,".webp")</f>
+        <f t="shared" ref="I4:I7" si="2">CONCATENATE("img/",A4,".webp")</f>
         <v>img/etb-destined-es.webp</v>
       </c>
       <c r="J4" t="str">
@@ -932,7 +943,7 @@
         <v>34990</v>
       </c>
       <c r="H5">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I5" t="str">
         <f>CONCATENATE("img/",A5,".webp")</f>
@@ -947,7 +958,7 @@
       </c>
       <c r="O5" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>special-charizardex-en,Charizard EX,SPECIAL,ESPAÑOL,SPECIAL,25000,34990,5,img/special-charizardex-en.webp,['SPECIAL,'ESPAÑOL'],Oferta Flash,</v>
+        <v>special-charizardex-en,Charizard EX,SPECIAL,ESPAÑOL,SPECIAL,25000,34990,10,img/special-charizardex-en.webp,['SPECIAL,'ESPAÑOL'],Oferta Flash,</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.35">
@@ -973,7 +984,7 @@
         <v>69990</v>
       </c>
       <c r="H6">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="I6" t="str">
         <f t="shared" ref="I6" si="3">CONCATENATE("img/",A6,".webp")</f>
@@ -985,7 +996,7 @@
       </c>
       <c r="O6" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>etb-prismatic-es,Evoluciones Prismáticas,ETB,ESPAÑOL,ETB,55000,69990,2,img/etb-prismatic-es.webp,['ETB,'ESPAÑOL'],,</v>
+        <v>etb-prismatic-es,Evoluciones Prismáticas,ETB,ESPAÑOL,ETB,55000,69990,10,img/etb-prismatic-es.webp,['ETB,'ESPAÑOL'],,</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.35">
@@ -1011,133 +1022,133 @@
         <v>34990</v>
       </c>
       <c r="H7">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I7" t="str">
         <f t="shared" si="2"/>
         <v>img/special-charizardex-en.webp</v>
       </c>
       <c r="J7" t="str">
-        <f t="shared" ref="J7:J8" si="4">CONCATENATE("['",C7,",'",D7,"']")</f>
+        <f t="shared" ref="J7" si="4">CONCATENATE("['",C7,",'",D7,"']")</f>
         <v>['SPECIAL,'INGLÉS']</v>
       </c>
       <c r="O7" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>special-charizardex-en,Charizard EX,SPECIAL,INGLÉS,SPECIAL,28000,34990,5,img/special-charizardex-en.webp,['SPECIAL,'INGLÉS'],,</v>
+        <v>special-charizardex-en,Charizard EX,SPECIAL,INGLÉS,SPECIAL,28000,34990,10,img/special-charizardex-en.webp,['SPECIAL,'INGLÉS'],,</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="C8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D8" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F8">
-        <v>18000</v>
+        <v>28000</v>
       </c>
       <c r="G8">
-        <v>19990</v>
+        <v>35990</v>
       </c>
       <c r="H8">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="I8" t="str">
-        <f t="shared" si="2"/>
-        <v>img/poster-prismatic-en.webp</v>
+        <f t="shared" ref="I8" si="5">CONCATENATE("img/",A8,".webp")</f>
+        <v>img/special-garchomp-en.webp</v>
       </c>
       <c r="J8" t="str">
-        <f t="shared" si="4"/>
-        <v>['POSTER,'ESPAÑOL']</v>
+        <f t="shared" ref="J8:J9" si="6">CONCATENATE("['",C8,",'",D8,"']")</f>
+        <v>['SPECIAL,'INGLÉS']</v>
       </c>
       <c r="O8" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>poster-prismatic-en,Prismatic Evolutions,POSTER,ESPAÑOL,POSTER,18000,19990,2,img/poster-prismatic-en.webp,['POSTER,'ESPAÑOL'],,</v>
+        <v>special-garchomp-en,Garchomp EX,SPECIAL,INGLÉS,SPECIAL,28000,35990,10,img/special-garchomp-en.webp,['SPECIAL,'INGLÉS'],,</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="B9" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="C9" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="D9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E9" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="F9">
-        <v>28000</v>
+        <v>120000</v>
       </c>
       <c r="G9">
-        <v>35990</v>
+        <v>179990</v>
       </c>
       <c r="H9">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I9" t="str">
-        <f t="shared" ref="I9" si="5">CONCATENATE("img/",A9,".webp")</f>
-        <v>img/special-garchomp-en.webp</v>
+        <f>CONCATENATE("img/",A9,".webp")</f>
+        <v>img/spc-prismatic-en.webp</v>
       </c>
       <c r="J9" t="str">
-        <f t="shared" ref="J9:J10" si="6">CONCATENATE("['",C9,",'",D9,"']")</f>
-        <v>['SPECIAL,'INGLÉS']</v>
+        <f t="shared" si="6"/>
+        <v>['SPC,'ESPAÑOL']</v>
       </c>
       <c r="O9" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>special-garchomp-en,Garchomp EX,SPECIAL,INGLÉS,SPECIAL,28000,35990,5,img/special-garchomp-en.webp,['SPECIAL,'INGLÉS'],,</v>
+        <v>spc-prismatic-en,Evoluciones Prismáticas,SPC,ESPAÑOL,SPC,120000,179990,10,img/spc-prismatic-en.webp,['SPC,'ESPAÑOL'],,</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="B10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C10" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E10" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="F10">
-        <v>120000</v>
+        <v>35000</v>
       </c>
       <c r="G10">
-        <v>179990</v>
+        <v>39990</v>
       </c>
       <c r="H10">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="I10" t="str">
-        <f>CONCATENATE("img/",A10,".webp")</f>
-        <v>img/spc-prismatic-en.webp</v>
+        <f t="shared" ref="I10:I11" si="7">CONCATENATE("img/",A10,".webp")</f>
+        <v>img/surprisebox-en.webp</v>
       </c>
       <c r="J10" t="str">
-        <f t="shared" si="6"/>
-        <v>['SPC,'ESPAÑOL']</v>
+        <f t="shared" ref="J10:J11" si="8">CONCATENATE("['",C10,",'",D10,"']")</f>
+        <v>['SURPRISE BOX,'INGLÉS']</v>
       </c>
       <c r="O10" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>spc-prismatic-en,Evoluciones Prismáticas,SPC,ESPAÑOL,SPC,120000,179990,2,img/spc-prismatic-en.webp,['SPC,'ESPAÑOL'],,</v>
+        <v>surprisebox-en,Prismatic Evolutions,SURPRISE BOX,INGLÉS,SURPRISE BOX,35000,39990,10,img/surprisebox-en.webp,['SURPRISE BOX,'INGLÉS'],,</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.35">
@@ -1151,69 +1162,72 @@
         <v>42</v>
       </c>
       <c r="D11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E11" t="s">
         <v>42</v>
       </c>
       <c r="F11">
-        <v>35000</v>
+        <v>30000</v>
       </c>
       <c r="G11">
-        <v>39990</v>
+        <v>34990</v>
       </c>
       <c r="H11">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="I11" t="str">
-        <f t="shared" ref="I11:I12" si="7">CONCATENATE("img/",A11,".webp")</f>
+        <f t="shared" si="7"/>
         <v>img/surprisebox-en.webp</v>
       </c>
       <c r="J11" t="str">
-        <f t="shared" ref="J11:J12" si="8">CONCATENATE("['",C11,",'",D11,"']")</f>
-        <v>['SURPRISE BOX,'INGLÉS']</v>
+        <f t="shared" si="8"/>
+        <v>['SURPRISE BOX,'ESPAÑOL']</v>
       </c>
       <c r="O11" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>surprisebox-en,Prismatic Evolutions,SURPRISE BOX,INGLÉS,SURPRISE BOX,35000,39990,2,img/surprisebox-en.webp,['SURPRISE BOX,'INGLÉS'],,</v>
+        <v>surprisebox-en,Prismatic Evolutions,SURPRISE BOX,ESPAÑOL,SURPRISE BOX,30000,34990,10,img/surprisebox-en.webp,['SURPRISE BOX,'ESPAÑOL'],,</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B12" t="s">
-        <v>21</v>
+        <v>45</v>
       </c>
       <c r="C12" t="s">
-        <v>42</v>
+        <v>20</v>
       </c>
       <c r="D12" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E12" t="s">
-        <v>42</v>
+        <v>20</v>
       </c>
       <c r="F12">
-        <v>30000</v>
+        <v>64990</v>
       </c>
       <c r="G12">
-        <v>34990</v>
+        <v>29990</v>
       </c>
       <c r="H12">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="I12" t="str">
-        <f t="shared" si="7"/>
-        <v>img/surprisebox-en.webp</v>
+        <f t="shared" ref="I12:I15" si="9">CONCATENATE("img/",A12,".webp")</f>
+        <v>img/etb-megalucario-en.webp</v>
       </c>
       <c r="J12" t="str">
-        <f t="shared" si="8"/>
-        <v>['SURPRISE BOX,'ESPAÑOL']</v>
+        <f t="shared" ref="J12:J15" si="10">CONCATENATE("['",C12,",'",D12,"']")</f>
+        <v>['ETB,'INGLÉS']</v>
+      </c>
+      <c r="K12" t="s">
+        <v>50</v>
       </c>
       <c r="O12" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>surprisebox-en,Prismatic Evolutions,SURPRISE BOX,ESPAÑOL,SURPRISE BOX,30000,34990,2,img/surprisebox-en.webp,['SURPRISE BOX,'ESPAÑOL'],,</v>
+        <v>etb-megalucario-en,Mega Evolutions,ETB,INGLÉS,ETB,64990,29990,10,img/etb-megalucario-en.webp,['ETB,'INGLÉS'],Preventa 26/09,</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.35">
@@ -1221,19 +1235,19 @@
         <v>44</v>
       </c>
       <c r="B13" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C13" t="s">
         <v>20</v>
       </c>
       <c r="D13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E13" t="s">
         <v>20</v>
       </c>
       <c r="F13">
-        <v>64990</v>
+        <v>54990</v>
       </c>
       <c r="G13">
         <v>29990</v>
@@ -1242,39 +1256,39 @@
         <v>10</v>
       </c>
       <c r="I13" t="str">
-        <f t="shared" ref="I13:I16" si="9">CONCATENATE("img/",A13,".webp")</f>
+        <f t="shared" si="9"/>
         <v>img/etb-megalucario-en.webp</v>
       </c>
       <c r="J13" t="str">
-        <f t="shared" ref="J13:J16" si="10">CONCATENATE("['",C13,",'",D13,"']")</f>
-        <v>['ETB,'INGLÉS']</v>
+        <f t="shared" si="10"/>
+        <v>['ETB,'ESPAÑOL']</v>
       </c>
       <c r="K13" t="s">
         <v>50</v>
       </c>
       <c r="O13" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>etb-megalucario-en,Mega Evolutions,ETB,INGLÉS,ETB,64990,29990,10,img/etb-megalucario-en.webp,['ETB,'INGLÉS'],Preventa 26/09,</v>
+        <v>etb-megalucario-en,Megaevolución,ETB,ESPAÑOL,ETB,54990,29990,10,img/etb-megalucario-en.webp,['ETB,'ESPAÑOL'],Preventa 26/09,</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C14" t="s">
         <v>20</v>
       </c>
       <c r="D14" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E14" t="s">
         <v>20</v>
       </c>
       <c r="F14">
-        <v>54990</v>
+        <v>64990</v>
       </c>
       <c r="G14">
         <v>29990</v>
@@ -1284,18 +1298,18 @@
       </c>
       <c r="I14" t="str">
         <f t="shared" si="9"/>
-        <v>img/etb-megalucario-en.webp</v>
+        <v>img/etb-megagardevoir-en.webp</v>
       </c>
       <c r="J14" t="str">
         <f t="shared" si="10"/>
-        <v>['ETB,'ESPAÑOL']</v>
+        <v>['ETB,'INGLÉS']</v>
       </c>
       <c r="K14" t="s">
         <v>50</v>
       </c>
       <c r="O14" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>etb-megalucario-en,Megaevolución,ETB,ESPAÑOL,ETB,54990,29990,10,img/etb-megalucario-en.webp,['ETB,'ESPAÑOL'],Preventa 26/09,</v>
+        <v>etb-megagardevoir-en,Mega Evolutions,ETB,INGLÉS,ETB,64990,29990,10,img/etb-megagardevoir-en.webp,['ETB,'INGLÉS'],Preventa 26/09,</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.35">
@@ -1303,19 +1317,19 @@
         <v>43</v>
       </c>
       <c r="B15" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C15" t="s">
         <v>20</v>
       </c>
       <c r="D15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E15" t="s">
         <v>20</v>
       </c>
       <c r="F15">
-        <v>64990</v>
+        <v>54990</v>
       </c>
       <c r="G15">
         <v>29990</v>
@@ -1329,55 +1343,52 @@
       </c>
       <c r="J15" t="str">
         <f t="shared" si="10"/>
-        <v>['ETB,'INGLÉS']</v>
+        <v>['ETB,'ESPAÑOL']</v>
       </c>
       <c r="K15" t="s">
         <v>50</v>
       </c>
       <c r="O15" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>etb-megagardevoir-en,Mega Evolutions,ETB,INGLÉS,ETB,64990,29990,10,img/etb-megagardevoir-en.webp,['ETB,'INGLÉS'],Preventa 26/09,</v>
+        <v>etb-megagardevoir-en,Megaevolución,ETB,ESPAÑOL,ETB,54990,29990,10,img/etb-megagardevoir-en.webp,['ETB,'ESPAÑOL'],Preventa 26/09,</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>46</v>
+        <v>23</v>
       </c>
       <c r="C16" t="s">
         <v>20</v>
       </c>
       <c r="D16" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E16" t="s">
         <v>20</v>
       </c>
       <c r="F16">
-        <v>54990</v>
+        <v>74990</v>
       </c>
       <c r="G16">
-        <v>29990</v>
+        <v>79990</v>
       </c>
       <c r="H16">
         <v>10</v>
       </c>
       <c r="I16" t="str">
-        <f t="shared" si="9"/>
-        <v>img/etb-megagardevoir-en.webp</v>
+        <f t="shared" ref="I16:I23" si="11">CONCATENATE("img/",A16,".webp")</f>
+        <v>img/etb-white-flare-en.webp</v>
       </c>
       <c r="J16" t="str">
-        <f t="shared" si="10"/>
-        <v>['ETB,'ESPAÑOL']</v>
-      </c>
-      <c r="K16" t="s">
-        <v>50</v>
+        <f t="shared" ref="J16:J23" si="12">CONCATENATE("['",C16,",'",D16,"']")</f>
+        <v>['ETB,'INGLÉS']</v>
       </c>
       <c r="O16" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>etb-megagardevoir-en,Megaevolución,ETB,ESPAÑOL,ETB,54990,29990,10,img/etb-megagardevoir-en.webp,['ETB,'ESPAÑOL'],Preventa 26/09,</v>
+        <v>etb-white-flare-en,White Flare,ETB,INGLÉS,ETB,74990,79990,10,img/etb-white-flare-en.webp,['ETB,'INGLÉS'],,</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.35">
@@ -1385,151 +1396,151 @@
         <v>14</v>
       </c>
       <c r="B17" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C17" t="s">
         <v>20</v>
       </c>
       <c r="D17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E17" t="s">
         <v>20</v>
       </c>
       <c r="F17">
-        <v>74990</v>
+        <v>69990</v>
       </c>
       <c r="G17">
         <v>79990</v>
       </c>
       <c r="H17">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="I17" t="str">
-        <f t="shared" ref="I17:I24" si="11">CONCATENATE("img/",A17,".webp")</f>
+        <f t="shared" si="11"/>
         <v>img/etb-white-flare-en.webp</v>
       </c>
       <c r="J17" t="str">
-        <f t="shared" ref="J17:J24" si="12">CONCATENATE("['",C17,",'",D17,"']")</f>
-        <v>['ETB,'INGLÉS']</v>
+        <f t="shared" si="12"/>
+        <v>['ETB,'ESPAÑOL']</v>
       </c>
       <c r="O17" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>etb-white-flare-en,White Flare,ETB,INGLÉS,ETB,74990,79990,2,img/etb-white-flare-en.webp,['ETB,'INGLÉS'],,</v>
+        <v>etb-white-flare-en,Llama Blanca,ETB,ESPAÑOL,ETB,69990,79990,10,img/etb-white-flare-en.webp,['ETB,'ESPAÑOL'],,</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B18" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C18" t="s">
         <v>20</v>
       </c>
       <c r="D18" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E18" t="s">
         <v>20</v>
       </c>
       <c r="F18">
-        <v>69990</v>
+        <v>74990</v>
       </c>
       <c r="G18">
         <v>79990</v>
       </c>
       <c r="H18">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="I18" t="str">
         <f t="shared" si="11"/>
-        <v>img/etb-white-flare-en.webp</v>
+        <v>img/etb-black-bolt-en.webp</v>
       </c>
       <c r="J18" t="str">
         <f t="shared" si="12"/>
-        <v>['ETB,'ESPAÑOL']</v>
+        <v>['ETB,'INGLÉS']</v>
       </c>
       <c r="O18" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>etb-white-flare-en,Llama Blanca,ETB,ESPAÑOL,ETB,69990,79990,2,img/etb-white-flare-en.webp,['ETB,'ESPAÑOL'],,</v>
+        <v>etb-black-bolt-en,Black Bolt,ETB,INGLÉS,ETB,74990,79990,10,img/etb-black-bolt-en.webp,['ETB,'INGLÉS'],,</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B19" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="C19" t="s">
         <v>20</v>
       </c>
       <c r="D19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E19" t="s">
         <v>20</v>
       </c>
       <c r="F19">
-        <v>74990</v>
+        <v>69990</v>
       </c>
       <c r="G19">
         <v>79990</v>
       </c>
       <c r="H19">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="I19" t="str">
         <f t="shared" si="11"/>
-        <v>img/etb-black-bolt-en.webp</v>
+        <v>img/etb-black-bolt-es.webp</v>
       </c>
       <c r="J19" t="str">
         <f t="shared" si="12"/>
-        <v>['ETB,'INGLÉS']</v>
+        <v>['ETB,'ESPAÑOL']</v>
       </c>
       <c r="O19" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>etb-black-bolt-en,Black Bolt,ETB,INGLÉS,ETB,74990,79990,2,img/etb-black-bolt-en.webp,['ETB,'INGLÉS'],,</v>
+        <v>etb-black-bolt-es,Fulgor Negro,ETB,ESPAÑOL,ETB,69990,79990,10,img/etb-black-bolt-es.webp,['ETB,'ESPAÑOL'],,</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C20" t="s">
         <v>20</v>
       </c>
       <c r="D20" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E20" t="s">
         <v>20</v>
       </c>
       <c r="F20">
-        <v>69990</v>
+        <v>74990</v>
       </c>
       <c r="G20">
         <v>79990</v>
       </c>
       <c r="H20">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="I20" t="str">
         <f t="shared" si="11"/>
-        <v>img/etb-black-bolt-es.webp</v>
+        <v>img/etb-aventuras-es.webp</v>
       </c>
       <c r="J20" t="str">
         <f t="shared" si="12"/>
-        <v>['ETB,'ESPAÑOL']</v>
+        <v>['ETB,'INGLÉS']</v>
       </c>
       <c r="O20" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>etb-black-bolt-es,Fulgor Negro,ETB,ESPAÑOL,ETB,69990,79990,2,img/etb-black-bolt-es.webp,['ETB,'ESPAÑOL'],,</v>
+        <v>etb-aventuras-es,Journey Together,ETB,INGLÉS,ETB,74990,79990,10,img/etb-aventuras-es.webp,['ETB,'INGLÉS'],,</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.35">
@@ -1537,25 +1548,25 @@
         <v>17</v>
       </c>
       <c r="B21" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C21" t="s">
         <v>20</v>
       </c>
       <c r="D21" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E21" t="s">
         <v>20</v>
       </c>
       <c r="F21">
-        <v>74990</v>
+        <v>69990</v>
       </c>
       <c r="G21">
         <v>79990</v>
       </c>
       <c r="H21">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="I21" t="str">
         <f t="shared" si="11"/>
@@ -1563,57 +1574,57 @@
       </c>
       <c r="J21" t="str">
         <f t="shared" si="12"/>
-        <v>['ETB,'INGLÉS']</v>
+        <v>['ETB,'ESPAÑOL']</v>
       </c>
       <c r="O21" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>etb-aventuras-es,Journey Together,ETB,INGLÉS,ETB,74990,79990,2,img/etb-aventuras-es.webp,['ETB,'INGLÉS'],,</v>
+        <v>etb-aventuras-es,Aventuras Compartidas,ETB,ESPAÑOL,ETB,69990,79990,10,img/etb-aventuras-es.webp,['ETB,'ESPAÑOL'],,</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="B22" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C22" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="D22" t="s">
         <v>18</v>
       </c>
       <c r="E22" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="F22">
-        <v>69990</v>
+        <v>34990</v>
       </c>
       <c r="G22">
-        <v>79990</v>
+        <v>34990</v>
       </c>
       <c r="H22">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="I22" t="str">
         <f t="shared" si="11"/>
-        <v>img/etb-aventuras-es.webp</v>
+        <v>img/bin-white-flare-es.webp</v>
       </c>
       <c r="J22" t="str">
         <f t="shared" si="12"/>
-        <v>['ETB,'ESPAÑOL']</v>
+        <v>['BINDER,'ESPAÑOL']</v>
       </c>
       <c r="O22" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>etb-aventuras-es,Aventuras Compartidas,ETB,ESPAÑOL,ETB,69990,79990,2,img/etb-aventuras-es.webp,['ETB,'ESPAÑOL'],,</v>
+        <v>bin-white-flare-es,Llama Blanca,BINDER,ESPAÑOL,BINDER,34990,34990,10,img/bin-white-flare-es.webp,['BINDER,'ESPAÑOL'],,</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B23" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C23" t="s">
         <v>33</v>
@@ -1631,11 +1642,11 @@
         <v>34990</v>
       </c>
       <c r="H23">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="I23" t="str">
         <f t="shared" si="11"/>
-        <v>img/bin-white-flare-es.webp</v>
+        <v>img/bin-black-bolt-es.webp</v>
       </c>
       <c r="J23" t="str">
         <f t="shared" si="12"/>
@@ -1643,45 +1654,83 @@
       </c>
       <c r="O23" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>bin-white-flare-es,Llama Blanca,BINDER,ESPAÑOL,BINDER,34990,34990,2,img/bin-white-flare-es.webp,['BINDER,'ESPAÑOL'],,</v>
+        <v>bin-black-bolt-es,Fulgor Negro,BINDER,ESPAÑOL,BINDER,34990,34990,10,img/bin-black-bolt-es.webp,['BINDER,'ESPAÑOL'],,</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="B24" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="C24" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="D24" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E24" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="F24">
-        <v>34990</v>
+        <v>29990</v>
       </c>
       <c r="G24">
         <v>34990</v>
       </c>
       <c r="H24">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="I24" t="str">
-        <f t="shared" si="11"/>
-        <v>img/bin-black-bolt-es.webp</v>
+        <f t="shared" ref="I24" si="13">CONCATENATE("img/",A24,".webp")</f>
+        <v>img/poster-prismatic-en.webp</v>
       </c>
       <c r="J24" t="str">
-        <f t="shared" si="12"/>
-        <v>['BINDER,'ESPAÑOL']</v>
+        <f t="shared" ref="J24" si="14">CONCATENATE("['",C24,",'",D24,"']")</f>
+        <v>['POSTER,'INGLÉS']</v>
       </c>
       <c r="O24" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>bin-black-bolt-es,Fulgor Negro,BINDER,ESPAÑOL,BINDER,34990,34990,2,img/bin-black-bolt-es.webp,['BINDER,'ESPAÑOL'],,</v>
+        <v>poster-prismatic-en,Prismatic Evolutions,POSTER,INGLÉS,POSTER,29990,34990,10,img/poster-prismatic-en.webp,['POSTER,'INGLÉS'],,</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>37</v>
+      </c>
+      <c r="B25" t="s">
+        <v>21</v>
+      </c>
+      <c r="C25" t="s">
+        <v>38</v>
+      </c>
+      <c r="D25" t="s">
+        <v>18</v>
+      </c>
+      <c r="E25" t="s">
+        <v>38</v>
+      </c>
+      <c r="F25">
+        <v>18000</v>
+      </c>
+      <c r="G25">
+        <v>19990</v>
+      </c>
+      <c r="H25">
+        <v>10</v>
+      </c>
+      <c r="I25" t="str">
+        <f>CONCATENATE("img/",A25,".webp")</f>
+        <v>img/poster-prismatic-en.webp</v>
+      </c>
+      <c r="J25" t="str">
+        <f>CONCATENATE("['",C25,",'",D25,"']")</f>
+        <v>['POSTER,'ESPAÑOL']</v>
+      </c>
+      <c r="O25" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>poster-prismatic-en,Prismatic Evolutions,POSTER,ESPAÑOL,POSTER,18000,19990,10,img/poster-prismatic-en.webp,['POSTER,'ESPAÑOL'],,</v>
       </c>
     </row>
   </sheetData>

</xml_diff>